<commit_message>
Update risk history and reports with new data for January 2026
- Added multiple entries for January 22, 2026, with updated scores, SPY, VIX, and VIX structure in risk_history.json.
- Introduced drift history for January 22, 2026, detailing total drift and category contributions.
- Updated risk_report_20260120.txt with revised portfolio allocations and drift percentages.
- Created new risk_report_20260122.txt with comprehensive portfolio allocation, drift analysis, and risk trend data.
- Adjusted key signals and tier scores in the risk reports to reflect the latest data.
</commit_message>
<xml_diff>
--- a/projects/fetch-ibkr-positions-dashboard.xlsx
+++ b/projects/fetch-ibkr-positions-dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hongkiatkoh/Desktop/timeless-workspace/timeless-workspace/projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2033401-5918-4943-AAB7-547F3EEC4A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0221FD-8467-1948-BF8C-8B1A2E94D03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="1460" windowWidth="39920" windowHeight="25120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5820" yWindow="1940" windowWidth="32100" windowHeight="25120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -1496,10 +1496,10 @@
                   <c:v>249394.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29927.31</c:v>
+                  <c:v>24939.425000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19951.540000000005</c:v>
+                  <c:v>24939.425000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>29927.309999999998</c:v>
@@ -1634,25 +1634,25 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>426308.66674999997</c:v>
+                  <c:v>425631.65714999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>121926.18</c:v>
+                  <c:v>121670.56</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>144514</c:v>
+                  <c:v>139180</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42550.624000000033</c:v>
+                  <c:v>34190.832800000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2250</c:v>
+                  <c:v>4540</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25782.959580000002</c:v>
+                  <c:v>26101.25532</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>242000</c:v>
+                  <c:v>249197.82785991702</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2480,7 +2480,7 @@
             <v>Long</v>
           </cell>
           <cell r="U2">
-            <v>4562.625</v>
+            <v>4551.7582000000002</v>
           </cell>
         </row>
         <row r="3">
@@ -2494,7 +2494,7 @@
             <v>Long</v>
           </cell>
           <cell r="U3">
-            <v>7381.7655000000004</v>
+            <v>7345.166400000001</v>
           </cell>
         </row>
         <row r="4">
@@ -2508,7 +2508,7 @@
             <v>Long</v>
           </cell>
           <cell r="U4">
-            <v>19088.543249999999</v>
+            <v>19083.758849999998</v>
           </cell>
         </row>
         <row r="5">
@@ -2522,7 +2522,7 @@
             <v>Long</v>
           </cell>
           <cell r="U5">
-            <v>21485.799650000001</v>
+            <v>21751.0461</v>
           </cell>
         </row>
         <row r="6">
@@ -2536,7 +2536,7 @@
             <v>Long</v>
           </cell>
           <cell r="U6">
-            <v>23912</v>
+            <v>23100</v>
           </cell>
         </row>
         <row r="7">
@@ -2550,7 +2550,7 @@
             <v>Long</v>
           </cell>
           <cell r="U7">
-            <v>1326</v>
+            <v>1242</v>
           </cell>
         </row>
         <row r="8">
@@ -2564,7 +2564,7 @@
             <v>Long</v>
           </cell>
           <cell r="U8">
-            <v>2719.5</v>
+            <v>2834.5</v>
           </cell>
         </row>
         <row r="9">
@@ -2592,7 +2592,7 @@
             <v>Long</v>
           </cell>
           <cell r="U10">
-            <v>14440</v>
+            <v>14474</v>
           </cell>
         </row>
         <row r="11">
@@ -2606,7 +2606,7 @@
             <v>Long</v>
           </cell>
           <cell r="U11">
-            <v>10976</v>
+            <v>10788</v>
           </cell>
         </row>
         <row r="12">
@@ -2620,7 +2620,7 @@
             <v>Long</v>
           </cell>
           <cell r="U12">
-            <v>33000</v>
+            <v>32200</v>
           </cell>
         </row>
         <row r="13">
@@ -2634,7 +2634,7 @@
             <v>Long</v>
           </cell>
           <cell r="U13">
-            <v>2190</v>
+            <v>2255</v>
           </cell>
         </row>
         <row r="14">
@@ -2648,7 +2648,7 @@
             <v>Long</v>
           </cell>
           <cell r="U14">
-            <v>9267.5</v>
+            <v>9335</v>
           </cell>
         </row>
         <row r="15">
@@ -2662,7 +2662,7 @@
             <v>Long</v>
           </cell>
           <cell r="U15">
-            <v>9986.59</v>
+            <v>9947.2800000000007</v>
           </cell>
         </row>
         <row r="16">
@@ -2676,7 +2676,7 @@
             <v>Long</v>
           </cell>
           <cell r="U16">
-            <v>1697.5</v>
+            <v>1682.5</v>
           </cell>
         </row>
         <row r="17">
@@ -2690,7 +2690,7 @@
             <v>Long</v>
           </cell>
           <cell r="U17">
-            <v>9939</v>
+            <v>9975.5</v>
           </cell>
         </row>
         <row r="18">
@@ -2698,13 +2698,13 @@
             <v>STK</v>
           </cell>
           <cell r="F18" t="str">
-            <v>LULU</v>
+            <v>MELI</v>
           </cell>
           <cell r="T18" t="str">
             <v>Long</v>
           </cell>
           <cell r="U18">
-            <v>8074.8</v>
+            <v>2034.82</v>
           </cell>
         </row>
         <row r="19">
@@ -2712,13 +2712,13 @@
             <v>STK</v>
           </cell>
           <cell r="F19" t="str">
-            <v>MELI</v>
+            <v>NVDA</v>
           </cell>
           <cell r="T19" t="str">
             <v>Long</v>
           </cell>
           <cell r="U19">
-            <v>2075.0100000000002</v>
+            <v>35614</v>
           </cell>
         </row>
         <row r="20">
@@ -2726,13 +2726,13 @@
             <v>STK</v>
           </cell>
           <cell r="F20" t="str">
-            <v>NVDA</v>
+            <v>ORCL</v>
           </cell>
           <cell r="T20" t="str">
             <v>Long</v>
           </cell>
           <cell r="U20">
-            <v>37246</v>
+            <v>17992</v>
           </cell>
         </row>
         <row r="21">
@@ -2740,13 +2740,13 @@
             <v>STK</v>
           </cell>
           <cell r="F21" t="str">
-            <v>ORCL</v>
+            <v>SE</v>
           </cell>
           <cell r="T21" t="str">
             <v>Long</v>
           </cell>
           <cell r="U21">
-            <v>19109</v>
+            <v>1212.2</v>
           </cell>
         </row>
         <row r="22">
@@ -2754,27 +2754,27 @@
             <v>STK</v>
           </cell>
           <cell r="F22" t="str">
-            <v>SE</v>
+            <v>VWRA</v>
           </cell>
           <cell r="T22" t="str">
             <v>Long</v>
           </cell>
           <cell r="U22">
-            <v>1214.2</v>
+            <v>103248</v>
           </cell>
         </row>
         <row r="23">
           <cell r="D23" t="str">
-            <v>STK</v>
+            <v>FOP</v>
           </cell>
           <cell r="F23" t="str">
-            <v>VWRA</v>
+            <v>EW2G6 P6525</v>
           </cell>
           <cell r="T23" t="str">
             <v>Long</v>
           </cell>
           <cell r="U23">
-            <v>103476</v>
+            <v>4450</v>
           </cell>
         </row>
         <row r="24">
@@ -2782,27 +2782,27 @@
             <v>FOP</v>
           </cell>
           <cell r="F24" t="str">
-            <v>EW2G6 P6525</v>
+            <v>EW2G6 C7300</v>
           </cell>
           <cell r="T24" t="str">
             <v>Long</v>
           </cell>
           <cell r="U24">
-            <v>1900</v>
+            <v>90</v>
           </cell>
         </row>
         <row r="25">
           <cell r="D25" t="str">
-            <v>FOP</v>
+            <v>OPT</v>
           </cell>
           <cell r="F25" t="str">
-            <v>EW2G6 C7300</v>
+            <v>AMZN  260220P00215000</v>
           </cell>
           <cell r="T25" t="str">
-            <v>Long</v>
+            <v>Short</v>
           </cell>
           <cell r="U25">
-            <v>350</v>
+            <v>-482.5</v>
           </cell>
         </row>
         <row r="26">
@@ -2810,13 +2810,13 @@
             <v>OPT</v>
           </cell>
           <cell r="F26" t="str">
-            <v>AAPL  260130P00250000</v>
+            <v>AMZN  260227C00255000</v>
           </cell>
           <cell r="T26" t="str">
             <v>Short</v>
           </cell>
           <cell r="U26">
-            <v>-355</v>
+            <v>-352.5</v>
           </cell>
         </row>
         <row r="27">
@@ -2824,13 +2824,13 @@
             <v>OPT</v>
           </cell>
           <cell r="F27" t="str">
-            <v>AMZN  260220P00215000</v>
+            <v>GOOGL 260227P00310000</v>
           </cell>
           <cell r="T27" t="str">
             <v>Short</v>
           </cell>
           <cell r="U27">
-            <v>-271.5</v>
+            <v>-958.76</v>
           </cell>
         </row>
         <row r="28">
@@ -2838,13 +2838,13 @@
             <v>OPT</v>
           </cell>
           <cell r="F28" t="str">
-            <v>AMZN  260227C00255000</v>
+            <v>GOOGL 260227C00370000</v>
           </cell>
           <cell r="T28" t="str">
             <v>Short</v>
           </cell>
           <cell r="U28">
-            <v>-550</v>
+            <v>-234.5</v>
           </cell>
         </row>
         <row r="29">
@@ -2852,13 +2852,13 @@
             <v>OPT</v>
           </cell>
           <cell r="F29" t="str">
-            <v>GOOGL 260227P00310000</v>
+            <v>JPM   260206P00300000</v>
           </cell>
           <cell r="T29" t="str">
             <v>Short</v>
           </cell>
           <cell r="U29">
-            <v>-697.5</v>
+            <v>-530</v>
           </cell>
         </row>
         <row r="30">
@@ -2866,13 +2866,13 @@
             <v>OPT</v>
           </cell>
           <cell r="F30" t="str">
-            <v>GOOGL 260227C00370000</v>
+            <v>NVDA  260130C00195000</v>
           </cell>
           <cell r="T30" t="str">
             <v>Short</v>
           </cell>
           <cell r="U30">
-            <v>-365</v>
+            <v>-110</v>
           </cell>
         </row>
         <row r="31">
@@ -2880,69 +2880,55 @@
             <v>OPT</v>
           </cell>
           <cell r="F31" t="str">
-            <v>JPM   260206P00300000</v>
+            <v>ORCL  260123C00195000</v>
           </cell>
           <cell r="T31" t="str">
             <v>Short</v>
           </cell>
           <cell r="U31">
-            <v>-218.5</v>
+            <v>-29.5</v>
           </cell>
         </row>
         <row r="32">
           <cell r="D32" t="str">
-            <v>OPT</v>
+            <v>FOP</v>
           </cell>
           <cell r="F32" t="str">
-            <v>NVDA  260130C00195000</v>
+            <v>EW2G6 P6625</v>
           </cell>
           <cell r="T32" t="str">
             <v>Short</v>
           </cell>
           <cell r="U32">
-            <v>-356</v>
+            <v>-6075</v>
           </cell>
         </row>
         <row r="33">
           <cell r="D33" t="str">
-            <v>OPT</v>
+            <v>FOP</v>
           </cell>
           <cell r="F33" t="str">
-            <v>ORCL  260123C00195000</v>
+            <v>EW2G6 C7200</v>
           </cell>
           <cell r="T33" t="str">
             <v>Short</v>
           </cell>
           <cell r="U33">
-            <v>-275.5</v>
+            <v>-320</v>
           </cell>
         </row>
         <row r="34">
           <cell r="D34" t="str">
-            <v>FOP</v>
+            <v>CASH</v>
           </cell>
           <cell r="F34" t="str">
-            <v>EW2G6 P6625</v>
+            <v>USD</v>
           </cell>
           <cell r="T34" t="str">
-            <v>Short</v>
+            <v>Long</v>
           </cell>
           <cell r="U34">
-            <v>-2625</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="D35" t="str">
-            <v>FOP</v>
-          </cell>
-          <cell r="F35" t="str">
-            <v>EW2G6 C7200</v>
-          </cell>
-          <cell r="T35" t="str">
-            <v>Short</v>
-          </cell>
-          <cell r="U35">
-            <v>-1225</v>
+            <v>112742.88745569601</v>
           </cell>
         </row>
       </sheetData>
@@ -2972,7 +2958,7 @@
             <v>Long</v>
           </cell>
           <cell r="U2">
-            <v>54079.38</v>
+            <v>54127.216000000008</v>
           </cell>
         </row>
         <row r="3">
@@ -2986,7 +2972,7 @@
             <v>Long</v>
           </cell>
           <cell r="U3">
-            <v>3393.3530000000001</v>
+            <v>3341.91</v>
           </cell>
         </row>
         <row r="4">
@@ -3000,7 +2986,7 @@
             <v>Long</v>
           </cell>
           <cell r="U4">
-            <v>7381.7655000000004</v>
+            <v>7345.166400000001</v>
           </cell>
         </row>
         <row r="5">
@@ -3014,7 +3000,7 @@
             <v>Long</v>
           </cell>
           <cell r="U5">
-            <v>68957.032000000007</v>
+            <v>68789.406400000007</v>
           </cell>
         </row>
         <row r="6">
@@ -3028,7 +3014,7 @@
             <v>Long</v>
           </cell>
           <cell r="U6">
-            <v>38177.086499999998</v>
+            <v>38167.517699999997</v>
           </cell>
         </row>
         <row r="7">
@@ -3042,7 +3028,7 @@
             <v>Long</v>
           </cell>
           <cell r="U7">
-            <v>4297.1599299999998</v>
+            <v>4350.2092199999997</v>
           </cell>
         </row>
         <row r="8">
@@ -3056,7 +3042,7 @@
             <v>Long</v>
           </cell>
           <cell r="U8">
-            <v>2652</v>
+            <v>2484</v>
           </cell>
         </row>
         <row r="9">
@@ -3070,7 +3056,7 @@
             <v>Long</v>
           </cell>
           <cell r="U9">
-            <v>21660</v>
+            <v>21711</v>
           </cell>
         </row>
         <row r="10">
@@ -3084,7 +3070,7 @@
             <v>Long</v>
           </cell>
           <cell r="U10">
-            <v>16464</v>
+            <v>16182</v>
           </cell>
         </row>
         <row r="11">
@@ -3098,7 +3084,7 @@
             <v>Long</v>
           </cell>
           <cell r="U11">
-            <v>9267.5</v>
+            <v>9335</v>
           </cell>
         </row>
         <row r="12">
@@ -3112,7 +3098,7 @@
             <v>Long</v>
           </cell>
           <cell r="U12">
-            <v>1235.73</v>
+            <v>1204.57</v>
           </cell>
         </row>
         <row r="13">
@@ -3126,7 +3112,7 @@
             <v>Long</v>
           </cell>
           <cell r="U13">
-            <v>9986.59</v>
+            <v>9947.2800000000007</v>
           </cell>
         </row>
         <row r="14">
@@ -3140,7 +3126,7 @@
             <v>Long</v>
           </cell>
           <cell r="U14">
-            <v>31247</v>
+            <v>30274</v>
           </cell>
         </row>
         <row r="15">
@@ -3154,7 +3140,7 @@
             <v>Long</v>
           </cell>
           <cell r="U15">
-            <v>9939</v>
+            <v>9975.5</v>
           </cell>
         </row>
         <row r="16">
@@ -3168,7 +3154,7 @@
             <v>Long</v>
           </cell>
           <cell r="U16">
-            <v>137968</v>
+            <v>137664</v>
           </cell>
         </row>
         <row r="17">
@@ -3176,13 +3162,13 @@
             <v>OPT</v>
           </cell>
           <cell r="F17" t="str">
-            <v>AAPL  260130P00250000</v>
+            <v>GOOGL 260130P00310000</v>
           </cell>
           <cell r="T17" t="str">
             <v>Short</v>
           </cell>
           <cell r="U17">
-            <v>-355</v>
+            <v>-268.5</v>
           </cell>
         </row>
         <row r="18">
@@ -3190,13 +3176,13 @@
             <v>OPT</v>
           </cell>
           <cell r="F18" t="str">
-            <v>GOOGL 260130P00310000</v>
+            <v>JPM   260130C00325000</v>
           </cell>
           <cell r="T18" t="str">
             <v>Short</v>
           </cell>
           <cell r="U18">
-            <v>-136</v>
+            <v>-32.6</v>
           </cell>
         </row>
         <row r="19">
@@ -3204,27 +3190,27 @@
             <v>OPT</v>
           </cell>
           <cell r="F19" t="str">
-            <v>JPM   260130C00325000</v>
+            <v>QQQ   260130P00608000</v>
           </cell>
           <cell r="T19" t="str">
             <v>Short</v>
           </cell>
           <cell r="U19">
-            <v>-112</v>
+            <v>-949</v>
           </cell>
         </row>
         <row r="20">
           <cell r="D20" t="str">
-            <v>OPT</v>
+            <v>CASH</v>
           </cell>
           <cell r="F20" t="str">
-            <v>QQQ   260130P00608000</v>
+            <v>USD</v>
           </cell>
           <cell r="T20" t="str">
-            <v>Short</v>
+            <v>Long</v>
           </cell>
           <cell r="U20">
-            <v>-405.5</v>
+            <v>136454.94040422101</v>
           </cell>
         </row>
       </sheetData>
@@ -3522,7 +3508,7 @@
   <dimension ref="A1:M56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="38.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3630,11 +3616,11 @@
       </c>
       <c r="E4" s="19" cm="1">
         <f t="array" ref="E4">SUMPRODUCT(SUMIFS([1]PositionsHK!U:U,[1]PositionsHK!F:F,GlobalETF!A:A))</f>
-        <v>127127.16825</v>
+        <v>126883.51704999999</v>
       </c>
       <c r="F4" s="20">
         <f>E4/D4</f>
-        <v>0.95285870161584085</v>
+        <v>0.95103245810491344</v>
       </c>
       <c r="G4" s="19">
         <f>$G$2*B4</f>
@@ -3642,23 +3628,23 @@
       </c>
       <c r="H4" s="19" cm="1">
         <f t="array" ref="H4">SUMPRODUCT(SUMIFS([1]PositionsAL!U:U,[1]PositionsAL!F:F,GlobalETF!A:A))</f>
-        <v>299181.49849999999</v>
+        <v>298748.14010000002</v>
       </c>
       <c r="I4" s="20">
         <f>H4/G4</f>
-        <v>1.8038575425141612</v>
+        <v>1.801244691043161</v>
       </c>
       <c r="J4" s="25">
         <f t="shared" ref="J4:J21" si="0">E4+H4</f>
-        <v>426308.66674999997</v>
+        <v>425631.65714999998</v>
       </c>
       <c r="K4" s="20">
         <f t="shared" ref="K4:K21" si="1">J4/C4</f>
-        <v>1.4244804051884383</v>
+        <v>1.4222182252598046</v>
       </c>
       <c r="L4" s="19">
         <f t="shared" ref="L4:L21" si="2">J4-C4</f>
-        <v>127035.56675</v>
+        <v>126358.55715000001</v>
       </c>
       <c r="M4" s="34" t="s">
         <v>178</v>
@@ -3681,11 +3667,11 @@
       </c>
       <c r="E5" s="17">
         <f>SUMIFS([1]PositionsHK!U:U,[1]PositionsHK!F:F,"82846")</f>
-        <v>4562.625</v>
+        <v>4551.7582000000002</v>
       </c>
       <c r="F5" s="18">
         <f>E5/D5</f>
-        <v>0.34198330642513747</v>
+        <v>0.34116880508122677</v>
       </c>
       <c r="G5" s="17">
         <f>$G$4*B5</f>
@@ -3701,15 +3687,15 @@
       </c>
       <c r="J5" s="27">
         <f t="shared" ref="J5:J7" si="3">E5+H5</f>
-        <v>4562.625</v>
+        <v>4551.7582000000002</v>
       </c>
       <c r="K5" s="18">
         <f t="shared" ref="K5:K7" si="4">J5/C5</f>
-        <v>0.15245690307615353</v>
+        <v>0.15209379660250122</v>
       </c>
       <c r="L5" s="17">
         <f t="shared" ref="L5:L7" si="5">J5-C5</f>
-        <v>-25364.684999999998</v>
+        <v>-25375.551799999997</v>
       </c>
       <c r="M5" s="28"/>
     </row>
@@ -3742,23 +3728,23 @@
       </c>
       <c r="H6" s="17">
         <f>SUMIFS([1]PositionsAL!U:U,[1]PositionsAL!F:F,"DHL")</f>
-        <v>54079.38</v>
+        <v>54127.216000000008</v>
       </c>
       <c r="I6" s="18">
         <f t="shared" ref="I6:I7" si="10">H6/G6</f>
-        <v>1.6303063190167402</v>
+        <v>1.631748409016228</v>
       </c>
       <c r="J6" s="27">
         <f t="shared" si="3"/>
-        <v>54079.38</v>
+        <v>54127.216000000008</v>
       </c>
       <c r="K6" s="18">
         <f t="shared" si="4"/>
-        <v>0.90351221008503602</v>
+        <v>0.90431141322090114</v>
       </c>
       <c r="L6" s="17">
         <f t="shared" si="5"/>
-        <v>-5775.239999999998</v>
+        <v>-5727.4039999999877</v>
       </c>
       <c r="M6" s="28"/>
     </row>
@@ -3779,11 +3765,11 @@
       </c>
       <c r="E7" s="17">
         <f>SUMIFS([1]PositionsHK!U:U,[1]PositionsHK!F:F,"ES3")</f>
-        <v>19088.543249999999</v>
+        <v>19083.758849999998</v>
       </c>
       <c r="F7" s="18">
         <f t="shared" si="8"/>
-        <v>0.71537362104865498</v>
+        <v>0.71519431802339428</v>
       </c>
       <c r="G7" s="17">
         <f t="shared" si="9"/>
@@ -3791,23 +3777,23 @@
       </c>
       <c r="H7" s="17">
         <f>SUMIFS([1]PositionsAL!U:U,[1]PositionsAL!F:F,"ES3")</f>
-        <v>38177.086499999998</v>
+        <v>38167.517699999997</v>
       </c>
       <c r="I7" s="18">
         <f t="shared" si="10"/>
-        <v>1.150907154678894</v>
+        <v>1.1506186884445286</v>
       </c>
       <c r="J7" s="27">
         <f t="shared" si="3"/>
-        <v>57265.629749999993</v>
+        <v>57251.276549999995</v>
       </c>
       <c r="K7" s="18">
         <f t="shared" si="4"/>
-        <v>0.95674535649879655</v>
+        <v>0.95650555546088167</v>
       </c>
       <c r="L7" s="17">
         <f t="shared" si="5"/>
-        <v>-2588.9902500000026</v>
+        <v>-2603.3434500000003</v>
       </c>
       <c r="M7" s="28"/>
     </row>
@@ -3828,11 +3814,11 @@
       </c>
       <c r="E8" s="17">
         <f>SUMIFS([1]PositionsHK!U:U,[1]PositionsHK!F:F,"VWRA")</f>
-        <v>103476</v>
+        <v>103248</v>
       </c>
       <c r="F8" s="18">
         <f>E8/D8</f>
-        <v>3.1023425870543844</v>
+        <v>3.0955068559684475</v>
       </c>
       <c r="G8" s="17">
         <f t="shared" si="9"/>
@@ -3840,23 +3826,23 @@
       </c>
       <c r="H8" s="17">
         <f>SUMIFS([1]PositionsAL!U:U,[1]PositionsAL!F:F,"VWRA")</f>
-        <v>137968</v>
+        <v>137664</v>
       </c>
       <c r="I8" s="18">
         <f>H8/G8</f>
-        <v>3.3274065231088321</v>
+        <v>3.3200748840111785</v>
       </c>
       <c r="J8" s="27">
         <f>E8+H8</f>
-        <v>241444</v>
+        <v>240912</v>
       </c>
       <c r="K8" s="18">
         <f>J8/C8</f>
-        <v>3.227072530073702</v>
+        <v>3.2199619678480964</v>
       </c>
       <c r="L8" s="17">
         <f>J8-C8</f>
-        <v>166625.72500000001</v>
+        <v>166093.72500000001</v>
       </c>
       <c r="M8" s="28"/>
     </row>
@@ -3889,23 +3875,23 @@
       </c>
       <c r="H9" s="17">
         <f>SUMIFS([1]PositionsAL!U:U,[1]PositionsAL!F:F,"VWCE")</f>
-        <v>68957.032000000007</v>
+        <v>68789.406400000007</v>
       </c>
       <c r="I9" s="18">
         <f>H9/G9</f>
-        <v>1.6630528679913059</v>
+        <v>1.6590102021928597</v>
       </c>
       <c r="J9" s="27">
         <f>E9+H9</f>
-        <v>68957.032000000007</v>
+        <v>68789.406400000007</v>
       </c>
       <c r="K9" s="18">
         <f>J9/C9</f>
-        <v>0.92166027618252377</v>
+        <v>0.91941983960469564</v>
       </c>
       <c r="L9" s="17">
         <f>J9-C9</f>
-        <v>-5861.2429999999877</v>
+        <v>-6028.8685999999871</v>
       </c>
       <c r="M9" s="28"/>
     </row>
@@ -3926,11 +3912,11 @@
       </c>
       <c r="E10" s="19">
         <f>E11+E12+E13+E15+E14</f>
-        <v>54609.09</v>
+        <v>54519.78</v>
       </c>
       <c r="F10" s="20">
         <f>E10/D10</f>
-        <v>0.4093125593067129</v>
+        <v>0.40864315235135656</v>
       </c>
       <c r="G10" s="19">
         <f>$G$2*B10</f>
@@ -3938,23 +3924,23 @@
       </c>
       <c r="H10" s="19">
         <f>H11+H12+H13+H15+H14</f>
-        <v>67317.09</v>
+        <v>67150.78</v>
       </c>
       <c r="I10" s="20">
         <f>H10/G10</f>
-        <v>0.40587550080943463</v>
+        <v>0.40487276651804421</v>
       </c>
       <c r="J10" s="25">
         <f>E10+H10</f>
-        <v>121926.18</v>
+        <v>121670.56</v>
       </c>
       <c r="K10" s="18">
         <f>J10/C10</f>
-        <v>0.40740774897576831</v>
+        <v>0.40655361273699508</v>
       </c>
       <c r="L10" s="19">
         <f t="shared" si="2"/>
-        <v>-177346.91999999998</v>
+        <v>-177602.53999999998</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -3962,47 +3948,47 @@
         <v>15</v>
       </c>
       <c r="B11" s="26">
-        <v>0.35</v>
+        <v>0.45</v>
       </c>
       <c r="C11" s="17">
         <f>$C$10*B11</f>
-        <v>104745.58499999999</v>
+        <v>134672.89499999999</v>
       </c>
       <c r="D11" s="17">
         <f t="shared" ref="D11:D15" si="11">$D$10*B11</f>
-        <v>46695.81</v>
+        <v>60037.47</v>
       </c>
       <c r="E11" s="17">
         <f>SUMIFS([1]PositionsHK!U:U,[1]PositionsHK!F:F,"CSNDX")</f>
-        <v>14440</v>
+        <v>14474</v>
       </c>
       <c r="F11" s="18">
         <f>E11/D11</f>
-        <v>0.30923545388761864</v>
+        <v>0.24108277713901002</v>
       </c>
       <c r="G11" s="17">
         <f t="shared" ref="G11:G15" si="12">$G$10*B11</f>
-        <v>58049.774999999994</v>
+        <v>74635.425000000003</v>
       </c>
       <c r="H11" s="17">
         <f>SUMIFS([1]PositionsAL!U:U,[1]PositionsAL!F:F,"CSNDX")</f>
-        <v>21660</v>
+        <v>21711</v>
       </c>
       <c r="I11" s="18">
         <f>H11/G11</f>
-        <v>0.37312806121987557</v>
+        <v>0.29089403590855145</v>
       </c>
       <c r="J11" s="27">
         <f t="shared" si="0"/>
-        <v>36100</v>
+        <v>36185</v>
       </c>
       <c r="K11" s="18">
         <f t="shared" si="1"/>
-        <v>0.34464459766967748</v>
+        <v>0.2686880682263495</v>
       </c>
       <c r="L11" s="17">
         <f t="shared" si="2"/>
-        <v>-68645.584999999992</v>
+        <v>-98487.89499999999</v>
       </c>
       <c r="M11" s="28"/>
     </row>
@@ -4023,11 +4009,11 @@
       </c>
       <c r="E12" s="17">
         <f>SUMIFS([1]PositionsHK!U:U,[1]PositionsHK!F:F,"CTEC")</f>
-        <v>10976</v>
+        <v>10788</v>
       </c>
       <c r="F12" s="18">
         <f t="shared" ref="F12:F15" si="13">E12/D12</f>
-        <v>0.41134311622391811</v>
+        <v>0.40429751620113236</v>
       </c>
       <c r="G12" s="17">
         <f t="shared" si="12"/>
@@ -4035,23 +4021,23 @@
       </c>
       <c r="H12" s="17">
         <f>SUMIFS([1]PositionsAL!U:U,[1]PositionsAL!F:F,"CTEC")</f>
-        <v>16464</v>
+        <v>16182</v>
       </c>
       <c r="I12" s="18">
         <f t="shared" ref="I12:I15" si="14">H12/G12</f>
-        <v>0.49633267312405599</v>
+        <v>0.48783134818352003</v>
       </c>
       <c r="J12" s="27">
         <f t="shared" si="0"/>
-        <v>27440</v>
+        <v>26970</v>
       </c>
       <c r="K12" s="18">
         <f t="shared" si="1"/>
-        <v>0.45844414349301693</v>
+        <v>0.45059178389237126</v>
       </c>
       <c r="L12" s="17">
         <f t="shared" si="2"/>
-        <v>-32414.619999999995</v>
+        <v>-32884.619999999995</v>
       </c>
       <c r="M12" s="28"/>
     </row>
@@ -4060,47 +4046,47 @@
         <v>175</v>
       </c>
       <c r="B13" s="26">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="C13" s="17">
         <f>$C$10*B13</f>
-        <v>44890.964999999997</v>
+        <v>29927.309999999998</v>
       </c>
       <c r="D13" s="17">
         <f t="shared" si="11"/>
-        <v>20012.490000000002</v>
+        <v>13341.660000000002</v>
       </c>
       <c r="E13" s="17">
         <f>SUMIFS([1]PositionsHK!U:U,[1]PositionsHK!F:F,"HEAL")</f>
-        <v>9267.5</v>
+        <v>9335</v>
       </c>
       <c r="F13" s="18">
         <f t="shared" si="13"/>
-        <v>0.46308580291607887</v>
+        <v>0.69968804481601232</v>
       </c>
       <c r="G13" s="17">
         <f t="shared" si="12"/>
-        <v>24878.474999999999</v>
+        <v>16585.650000000001</v>
       </c>
       <c r="H13" s="17">
         <f>SUMIFS([1]PositionsAL!U:U,[1]PositionsAL!F:F,"HEAL")</f>
-        <v>9267.5</v>
+        <v>9335</v>
       </c>
       <c r="I13" s="18">
         <f t="shared" si="14"/>
-        <v>0.37251077487667555</v>
+        <v>0.56283594553122729</v>
       </c>
       <c r="J13" s="27">
         <f t="shared" si="0"/>
-        <v>18535</v>
+        <v>18670</v>
       </c>
       <c r="K13" s="18">
         <f t="shared" si="1"/>
-        <v>0.4128893197105476</v>
+        <v>0.62384490954917104</v>
       </c>
       <c r="L13" s="17">
         <f t="shared" si="2"/>
-        <v>-26355.964999999997</v>
+        <v>-11257.309999999998</v>
       </c>
       <c r="M13" s="28"/>
     </row>
@@ -4109,47 +4095,47 @@
         <v>22</v>
       </c>
       <c r="B14" s="26">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="C14" s="17">
         <f>$C$10*B14</f>
-        <v>44890.964999999997</v>
+        <v>29927.309999999998</v>
       </c>
       <c r="D14" s="17">
         <f>$D$10*B14</f>
-        <v>20012.490000000002</v>
+        <v>13341.660000000002</v>
       </c>
       <c r="E14" s="17">
         <f>SUMIFS([1]PositionsHK!U:U,[1]PositionsHK!F:F,"INRA")</f>
-        <v>9986.59</v>
+        <v>9947.2800000000007</v>
       </c>
       <c r="F14" s="18">
         <f>E14/D14</f>
-        <v>0.49901786334434145</v>
+        <v>0.7455803850495365</v>
       </c>
       <c r="G14" s="17">
         <f>$G$10*B14</f>
-        <v>24878.474999999999</v>
+        <v>16585.650000000001</v>
       </c>
       <c r="H14" s="17">
         <f>SUMIFS([1]PositionsAL!U:U,[1]PositionsAL!F:F,"INRA")</f>
-        <v>9986.59</v>
+        <v>9947.2800000000007</v>
       </c>
       <c r="I14" s="18">
         <f>H14/G14</f>
-        <v>0.40141487772059986</v>
+        <v>0.59975219542194602</v>
       </c>
       <c r="J14" s="27">
         <f>E14+H14</f>
-        <v>19973.18</v>
+        <v>19894.560000000001</v>
       </c>
       <c r="K14" s="18">
         <f>J14/C14</f>
-        <v>0.44492650135723305</v>
+        <v>0.66476272007073145</v>
       </c>
       <c r="L14" s="17">
         <f>J14-C14</f>
-        <v>-24917.784999999996</v>
+        <v>-10032.749999999996</v>
       </c>
       <c r="M14" s="28"/>
     </row>
@@ -4170,11 +4156,11 @@
       </c>
       <c r="E15" s="17">
         <f>SUMIFS([1]PositionsHK!U:U,[1]PositionsHK!F:F,"LOCK")</f>
-        <v>9939</v>
+        <v>9975.5</v>
       </c>
       <c r="F15" s="18">
         <f t="shared" si="13"/>
-        <v>0.49663984841466502</v>
+        <v>0.49846370941347123</v>
       </c>
       <c r="G15" s="17">
         <f t="shared" si="12"/>
@@ -4182,23 +4168,23 @@
       </c>
       <c r="H15" s="17">
         <f>SUMIFS([1]PositionsAL!U:U,[1]PositionsAL!F:F,"LOCK")</f>
-        <v>9939</v>
+        <v>9975.5</v>
       </c>
       <c r="I15" s="18">
         <f t="shared" si="14"/>
-        <v>0.39950197912050478</v>
+        <v>0.40096911084783132</v>
       </c>
       <c r="J15" s="27">
         <f t="shared" si="0"/>
-        <v>19878</v>
+        <v>19951</v>
       </c>
       <c r="K15" s="18">
         <f t="shared" si="1"/>
-        <v>0.44280625288407149</v>
+        <v>0.44443241529782224</v>
       </c>
       <c r="L15" s="17">
         <f t="shared" si="2"/>
-        <v>-25012.964999999997</v>
+        <v>-24939.964999999997</v>
       </c>
       <c r="M15" s="28"/>
     </row>
@@ -4219,11 +4205,11 @@
       </c>
       <c r="E16" s="19" cm="1">
         <f t="array" ref="E16">SUMPRODUCT(SUMIFS([1]PositionsHK!U:U,[1]PositionsHK!F:F,IncomeStrategy!A:A))</f>
-        <v>113267</v>
+        <v>108906</v>
       </c>
       <c r="F16" s="20">
         <f>E16/D16</f>
-        <v>1.0187667801457989</v>
+        <v>0.97954227584873244</v>
       </c>
       <c r="G16" s="19">
         <f>$G$2*B16</f>
@@ -4231,23 +4217,23 @@
       </c>
       <c r="H16" s="19" cm="1">
         <f t="array" ref="H16">SUMPRODUCT(SUMIFS([1]PositionsAL!U:U,[1]PositionsAL!F:F,IncomeStrategy!A:A))</f>
-        <v>31247</v>
+        <v>30274</v>
       </c>
       <c r="I16" s="20">
         <f t="shared" ref="I16:I21" si="15">H16/G16</f>
-        <v>0.22607736205695889</v>
+        <v>0.21903754148917889</v>
       </c>
       <c r="J16" s="25">
         <f t="shared" si="0"/>
-        <v>144514</v>
+        <v>139180</v>
       </c>
       <c r="K16" s="20">
         <f t="shared" si="1"/>
-        <v>0.57946003165670423</v>
+        <v>0.55807220896231569</v>
       </c>
       <c r="L16" s="19">
         <f t="shared" si="2"/>
-        <v>-104880.25</v>
+        <v>-110214.25</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -4267,11 +4253,11 @@
       </c>
       <c r="E17" s="19">
         <f>E18+E19</f>
-        <v>30137.775500000018</v>
+        <v>24355.186399999984</v>
       </c>
       <c r="F17" s="20">
         <f>E17/D17</f>
-        <v>1.3553534792522077</v>
+        <v>1.0952993735412226</v>
       </c>
       <c r="G17" s="19">
         <f>$G$2*B17</f>
@@ -4279,23 +4265,23 @@
       </c>
       <c r="H17" s="19">
         <f>H18+H19</f>
-        <v>14662.848500000016</v>
+        <v>14375.646400000016</v>
       </c>
       <c r="I17" s="20">
         <f>H17/G17</f>
-        <v>0.5304410197972349</v>
+        <v>0.52005123947508902</v>
       </c>
       <c r="J17" s="25">
         <f>E17+H17</f>
-        <v>44800.624000000033</v>
+        <v>38730.832800000004</v>
       </c>
       <c r="K17" s="20">
         <f t="shared" si="1"/>
-        <v>0.89818879144166375</v>
+        <v>0.77649811092276588</v>
       </c>
       <c r="L17" s="19">
         <f t="shared" si="2"/>
-        <v>-5078.2259999999733</v>
+        <v>-11148.017200000002</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -4303,47 +4289,47 @@
         <v>173</v>
       </c>
       <c r="B18" s="29">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="C18" s="15">
         <f>$C$17*B18</f>
-        <v>29927.31</v>
+        <v>24939.425000000003</v>
       </c>
       <c r="D18" s="15">
         <f>$D$17*B18</f>
-        <v>13341.660000000002</v>
+        <v>11118.050000000001</v>
       </c>
       <c r="E18" s="15" cm="1">
         <f t="array" ref="E18">SUMIFS([1]PositionsHK!U:U,[1]PositionsHK!D:D,"STK")-SUMPRODUCT(SUMIFS([1]PositionsHK!U:U,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,GlobalETF!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!U:U,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,GrowthEngine!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!U:U,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,IncomeStrategy!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!U:U,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,Gold!A:A))</f>
-        <v>27887.775500000018</v>
+        <v>19815.186399999984</v>
       </c>
       <c r="F18" s="16">
         <f t="shared" ref="F18:F21" si="16">E18/G18</f>
-        <v>1.6814400098880673</v>
+        <v>1.4336624539888385</v>
       </c>
       <c r="G18" s="15">
         <f>$G$17*B18</f>
-        <v>16585.649999999998</v>
+        <v>13821.375</v>
       </c>
       <c r="H18" s="15" cm="1">
         <f t="array" ref="H18">SUMIFS([1]PositionsAL!U:U,[1]PositionsAL!D:D,"STK")-SUMPRODUCT(SUMIFS([1]PositionsAL!U:U,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,GlobalETF!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!U:U,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,GrowthEngine!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!U:U,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,IncomeStrategy!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!U:U,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,Gold!A:A))</f>
-        <v>14662.848500000016</v>
+        <v>14375.646400000016</v>
       </c>
       <c r="I18" s="16">
         <f>H18/G18</f>
-        <v>0.88406836632872499</v>
+        <v>1.040102478950178</v>
       </c>
       <c r="J18" s="30">
         <f t="shared" si="0"/>
-        <v>42550.624000000033</v>
+        <v>34190.832800000004</v>
       </c>
       <c r="K18" s="16">
         <f t="shared" si="1"/>
-        <v>1.4217991526802787</v>
+        <v>1.3709551362952435</v>
       </c>
       <c r="L18" s="15">
         <f t="shared" si="2"/>
-        <v>12623.314000000031</v>
+        <v>9251.4078000000009</v>
       </c>
       <c r="M18" s="31"/>
     </row>
@@ -4352,27 +4338,27 @@
         <v>184</v>
       </c>
       <c r="B19" s="29">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="C19" s="15">
         <f>$C$17*B19</f>
-        <v>19951.540000000005</v>
+        <v>24939.425000000003</v>
       </c>
       <c r="D19" s="15">
         <f>$D$17*B19</f>
-        <v>8894.44</v>
+        <v>11118.050000000001</v>
       </c>
       <c r="E19" s="15">
         <f>SUMIFS([1]PositionsHK!U:U,[1]PositionsHK!D:D,"OPT",[1]PositionsHK!T:T,"Long")+SUMIFS([1]PositionsHK!U:U,[1]PositionsHK!D:D,"FOP",[1]PositionsHK!T:T,"Long")</f>
-        <v>2250</v>
+        <v>4540</v>
       </c>
       <c r="F19" s="16">
         <f t="shared" si="16"/>
-        <v>0.20348916081070081</v>
+        <v>0.32847672536198463</v>
       </c>
       <c r="G19" s="15">
         <f>$G$17*B19</f>
-        <v>11057.1</v>
+        <v>13821.375</v>
       </c>
       <c r="H19" s="15">
         <f>SUMIFS([1]PositionsAL!U:U,[1]PositionsAL!D:D,"OPT",[1]PositionsAL!T:T,"Long")+SUMIFS([1]PositionsAL!U:U,[1]PositionsAL!D:D,"FOP",[1]PositionsAL!T:T,"Long")</f>
@@ -4384,15 +4370,15 @@
       </c>
       <c r="J19" s="30">
         <f t="shared" si="0"/>
-        <v>2250</v>
+        <v>4540</v>
       </c>
       <c r="K19" s="16">
         <f t="shared" si="1"/>
-        <v>0.11277324958374138</v>
+        <v>0.18204108555028833</v>
       </c>
       <c r="L19" s="15">
         <f t="shared" si="2"/>
-        <v>-17701.540000000005</v>
+        <v>-20399.425000000003</v>
       </c>
       <c r="M19" s="31"/>
     </row>
@@ -4413,11 +4399,11 @@
       </c>
       <c r="E20" s="19">
         <f>SUMIFS([1]PositionsHK!U:U,[1]PositionsHK!F:F,"GSD")</f>
-        <v>21485.799650000001</v>
+        <v>21751.0461</v>
       </c>
       <c r="F20" s="20">
         <f t="shared" si="16"/>
-        <v>1.2954451378149185</v>
+        <v>1.3114376644870718</v>
       </c>
       <c r="G20" s="19">
         <f>$G$2*B20</f>
@@ -4425,23 +4411,23 @@
       </c>
       <c r="H20" s="19">
         <f>SUMIFS([1]PositionsAL!U:U,[1]PositionsAL!F:F,"GSD")</f>
-        <v>4297.1599299999998</v>
+        <v>4350.2092199999997</v>
       </c>
       <c r="I20" s="20">
         <f t="shared" si="15"/>
-        <v>0.25908902756298369</v>
+        <v>0.26228753289741435</v>
       </c>
       <c r="J20" s="25">
         <f t="shared" si="0"/>
-        <v>25782.959580000002</v>
+        <v>26101.25532</v>
       </c>
       <c r="K20" s="20">
         <f t="shared" si="1"/>
-        <v>0.86151944762158728</v>
+        <v>0.87215507574853879</v>
       </c>
       <c r="L20" s="19">
         <f t="shared" si="2"/>
-        <v>-4144.3504199999952</v>
+        <v>-3826.0546799999975</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -4460,34 +4446,36 @@
         <v>31130.540000000005</v>
       </c>
       <c r="E21" s="32">
-        <v>105000</v>
+        <f>SUMIFS([1]PositionsHK!$U:$U,[1]PositionsHK!$D:$D,"CASH")</f>
+        <v>112742.88745569601</v>
       </c>
       <c r="F21" s="20">
         <f t="shared" si="16"/>
-        <v>2.7131888108093438</v>
+        <v>2.9132641975536337</v>
       </c>
       <c r="G21" s="19">
         <f>$G$2*B21</f>
         <v>38699.850000000006</v>
       </c>
       <c r="H21" s="32">
-        <v>137000</v>
+        <f>SUMIFS([1]PositionsAL!$U:$U,[1]PositionsAL!$D:$D,"CASH")</f>
+        <v>136454.94040422101</v>
       </c>
       <c r="I21" s="20">
         <f t="shared" si="15"/>
-        <v>3.5400654007702865</v>
+        <v>3.5259811188989358</v>
       </c>
       <c r="J21" s="25">
         <f t="shared" si="0"/>
-        <v>242000</v>
+        <v>249197.82785991702</v>
       </c>
       <c r="K21" s="20">
         <f t="shared" si="1"/>
-        <v>3.4655398602241805</v>
+        <v>3.56861572532986</v>
       </c>
       <c r="L21" s="19">
         <f t="shared" si="2"/>
-        <v>172169.61</v>
+        <v>179367.437859917</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -4500,13 +4488,13 @@
       <c r="D22" s="10"/>
       <c r="E22" s="12">
         <f>E4+E10+E16+E20+E21+E18-E19</f>
-        <v>447126.8334</v>
+        <v>440078.41700569598</v>
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
       <c r="H22" s="12">
         <f>H4+H10+H16+H20+H21+H18-H19</f>
-        <v>553705.59692999988</v>
+        <v>551353.71612422098</v>
       </c>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
@@ -4542,7 +4530,7 @@
       </c>
       <c r="C50" s="39">
         <f>J4</f>
-        <v>426308.66674999997</v>
+        <v>425631.65714999998</v>
       </c>
       <c r="D50" s="40"/>
       <c r="E50" s="40"/>
@@ -4558,7 +4546,7 @@
       </c>
       <c r="C51" s="39">
         <f>J10</f>
-        <v>121926.18</v>
+        <v>121670.56</v>
       </c>
       <c r="D51" s="40"/>
       <c r="E51" s="40"/>
@@ -4574,7 +4562,7 @@
       </c>
       <c r="C52" s="39">
         <f>J16</f>
-        <v>144514</v>
+        <v>139180</v>
       </c>
       <c r="D52" s="40"/>
       <c r="E52" s="40"/>
@@ -4586,11 +4574,11 @@
       </c>
       <c r="B53" s="38">
         <f>C18</f>
-        <v>29927.31</v>
+        <v>24939.425000000003</v>
       </c>
       <c r="C53" s="39">
         <f>J18</f>
-        <v>42550.624000000033</v>
+        <v>34190.832800000004</v>
       </c>
       <c r="D53" s="40"/>
       <c r="E53" s="40"/>
@@ -4602,11 +4590,11 @@
       </c>
       <c r="B54" s="38">
         <f>C19</f>
-        <v>19951.540000000005</v>
+        <v>24939.425000000003</v>
       </c>
       <c r="C54" s="39">
         <f>J19</f>
-        <v>2250</v>
+        <v>4540</v>
       </c>
       <c r="D54" s="40"/>
       <c r="E54" s="40"/>
@@ -4622,7 +4610,7 @@
       </c>
       <c r="C55" s="39">
         <f>J20</f>
-        <v>25782.959580000002</v>
+        <v>26101.25532</v>
       </c>
       <c r="D55" s="40"/>
       <c r="E55" s="40"/>
@@ -4638,7 +4626,7 @@
       </c>
       <c r="C56" s="39">
         <f>J21</f>
-        <v>242000</v>
+        <v>249197.82785991702</v>
       </c>
       <c r="D56" s="40"/>
       <c r="E56" s="40"/>

</xml_diff>

<commit_message>
refactor: Remove unnecessary separator from decision matrix alert message
</commit_message>
<xml_diff>
--- a/projects/fetch-ibkr-positions-dashboard.xlsx
+++ b/projects/fetch-ibkr-positions-dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hongkiatkoh/Desktop/timeless-workspace/timeless-workspace/projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2E2D67-1AEB-A24E-A533-76FE915E0E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F66060B-6D58-A346-B98C-08A55684299C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7080" yWindow="1300" windowWidth="32100" windowHeight="25120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14300" yWindow="1480" windowWidth="32100" windowHeight="25120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -1585,25 +1585,25 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>300948.26328000001</c:v>
+                  <c:v>238220.33627999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>300948.26328000001</c:v>
+                  <c:v>238220.33627999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>250790.2194</c:v>
+                  <c:v>198516.94690000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25079.021940000002</c:v>
+                  <c:v>19851.694690000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25079.021940000002</c:v>
+                  <c:v>19851.694690000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30094.826327999999</c:v>
+                  <c:v>23822.033628000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70221.261432000014</c:v>
+                  <c:v>55584.745132000011</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1750,7 +1750,7 @@
                   <c:v>27241.483500000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>209093.09000000003</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2183,10 +2183,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.79156574516717371</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20843425483282627</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4297,12 +4297,12 @@
       <sheetData sheetId="2">
         <row r="2">
           <cell r="C2" t="str">
-            <v>$103,358.02</v>
+            <v>$0.00</v>
           </cell>
         </row>
         <row r="3">
           <cell r="C3" t="str">
-            <v>$105,735.07</v>
+            <v>$0.00</v>
           </cell>
         </row>
       </sheetData>
@@ -4640,13 +4640,13 @@
       </c>
       <c r="D2" s="33">
         <f>E4+E10+E16+E20+E21+E18-E19</f>
-        <v>445194.83935000008</v>
+        <v>341836.81935000006</v>
       </c>
       <c r="E2" s="34"/>
       <c r="F2" s="42"/>
       <c r="G2" s="33">
         <f>H4+H10+H16+H20+H21+H18-H19</f>
-        <v>557966.03824999987</v>
+        <v>452230.96824999998</v>
       </c>
       <c r="H2" s="34"/>
       <c r="I2" s="42"/>
@@ -4700,11 +4700,11 @@
       </c>
       <c r="C4" s="26">
         <f>$F$40*B4</f>
-        <v>300948.26328000001</v>
+        <v>238220.33627999999</v>
       </c>
       <c r="D4" s="36">
         <f>$D$2*B4</f>
-        <v>133558.45180500002</v>
+        <v>102551.04580500002</v>
       </c>
       <c r="E4" s="26" cm="1">
         <f t="array" ref="E4">SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,GlobalETF!A:A))</f>
@@ -4712,11 +4712,11 @@
       </c>
       <c r="F4" s="44">
         <f>E4/D4</f>
-        <v>0.96079745883364598</v>
+        <v>1.2513048510885438</v>
       </c>
       <c r="G4" s="36">
         <f>$G$2*B4</f>
-        <v>167389.81147499997</v>
+        <v>135669.29047499999</v>
       </c>
       <c r="H4" s="26" cm="1">
         <f t="array" ref="H4">SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,GlobalETF!A:A))</f>
@@ -4724,7 +4724,7 @@
       </c>
       <c r="I4" s="44">
         <f>H4/G4</f>
-        <v>1.8063448828554221</v>
+        <v>2.2286821751729962</v>
       </c>
       <c r="J4" s="53">
         <f t="shared" ref="J4:J21" si="0">E4+H4</f>
@@ -4732,7 +4732,7 @@
       </c>
       <c r="K4" s="44">
         <f t="shared" ref="K4:K21" si="1">J4/C4</f>
-        <v>1.4310976438474829</v>
+        <v>1.8079327618519472</v>
       </c>
       <c r="L4" s="17" t="s">
         <v>175</v>
@@ -4747,11 +4747,11 @@
       </c>
       <c r="C5" s="27">
         <f>$C$4*B5</f>
-        <v>30094.826328000003</v>
+        <v>23822.033628000001</v>
       </c>
       <c r="D5" s="37">
         <f>$D$4*B5</f>
-        <v>13355.845180500002</v>
+        <v>10255.104580500003</v>
       </c>
       <c r="E5" s="27">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"82846")</f>
@@ -4759,11 +4759,11 @@
       </c>
       <c r="F5" s="45">
         <f>E5/D5</f>
-        <v>0.34006081521753379</v>
+        <v>0.4428818413647575</v>
       </c>
       <c r="G5" s="37">
         <f>$G$4*B5</f>
-        <v>16738.981147499999</v>
+        <v>13566.9290475</v>
       </c>
       <c r="H5" s="27">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"82846")</f>
@@ -4779,7 +4779,7 @@
       </c>
       <c r="K5" s="45">
         <f t="shared" ref="K5:K7" si="3">J5/C5</f>
-        <v>0.15091629207291168</v>
+        <v>0.19065541048777837</v>
       </c>
       <c r="L5" s="14"/>
     </row>
@@ -4792,11 +4792,11 @@
       </c>
       <c r="C6" s="27">
         <f t="shared" ref="C6:C9" si="4">$C$4*B6</f>
-        <v>60189.652656000006</v>
+        <v>47644.067256000002</v>
       </c>
       <c r="D6" s="37">
         <f t="shared" ref="D6:D9" si="5">$D$4*B6</f>
-        <v>26711.690361000004</v>
+        <v>20510.209161000006</v>
       </c>
       <c r="E6" s="27">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"DHL")</f>
@@ -4808,7 +4808,7 @@
       </c>
       <c r="G6" s="37">
         <f t="shared" ref="G6:G9" si="7">$G$4*B6</f>
-        <v>33477.962294999998</v>
+        <v>27133.858095</v>
       </c>
       <c r="H6" s="27">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"DHL")</f>
@@ -4816,7 +4816,7 @@
       </c>
       <c r="I6" s="45">
         <f t="shared" ref="I6:I7" si="8">H6/G6</f>
-        <v>1.6252124164715387</v>
+        <v>2.005199548457357</v>
       </c>
       <c r="J6" s="54">
         <f t="shared" si="2"/>
@@ -4824,7 +4824,7 @@
       </c>
       <c r="K6" s="45">
         <f t="shared" si="3"/>
-        <v>0.90395603893846799</v>
+        <v>1.1419847870596751</v>
       </c>
       <c r="L6" s="14"/>
     </row>
@@ -4837,11 +4837,11 @@
       </c>
       <c r="C7" s="27">
         <f t="shared" si="4"/>
-        <v>60189.652656000006</v>
+        <v>47644.067256000002</v>
       </c>
       <c r="D7" s="37">
         <f t="shared" si="5"/>
-        <v>26711.690361000004</v>
+        <v>20510.209161000006</v>
       </c>
       <c r="E7" s="27">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"ES3")</f>
@@ -4849,11 +4849,11 @@
       </c>
       <c r="F7" s="45">
         <f t="shared" si="6"/>
-        <v>0.73139592575258494</v>
+        <v>0.95254130987357766</v>
       </c>
       <c r="G7" s="37">
         <f t="shared" si="7"/>
-        <v>33477.962294999998</v>
+        <v>27133.858095</v>
       </c>
       <c r="H7" s="27">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"ES3")</f>
@@ -4861,7 +4861,7 @@
       </c>
       <c r="I7" s="45">
         <f t="shared" si="8"/>
-        <v>1.1671452000480844</v>
+        <v>1.4400327024338702</v>
       </c>
       <c r="J7" s="54">
         <f t="shared" si="2"/>
@@ -4869,7 +4869,7 @@
       </c>
       <c r="K7" s="45">
         <f t="shared" si="3"/>
-        <v>0.97376312893803363</v>
+        <v>1.2301734061677732</v>
       </c>
       <c r="L7" s="14"/>
     </row>
@@ -4882,11 +4882,11 @@
       </c>
       <c r="C8" s="27">
         <f t="shared" si="4"/>
-        <v>75237.065820000003</v>
+        <v>59555.084069999997</v>
       </c>
       <c r="D8" s="37">
         <f t="shared" si="5"/>
-        <v>33389.612951250005</v>
+        <v>25637.761451250004</v>
       </c>
       <c r="E8" s="27">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"VWRA")</f>
@@ -4894,11 +4894,11 @@
       </c>
       <c r="F8" s="45">
         <f>E8/D8</f>
-        <v>3.1220487686455023</v>
+        <v>4.0660336199094109</v>
       </c>
       <c r="G8" s="37">
         <f t="shared" si="7"/>
-        <v>41847.452868749991</v>
+        <v>33917.322618749997</v>
       </c>
       <c r="H8" s="27">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"VWRA")</f>
@@ -4906,7 +4906,7 @@
       </c>
       <c r="I8" s="45">
         <f>H8/G8</f>
-        <v>3.3213968944760719</v>
+        <v>4.0979649709485964</v>
       </c>
       <c r="J8" s="54">
         <f>E8+H8</f>
@@ -4914,7 +4914,7 @@
       </c>
       <c r="K8" s="45">
         <f>J8/C8</f>
-        <v>3.2329277776718057</v>
+        <v>4.0842189008432044</v>
       </c>
       <c r="L8" s="14"/>
     </row>
@@ -4927,11 +4927,11 @@
       </c>
       <c r="C9" s="27">
         <f t="shared" si="4"/>
-        <v>75237.065820000003</v>
+        <v>59555.084069999997</v>
       </c>
       <c r="D9" s="37">
         <f t="shared" si="5"/>
-        <v>33389.612951250005</v>
+        <v>25637.761451250004</v>
       </c>
       <c r="E9" s="27">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"VWCE")</f>
@@ -4943,7 +4943,7 @@
       </c>
       <c r="G9" s="37">
         <f t="shared" si="7"/>
-        <v>41847.452868749991</v>
+        <v>33917.322618749997</v>
       </c>
       <c r="H9" s="27">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"VWCE")</f>
@@ -4951,7 +4951,7 @@
       </c>
       <c r="I9" s="45">
         <f>H9/G9</f>
-        <v>1.6700965437299178</v>
+        <v>2.0605779290304054</v>
       </c>
       <c r="J9" s="54">
         <f>E9+H9</f>
@@ -4959,7 +4959,7 @@
       </c>
       <c r="K9" s="45">
         <f>J9/C9</f>
-        <v>0.92892094658775992</v>
+        <v>1.1735234277875146</v>
       </c>
       <c r="L9" s="14"/>
     </row>
@@ -4972,11 +4972,11 @@
       </c>
       <c r="C10" s="26">
         <f>$F$40*B10</f>
-        <v>300948.26328000001</v>
+        <v>238220.33627999999</v>
       </c>
       <c r="D10" s="36">
         <f>$D$2*B10</f>
-        <v>133558.45180500002</v>
+        <v>102551.04580500002</v>
       </c>
       <c r="E10" s="26">
         <f>E11+E12+E13+E15+E14</f>
@@ -4984,11 +4984,11 @@
       </c>
       <c r="F10" s="44">
         <f>E10/D10</f>
-        <v>0.47190978293176383</v>
+        <v>0.61459675525734137</v>
       </c>
       <c r="G10" s="36">
         <f>$G$2*B10</f>
-        <v>167389.81147499997</v>
+        <v>135669.29047499999</v>
       </c>
       <c r="H10" s="26">
         <f>H11+H12+H13+H15+H14</f>
@@ -4996,7 +4996,7 @@
       </c>
       <c r="I10" s="44">
         <f>H10/G10</f>
-        <v>0.40954428107614321</v>
+        <v>0.50529887611251634</v>
       </c>
       <c r="J10" s="53">
         <f>E10+H10</f>
@@ -5004,7 +5004,7 @@
       </c>
       <c r="K10" s="45">
         <f>J10/C10</f>
-        <v>0.43722159605080679</v>
+        <v>0.55235032430372333</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -5016,11 +5016,11 @@
       </c>
       <c r="C11" s="27">
         <f>$C$10*B11</f>
-        <v>135426.71847600001</v>
+        <v>107199.15132599999</v>
       </c>
       <c r="D11" s="37">
         <f t="shared" ref="D11:D15" si="9">$D$10*B11</f>
-        <v>60101.303312250013</v>
+        <v>46147.970612250007</v>
       </c>
       <c r="E11" s="27">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"CSNDX")</f>
@@ -5028,11 +5028,11 @@
       </c>
       <c r="F11" s="45">
         <f>E11/D11</f>
-        <v>0.36708022595415601</v>
+        <v>0.47807086004652238</v>
       </c>
       <c r="G11" s="37">
         <f t="shared" ref="G11:G15" si="10">$G$10*B11</f>
-        <v>75325.415163749989</v>
+        <v>61051.180713749993</v>
       </c>
       <c r="H11" s="27">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"CSNDX")</f>
@@ -5040,7 +5040,7 @@
       </c>
       <c r="I11" s="45">
         <f>H11/G11</f>
-        <v>0.29288919220742954</v>
+        <v>0.36136893246081281</v>
       </c>
       <c r="J11" s="54">
         <f t="shared" si="0"/>
@@ -5048,7 +5048,7 @@
       </c>
       <c r="K11" s="45">
         <f t="shared" si="1"/>
-        <v>0.3258145844227891</v>
+        <v>0.4116077362013425</v>
       </c>
       <c r="L11" s="14"/>
     </row>
@@ -5061,11 +5061,11 @@
       </c>
       <c r="C12" s="27">
         <f>$C$10*B12</f>
-        <v>60189.652656000006</v>
+        <v>47644.067256000002</v>
       </c>
       <c r="D12" s="37">
         <f t="shared" si="9"/>
-        <v>26711.690361000004</v>
+        <v>20510.209161000006</v>
       </c>
       <c r="E12" s="27">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"CTEC")</f>
@@ -5073,11 +5073,11 @@
       </c>
       <c r="F12" s="45">
         <f t="shared" ref="F12:F15" si="11">E12/D12</f>
-        <v>0.41375142683355987</v>
+        <v>0.53885359789578779</v>
       </c>
       <c r="G12" s="37">
         <f t="shared" si="10"/>
-        <v>33477.962294999998</v>
+        <v>27133.858095</v>
       </c>
       <c r="H12" s="27">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"CTEC")</f>
@@ -5085,7 +5085,7 @@
       </c>
       <c r="I12" s="45">
         <f t="shared" ref="I12:I15" si="12">H12/G12</f>
-        <v>0.49519142933248234</v>
+        <v>0.6109709847364041</v>
       </c>
       <c r="J12" s="54">
         <f t="shared" si="0"/>
@@ -5093,7 +5093,7 @@
       </c>
       <c r="K12" s="45">
         <f t="shared" si="1"/>
-        <v>0.45904900229135487</v>
+        <v>0.57992530007018761</v>
       </c>
       <c r="L12" s="14"/>
     </row>
@@ -5106,11 +5106,11 @@
       </c>
       <c r="C13" s="27">
         <f>$C$10*B13</f>
-        <v>30094.826328000003</v>
+        <v>23822.033628000001</v>
       </c>
       <c r="D13" s="37">
         <f t="shared" si="9"/>
-        <v>13355.845180500002</v>
+        <v>10255.104580500003</v>
       </c>
       <c r="E13" s="27">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"HEAL")</f>
@@ -5118,11 +5118,11 @@
       </c>
       <c r="F13" s="45">
         <f t="shared" si="11"/>
-        <v>0.71092468291434152</v>
+        <v>0.92588036771996107</v>
       </c>
       <c r="G13" s="37">
         <f t="shared" si="10"/>
-        <v>16738.981147499999</v>
+        <v>13566.9290475</v>
       </c>
       <c r="H13" s="27">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"HEAL")</f>
@@ -5130,7 +5130,7 @@
       </c>
       <c r="I13" s="45">
         <f t="shared" si="12"/>
-        <v>0.567238825131128</v>
+        <v>0.69986361443746614</v>
       </c>
       <c r="J13" s="54">
         <f t="shared" si="0"/>
@@ -5138,7 +5138,7 @@
       </c>
       <c r="K13" s="45">
         <f t="shared" si="1"/>
-        <v>0.63100546894772558</v>
+        <v>0.79716116165999729</v>
       </c>
       <c r="L13" s="14"/>
     </row>
@@ -5151,11 +5151,11 @@
       </c>
       <c r="C14" s="27">
         <f>$C$10*B14</f>
-        <v>30094.826328000003</v>
+        <v>23822.033628000001</v>
       </c>
       <c r="D14" s="37">
         <f>$D$10*B14</f>
-        <v>13355.845180500002</v>
+        <v>10255.104580500003</v>
       </c>
       <c r="E14" s="27">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"INRA")</f>
@@ -5163,11 +5163,11 @@
       </c>
       <c r="F14" s="45">
         <f>E14/D14</f>
-        <v>0.77857596127141626</v>
+        <v>1.0139867339600552</v>
       </c>
       <c r="G14" s="37">
         <f>$G$10*B14</f>
-        <v>16738.981147499999</v>
+        <v>13566.9290475</v>
       </c>
       <c r="H14" s="27">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"INRA")</f>
@@ -5175,7 +5175,7 @@
       </c>
       <c r="I14" s="45">
         <f>H14/G14</f>
-        <v>0.62121702081927754</v>
+        <v>0.7664623264110132</v>
       </c>
       <c r="J14" s="54">
         <f>E14+H14</f>
@@ -5183,7 +5183,7 @@
       </c>
       <c r="K14" s="45">
         <f>J14/C14</f>
-        <v>0.69105167025504821</v>
+        <v>0.87301866518883087</v>
       </c>
       <c r="L14" s="14"/>
     </row>
@@ -5196,11 +5196,11 @@
       </c>
       <c r="C15" s="27">
         <f>$C$10*B15</f>
-        <v>45142.239492000001</v>
+        <v>35733.050442</v>
       </c>
       <c r="D15" s="37">
         <f t="shared" si="9"/>
-        <v>20033.767770750001</v>
+        <v>15382.656870750001</v>
       </c>
       <c r="E15" s="27">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"LOCK")</f>
@@ -5208,11 +5208,11 @@
       </c>
       <c r="F15" s="45">
         <f t="shared" si="11"/>
-        <v>0.5001555431140392</v>
+        <v>0.65138292326164737</v>
       </c>
       <c r="G15" s="37">
         <f t="shared" si="10"/>
-        <v>25108.471721249993</v>
+        <v>20350.393571249999</v>
       </c>
       <c r="H15" s="27">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"LOCK")</f>
@@ -5220,7 +5220,7 @@
       </c>
       <c r="I15" s="45">
         <f t="shared" si="12"/>
-        <v>0.39906849414175205</v>
+        <v>0.49237376982014475</v>
       </c>
       <c r="J15" s="54">
         <f t="shared" si="0"/>
@@ -5228,7 +5228,7 @@
       </c>
       <c r="K15" s="45">
         <f t="shared" si="1"/>
-        <v>0.44393012454668851</v>
+        <v>0.56082533542799173</v>
       </c>
       <c r="L15" s="14"/>
     </row>
@@ -5241,11 +5241,11 @@
       </c>
       <c r="C16" s="26">
         <f>$F$40*B16</f>
-        <v>250790.2194</v>
+        <v>198516.94690000001</v>
       </c>
       <c r="D16" s="36">
         <f>$D$2*B16</f>
-        <v>111298.70983750002</v>
+        <v>85459.204837500016</v>
       </c>
       <c r="E16" s="26" cm="1">
         <f t="array" ref="E16">SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,IncomeStrategy!A:A))</f>
@@ -5253,11 +5253,11 @@
       </c>
       <c r="F16" s="44">
         <f>E16/D16</f>
-        <v>1.0059325949372102</v>
+        <v>1.3100870785410317</v>
       </c>
       <c r="G16" s="36">
         <f>$G$2*B16</f>
-        <v>139491.50956249997</v>
+        <v>113057.74206249999</v>
       </c>
       <c r="H16" s="26" cm="1">
         <f t="array" ref="H16">SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,IncomeStrategy!A:A))</f>
@@ -5265,7 +5265,7 @@
       </c>
       <c r="I16" s="44">
         <f t="shared" ref="I16:I21" si="13">H16/G16</f>
-        <v>0.44852192220321047</v>
+        <v>0.55338978878079081</v>
       </c>
       <c r="J16" s="53">
         <f t="shared" si="0"/>
@@ -5273,7 +5273,7 @@
       </c>
       <c r="K16" s="44">
         <f t="shared" si="1"/>
-        <v>0.69589635679388862</v>
+        <v>0.87913904946318711</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -5285,11 +5285,11 @@
       </c>
       <c r="C17" s="26">
         <f>$F$40*B17</f>
-        <v>50158.043880000005</v>
+        <v>39703.389380000008</v>
       </c>
       <c r="D17" s="36">
         <f>$D$2*B17</f>
-        <v>22259.741967500006</v>
+        <v>17091.840967500004</v>
       </c>
       <c r="E17" s="26">
         <f>E18+E19</f>
@@ -5297,11 +5297,11 @@
       </c>
       <c r="F17" s="44">
         <f>E17/D17</f>
-        <v>1.1010883250931383</v>
+        <v>1.4340141618802487</v>
       </c>
       <c r="G17" s="36">
         <f>$G$2*B17</f>
-        <v>27898.301912499996</v>
+        <v>22611.5484125</v>
       </c>
       <c r="H17" s="26">
         <f>H18+H19</f>
@@ -5309,7 +5309,7 @@
       </c>
       <c r="I17" s="44">
         <f>H17/G17</f>
-        <v>0.55474529053919386</v>
+        <v>0.68444899560457984</v>
       </c>
       <c r="J17" s="53">
         <f>E17+H17</f>
@@ -5317,7 +5317,7 @@
       </c>
       <c r="K17" s="44">
         <f t="shared" si="1"/>
-        <v>0.79720799510572882</v>
+        <v>1.007127961224956</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -5329,11 +5329,11 @@
       </c>
       <c r="C18" s="28">
         <f>$C$17*B18</f>
-        <v>25079.021940000002</v>
+        <v>19851.694690000004</v>
       </c>
       <c r="D18" s="38">
         <f>$D$17*B18</f>
-        <v>11129.870983750003</v>
+        <v>8545.9204837500019</v>
       </c>
       <c r="E18" s="28" cm="1">
         <f t="array" ref="E18">SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK")-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,GlobalETF!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,GrowthEngine!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,IncomeStrategy!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,Gold!A:A))</f>
@@ -5341,11 +5341,11 @@
       </c>
       <c r="F18" s="46">
         <f t="shared" ref="F18:F21" si="14">E18/G18</f>
-        <v>1.4458358120329571</v>
+        <v>1.7838833176812203</v>
       </c>
       <c r="G18" s="38">
         <f>$G$17*B18</f>
-        <v>13949.150956249998</v>
+        <v>11305.77420625</v>
       </c>
       <c r="H18" s="28" cm="1">
         <f t="array" ref="H18">SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK")-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,GlobalETF!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,GrowthEngine!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,IncomeStrategy!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,Gold!A:A))</f>
@@ -5353,7 +5353,7 @@
       </c>
       <c r="I18" s="46">
         <f>H18/G18</f>
-        <v>1.064039786116854</v>
+        <v>1.3128204516763504</v>
       </c>
       <c r="J18" s="55">
         <f t="shared" si="0"/>
@@ -5361,7 +5361,7 @@
       </c>
       <c r="K18" s="46">
         <f t="shared" si="1"/>
-        <v>1.3960127186682452</v>
+        <v>1.7636093112814222</v>
       </c>
       <c r="L18" s="15"/>
     </row>
@@ -5374,11 +5374,11 @@
       </c>
       <c r="C19" s="28">
         <f>$C$17*B19</f>
-        <v>25079.021940000002</v>
+        <v>19851.694690000004</v>
       </c>
       <c r="D19" s="38">
         <f>$D$17*B19</f>
-        <v>11129.870983750003</v>
+        <v>8545.9204837500019</v>
       </c>
       <c r="E19" s="28">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"OPT",[1]PositionsHK!T:T,"Long")+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"FOP",[1]PositionsHK!T:T,"Long")</f>
@@ -5386,11 +5386,11 @@
       </c>
       <c r="F19" s="46">
         <f t="shared" si="14"/>
-        <v>0.31125622008231618</v>
+        <v>0.38403031236903801</v>
       </c>
       <c r="G19" s="38">
         <f>$G$17*B19</f>
-        <v>13949.150956249998</v>
+        <v>11305.77420625</v>
       </c>
       <c r="H19" s="28">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"OPT",[1]PositionsAL!T:T,"Long")+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"FOP",[1]PositionsAL!T:T,"Long")</f>
@@ -5398,7 +5398,7 @@
       </c>
       <c r="I19" s="46">
         <f>H19/G19</f>
-        <v>4.5450794961533675E-2</v>
+        <v>5.6077539532809292E-2</v>
       </c>
       <c r="J19" s="55">
         <f t="shared" si="0"/>
@@ -5406,7 +5406,7 @@
       </c>
       <c r="K19" s="46">
         <f t="shared" si="1"/>
-        <v>0.19840327154321233</v>
+        <v>0.25064661116848957</v>
       </c>
       <c r="L19" s="15"/>
     </row>
@@ -5419,11 +5419,11 @@
       </c>
       <c r="C20" s="26">
         <f>$F$40*B20</f>
-        <v>30094.826327999999</v>
+        <v>23822.033628000001</v>
       </c>
       <c r="D20" s="36">
         <f>$D$2*B20</f>
-        <v>13355.845180500002</v>
+        <v>10255.104580500001</v>
       </c>
       <c r="E20" s="26">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"GSD")</f>
@@ -5431,11 +5431,11 @@
       </c>
       <c r="F20" s="44">
         <f t="shared" si="14"/>
-        <v>1.3561898451262957</v>
+        <v>1.6732774359266807</v>
       </c>
       <c r="G20" s="36">
         <f>$G$2*B20</f>
-        <v>16738.981147499995</v>
+        <v>13566.929047499998</v>
       </c>
       <c r="H20" s="26">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"GSD")</f>
@@ -5443,7 +5443,7 @@
       </c>
       <c r="I20" s="44">
         <f t="shared" si="13"/>
-        <v>0.27123796902525915</v>
+        <v>0.33465548718533616</v>
       </c>
       <c r="J20" s="53">
         <f t="shared" si="0"/>
@@ -5451,7 +5451,7 @@
       </c>
       <c r="K20" s="44">
         <f t="shared" si="1"/>
-        <v>0.9051882607029611</v>
+        <v>1.1435414761559584</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -5463,39 +5463,39 @@
       </c>
       <c r="C21" s="26">
         <f>$F$40*B21</f>
-        <v>70221.261432000014</v>
+        <v>55584.745132000011</v>
       </c>
       <c r="D21" s="39">
         <f>$D$2*B21</f>
-        <v>31163.638754500007</v>
+        <v>23928.577354500008</v>
       </c>
       <c r="E21" s="40" t="str">
         <f>[1]Summary!$C$2</f>
-        <v>$103,358.02</v>
+        <v>$0.00</v>
       </c>
       <c r="F21" s="47">
         <f t="shared" si="14"/>
-        <v>2.6462957270448944</v>
+        <v>0</v>
       </c>
       <c r="G21" s="39">
         <f>$G$2*B21</f>
-        <v>39057.622677499996</v>
+        <v>31656.167777500003</v>
       </c>
       <c r="H21" s="40" t="str">
         <f>[1]Summary!$C$3</f>
-        <v>$105,735.07</v>
+        <v>$0.00</v>
       </c>
       <c r="I21" s="47">
         <f t="shared" si="13"/>
-        <v>2.7071558060012451</v>
+        <v>0</v>
       </c>
       <c r="J21" s="56">
         <f t="shared" si="0"/>
-        <v>209093.09000000003</v>
+        <v>0</v>
       </c>
       <c r="K21" s="47">
         <f t="shared" si="1"/>
-        <v>2.9776322118975171</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -5530,7 +5530,7 @@
     <row r="40" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F40" s="24">
         <f>D2+G2</f>
-        <v>1003160.8776</v>
+        <v>794067.78760000004</v>
       </c>
       <c r="G40" s="19"/>
     </row>
@@ -5540,13 +5540,13 @@
       </c>
       <c r="G41" s="25">
         <f>F42/F40</f>
-        <v>0.79156574516717371</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F42" s="24">
         <f>F40-F44</f>
-        <v>794067.78759999992</v>
+        <v>794067.78760000004</v>
       </c>
       <c r="G42" s="19"/>
     </row>
@@ -5556,13 +5556,13 @@
       </c>
       <c r="G43" s="25">
         <f>F44/F40</f>
-        <v>0.20843425483282627</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F44" s="24">
         <f>E21+H21</f>
-        <v>209093.09000000003</v>
+        <v>0</v>
       </c>
       <c r="G44" s="19"/>
     </row>
@@ -5584,7 +5584,7 @@
       </c>
       <c r="B50" s="21">
         <f>C4</f>
-        <v>300948.26328000001</v>
+        <v>238220.33627999999</v>
       </c>
       <c r="C50" s="22">
         <f>J4</f>
@@ -5600,7 +5600,7 @@
       </c>
       <c r="B51" s="21">
         <f>C10</f>
-        <v>300948.26328000001</v>
+        <v>238220.33627999999</v>
       </c>
       <c r="C51" s="22">
         <f>J10</f>
@@ -5616,7 +5616,7 @@
       </c>
       <c r="B52" s="21">
         <f>C16</f>
-        <v>250790.2194</v>
+        <v>198516.94690000001</v>
       </c>
       <c r="C52" s="22">
         <f>J16</f>
@@ -5632,7 +5632,7 @@
       </c>
       <c r="B53" s="21">
         <f>C18</f>
-        <v>25079.021940000002</v>
+        <v>19851.694690000004</v>
       </c>
       <c r="C53" s="22">
         <f>J18</f>
@@ -5648,7 +5648,7 @@
       </c>
       <c r="B54" s="21">
         <f>C19</f>
-        <v>25079.021940000002</v>
+        <v>19851.694690000004</v>
       </c>
       <c r="C54" s="22">
         <f>J19</f>
@@ -5664,7 +5664,7 @@
       </c>
       <c r="B55" s="21">
         <f>C20</f>
-        <v>30094.826327999999</v>
+        <v>23822.033628000001</v>
       </c>
       <c r="C55" s="22">
         <f>J20</f>
@@ -5680,11 +5680,11 @@
       </c>
       <c r="B56" s="21">
         <f>C21</f>
-        <v>70221.261432000014</v>
+        <v>55584.745132000011</v>
       </c>
       <c r="C56" s="22">
         <f>J21</f>
-        <v>209093.09000000003</v>
+        <v>0</v>
       </c>
       <c r="D56" s="23"/>
       <c r="E56" s="23"/>
@@ -6080,11 +6080,11 @@
       </c>
       <c r="J2" s="6">
         <f>Dashboard!$D$10*GrowthEngine!I2</f>
-        <v>53423.380722000009</v>
+        <v>41020.418322000012</v>
       </c>
       <c r="K2" s="6">
         <f>Dashboard!$G$10*GrowthEngine!I2</f>
-        <v>66955.924589999995</v>
+        <v>54267.716189999999</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -6117,11 +6117,11 @@
       </c>
       <c r="J3" s="6">
         <f>Dashboard!$D$10*GrowthEngine!I3</f>
-        <v>26711.690361000004</v>
+        <v>20510.209161000006</v>
       </c>
       <c r="K3" s="6">
         <f>Dashboard!$G$10*GrowthEngine!I3</f>
-        <v>33477.962294999998</v>
+        <v>27133.858095</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -6154,11 +6154,11 @@
       </c>
       <c r="J4" s="6">
         <f>Dashboard!$D$10*GrowthEngine!I4</f>
-        <v>20033.767770750001</v>
+        <v>15382.656870750001</v>
       </c>
       <c r="K4" s="6">
         <f>Dashboard!$G$10*GrowthEngine!I4</f>
-        <v>25108.471721249993</v>
+        <v>20350.393571249999</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -6191,11 +6191,11 @@
       </c>
       <c r="J5" s="6">
         <f>Dashboard!$D$10*GrowthEngine!I5</f>
-        <v>13355.845180500002</v>
+        <v>10255.104580500003</v>
       </c>
       <c r="K5" s="6">
         <f>Dashboard!$G$10*GrowthEngine!I5</f>
-        <v>16738.981147499999</v>
+        <v>13566.9290475</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -6228,11 +6228,11 @@
       </c>
       <c r="J6" s="6">
         <f>Dashboard!$D$10*GrowthEngine!I6</f>
-        <v>20033.767770750001</v>
+        <v>15382.656870750001</v>
       </c>
       <c r="K6" s="6">
         <f>Dashboard!$G$10*GrowthEngine!I6</f>
-        <v>25108.471721249993</v>
+        <v>20350.393571249999</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
change to new local workspace
</commit_message>
<xml_diff>
--- a/projects/fetch-ibkr-positions-dashboard.xlsx
+++ b/projects/fetch-ibkr-positions-dashboard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hongkiatkoh/Desktop/timeless-workspace/timeless-workspace/projects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hongkiatkoh/Developer/timeless-workspace/projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BC4395-0C6C-7341-BC3A-F2580D79D838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEAD97AC-57A8-644F-8DA1-B3ADB665D962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14300" yWindow="1480" windowWidth="32100" windowHeight="25120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3300" yWindow="1720" windowWidth="32620" windowHeight="25120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -165,7 +165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="F21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -218,7 +218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -268,7 +268,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="199">
   <si>
     <t>HK</t>
   </si>
@@ -288,12 +288,6 @@
     <t>Target</t>
   </si>
   <si>
-    <t>Actual HK</t>
-  </si>
-  <si>
-    <t>Actual AL</t>
-  </si>
-  <si>
     <t>Actual Total</t>
   </si>
   <si>
@@ -303,105 +297,39 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>Digital: 100 US Tech giants. Your core foundation.</t>
-  </si>
-  <si>
-    <t>Manufacturing: 150+ China Hard Tech &amp; AI leaders.</t>
-  </si>
-  <si>
-    <t>Biotic: Global Genomics &amp; Med-Tech Innovation.</t>
-  </si>
-  <si>
     <t>Security (LOCK)</t>
   </si>
   <si>
-    <t>Security: Cyberdefense &amp; Data Infrastructure.</t>
-  </si>
-  <si>
     <t>Energy (INRA)</t>
   </si>
   <si>
-    <t>Energy: Clean energy utilities powering AI data centers.</t>
-  </si>
-  <si>
     <t>Ticker</t>
   </si>
   <si>
-    <t>Weight</t>
-  </si>
-  <si>
-    <t>Trading Currency</t>
-  </si>
-  <si>
-    <t>Focus / Sector</t>
-  </si>
-  <si>
-    <t>Exp. Ratio (TER)</t>
-  </si>
-  <si>
-    <t>2026 Strategy Profile</t>
-  </si>
-  <si>
     <t>CNY</t>
   </si>
   <si>
-    <t>China Blue-Chips</t>
-  </si>
-  <si>
-    <t>The Value Hedge. Direct exposure to mainland Yuan &amp; economy.</t>
-  </si>
-  <si>
     <t>DHL</t>
   </si>
   <si>
     <t>EUR</t>
   </si>
   <si>
-    <t>Logistics (Stock)</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Physical Value. Industrial exposure with a strong Euro-yield.</t>
-  </si>
-  <si>
     <t>ES3</t>
   </si>
   <si>
     <t>SGD</t>
   </si>
   <si>
-    <t>Singapore Index</t>
-  </si>
-  <si>
-    <t>Income Anchor. Reliable ~3.7% yield in stable SGD.</t>
-  </si>
-  <si>
     <t>VWRA</t>
   </si>
   <si>
     <t>USD</t>
   </si>
   <si>
-    <t>Global Core (Acc)</t>
-  </si>
-  <si>
-    <t>USD Liquidity. Identical to VWCE; used for flexible USD entry.</t>
-  </si>
-  <si>
-    <t>VWCE</t>
-  </si>
-  <si>
-    <t>Primary Anchor. Captures world growth with a Euro-base.</t>
-  </si>
-  <si>
     <t>Primary Exchange</t>
   </si>
   <si>
-    <t>Manager</t>
-  </si>
-  <si>
     <t>AUM (USD)</t>
   </si>
   <si>
@@ -411,72 +339,21 @@
     <t>2025 Return</t>
   </si>
   <si>
-    <t>Top 1 Holding</t>
-  </si>
-  <si>
     <t>Strategy Profile</t>
   </si>
   <si>
-    <t>Allocation</t>
-  </si>
-  <si>
     <t>CSNDX</t>
   </si>
   <si>
-    <t>SIX (Swiss)</t>
-  </si>
-  <si>
-    <t>iShares</t>
-  </si>
-  <si>
-    <t>~$23.7 Billion</t>
-  </si>
-  <si>
-    <t>NVIDIA</t>
-  </si>
-  <si>
-    <t>CTEC</t>
-  </si>
-  <si>
-    <t>~$2.4 Billion</t>
-  </si>
-  <si>
-    <t>NetEase</t>
-  </si>
-  <si>
     <t>HEAL</t>
   </si>
   <si>
-    <t>LSE</t>
-  </si>
-  <si>
-    <t>~$1.1 Billion</t>
-  </si>
-  <si>
-    <t>Illumina</t>
-  </si>
-  <si>
     <t>INRA</t>
   </si>
   <si>
-    <t>AEB</t>
-  </si>
-  <si>
-    <t>~$3.2 Billion</t>
-  </si>
-  <si>
-    <t>Bloom Energy</t>
-  </si>
-  <si>
     <t>LOCK</t>
   </si>
   <si>
-    <t>~$1.8 Billion</t>
-  </si>
-  <si>
-    <t>Ciena Corp</t>
-  </si>
-  <si>
     <t>Best For</t>
   </si>
   <si>
@@ -765,15 +642,6 @@
     <t>update github actions</t>
   </si>
   <si>
-    <t>Reserve: Cash</t>
-  </si>
-  <si>
-    <t>The Sniper (theme stocks)</t>
-  </si>
-  <si>
-    <t>Reserve: Gold</t>
-  </si>
-  <si>
     <t>Biotic (HEAL)</t>
   </si>
   <si>
@@ -807,9 +675,6 @@
     <t xml:space="preserve">Actual % </t>
   </si>
   <si>
-    <t>Global Traids (The strategic core)</t>
-  </si>
-  <si>
     <t>Currency</t>
   </si>
   <si>
@@ -831,19 +696,175 @@
     <t>Energy (GRID)</t>
   </si>
   <si>
-    <t>Cash Cow (The Income Strategy)</t>
-  </si>
-  <si>
-    <t>Four Horsemen (The growth engine)</t>
-  </si>
-  <si>
-    <t>The Hedge (bear spreads 4xQQQ, 4xSPY)</t>
-  </si>
-  <si>
     <t>China Tech (CBUK, unhedged)</t>
   </si>
   <si>
-    <t>Alpha &amp; Omega (The circuit breaker)</t>
+    <t>Global Triads (the strategic core)</t>
+  </si>
+  <si>
+    <t>Four Horsemen (growth engine)</t>
+  </si>
+  <si>
+    <t>Cash Cow (income Strategy)</t>
+  </si>
+  <si>
+    <t>The Alpha (theme, buy calls)</t>
+  </si>
+  <si>
+    <t>The Omega (insurance, bear spreads)</t>
+  </si>
+  <si>
+    <t>The Vault (Gold)</t>
+  </si>
+  <si>
+    <t>The War Chest (Cash)</t>
+  </si>
+  <si>
+    <t>WORLD</t>
+  </si>
+  <si>
+    <t>XMME</t>
+  </si>
+  <si>
+    <t>Focus and Sector</t>
+  </si>
+  <si>
+    <t>Expense Ratio</t>
+  </si>
+  <si>
+    <t>Investment Strategy Profile</t>
+  </si>
+  <si>
+    <t>AUM</t>
+  </si>
+  <si>
+    <t>1 Year Returns</t>
+  </si>
+  <si>
+    <t>China Large &amp; Mid-Cap Equities (CSI 300 Index tracking top 300 stocks from Shanghai and Shenzhen exchanges)</t>
+  </si>
+  <si>
+    <t>Passive index replication via representative sampling. Tracks CSI 300 (300 largest A-shares). Hong Kong-listed, CNY counter (also available as 2846 HKD, 9846 USD)</t>
+  </si>
+  <si>
+    <t>~CNY 1.45B</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Stock ticker for Deutsche Post/DHL Group - integrated freight &amp; logistics company. Market cap ~€54B. Dividend yield ~4.5%</t>
+  </si>
+  <si>
+    <t>+29.64%</t>
+  </si>
+  <si>
+    <t>Singapore Blue-Chip Equities (Straits Times Index tracking top 30 Singapore companies including DBS, OCBC, UOB)</t>
+  </si>
+  <si>
+    <t>0.30%</t>
+  </si>
+  <si>
+    <t>Passive index tracking via representative sampling. Tracks STI (top 30 SGX blue-chips). Semi-annual dividend distribution. Low-cost Singapore market exposure</t>
+  </si>
+  <si>
+    <t>~SGD 2.4B</t>
+  </si>
+  <si>
+    <t>+34.03%</t>
+  </si>
+  <si>
+    <t>Global All-World Equities (Developed + Emerging Markets, ~3,900 holdings across 50 countries, 95% of global investable market cap)</t>
+  </si>
+  <si>
+    <t>0.19%</t>
+  </si>
+  <si>
+    <t>Passive full replication of FTSE All-World. Accumulating (reinvests dividends). Ireland-domiciled UCITS. Covers developed (90%) + emerging (10%) markets globally</t>
+  </si>
+  <si>
+    <t>~USD 51.5B</t>
+  </si>
+  <si>
+    <t>+22.49%</t>
+  </si>
+  <si>
+    <t>Developed Markets Equities (MSCI World Index, CHF-hedged, Large &amp; Mid-Cap stocks from 23 developed countries)</t>
+  </si>
+  <si>
+    <t>0.55%</t>
+  </si>
+  <si>
+    <t>Currency-hedged to CHF. Passive sampling methodology tracking MSCI World. Accumulating share class. Suitable for CHF-based investors seeking developed market exposure without FX risk</t>
+  </si>
+  <si>
+    <t>~CHF 981M</t>
+  </si>
+  <si>
+    <t>+13.29%</t>
+  </si>
+  <si>
+    <t>Emerging Markets Equities (MSCI Emerging Markets Index tracking large &amp; mid-cap stocks from 24 emerging market countries)</t>
+  </si>
+  <si>
+    <t>0.18%</t>
+  </si>
+  <si>
+    <t>Passive replication of MSCI EM Index. Accumulating share class. Covers 24 emerging markets with China (28%), Taiwan (21%), India (15%) as top country weights</t>
+  </si>
+  <si>
+    <t>~CHF 7.85B</t>
+  </si>
+  <si>
+    <t>+14.72%</t>
+  </si>
+  <si>
+    <t>Deutsche Post AG - logistics/freight)</t>
+  </si>
+  <si>
+    <t>EQCH</t>
+  </si>
+  <si>
+    <t>CBUK</t>
+  </si>
+  <si>
+    <t>GRID</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Swiss</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>1.1b</t>
+  </si>
+  <si>
+    <t>2.1b</t>
+  </si>
+  <si>
+    <t>600m</t>
+  </si>
+  <si>
+    <t>22.5b</t>
+  </si>
+  <si>
+    <t>686m</t>
+  </si>
+  <si>
+    <t>1.0b</t>
+  </si>
+  <si>
+    <t>1.6b</t>
   </si>
 </sst>
 </file>
@@ -857,7 +878,7 @@
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -955,6 +976,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1083,15 +1115,11 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1149,9 +1177,8 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -1160,6 +1187,22 @@
     <xf numFmtId="165" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -1167,21 +1210,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="40">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFD78"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <fill>
         <patternFill>
@@ -1406,48 +1435,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7E79"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7E79"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFD78"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7E79"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7E79"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1494,7 +1481,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dashboard!$B$52</c:f>
+              <c:f>Dashboard!$B$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1573,59 +1560,59 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Dashboard!$A$53:$A$59</c:f>
+              <c:f>Dashboard!$A$52:$A$58</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Global Traids (The strategic core)</c:v>
+                  <c:v>Global Triads (the strategic core)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Four Horsemen (The growth engine)</c:v>
+                  <c:v>Four Horsemen (growth engine)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Cash Cow (The Income Strategy)</c:v>
+                  <c:v>Cash Cow (income Strategy)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>The Sniper (theme stocks)</c:v>
+                  <c:v>The Alpha (theme, buy calls)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>The Hedge (bear spreads 4xQQQ, 4xSPY)</c:v>
+                  <c:v>The Omega (insurance, bear spreads)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Reserve: Gold</c:v>
+                  <c:v>The Vault (Gold)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Reserve: Cash</c:v>
+                  <c:v>The War Chest (Cash)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Dashboard!$B$53:$B$59</c:f>
+              <c:f>Dashboard!$B$52:$B$58</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>311419.48346999998</c:v>
+                  <c:v>283773.76941000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>311419.48346999998</c:v>
+                  <c:v>283773.76941000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>259516.23622499997</c:v>
+                  <c:v>236478.141175</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25951.623622499999</c:v>
+                  <c:v>23647.814117500002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25951.623622499999</c:v>
+                  <c:v>23647.814117500002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51903.247244999999</c:v>
+                  <c:v>47295.628235000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>51903.247244999999</c:v>
+                  <c:v>47295.628235000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1641,7 +1628,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dashboard!$C$52</c:f>
+              <c:f>Dashboard!$C$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1720,41 +1707,41 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Dashboard!$A$53:$A$59</c:f>
+              <c:f>Dashboard!$A$52:$A$58</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Global Traids (The strategic core)</c:v>
+                  <c:v>Global Triads (the strategic core)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Four Horsemen (The growth engine)</c:v>
+                  <c:v>Four Horsemen (growth engine)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Cash Cow (The Income Strategy)</c:v>
+                  <c:v>Cash Cow (income Strategy)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>The Sniper (theme stocks)</c:v>
+                  <c:v>The Alpha (theme, buy calls)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>The Hedge (bear spreads 4xQQQ, 4xSPY)</c:v>
+                  <c:v>The Omega (insurance, bear spreads)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Reserve: Gold</c:v>
+                  <c:v>The Vault (Gold)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Reserve: Cash</c:v>
+                  <c:v>The War Chest (Cash)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Dashboard!$C$53:$C$59</c:f>
+              <c:f>Dashboard!$C$52:$C$58</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>221311.57490000001</c:v>
+                  <c:v>296687.19050000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>158901.74780000001</c:v>
@@ -1763,7 +1750,7 @@
                   <c:v>153695</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>179024.47579999996</c:v>
+                  <c:v>11496.47999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>18733.440000000002</c:v>
@@ -2186,7 +2173,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>(Dashboard!$G$44,Dashboard!$G$46)</c:f>
+              <c:f>(Dashboard!$G$43,Dashboard!$G$45)</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -2200,15 +2187,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Dashboard!$H$44,Dashboard!$H$46)</c:f>
+              <c:f>(Dashboard!$H$43,Dashboard!$H$45)</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.71751546814034017</c:v>
+                  <c:v>0.68999535375343979</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.28248453185965983</c:v>
+                  <c:v>0.31000464624656027</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3388,13 +3375,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1219200</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3424,13 +3411,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4619,10 +4606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M59"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="38.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4642,1414 +4629,1341 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="44"/>
-      <c r="B1" s="53"/>
-      <c r="E1" s="29" t="s">
+      <c r="A1" s="42"/>
+      <c r="E1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="29" t="s">
+      <c r="G1" s="35"/>
+      <c r="H1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="37"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="37"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="35"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="12">
+      <c r="C2" s="10">
         <v>1</v>
       </c>
-      <c r="E2" s="30">
-        <f>F4+F11+F19+F23+F24+F21-F22</f>
-        <v>460776.63520000002</v>
-      </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="30">
-        <f>I4+I11+I19+I23+I24+I21-I22</f>
-        <v>577288.30969999987</v>
-      </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="37"/>
+      <c r="E2" s="28">
+        <f>F4+F11+F19+F22+F23+F20-F21</f>
+        <v>417382.99219999998</v>
+      </c>
+      <c r="F2" s="29"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="28">
+        <f>I4+I11+I19+I22+I23+I20-I21</f>
+        <v>528529.57250000001</v>
+      </c>
+      <c r="I2" s="29"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="35"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="54" t="s">
-        <v>180</v>
-      </c>
-      <c r="C3" s="18" t="s">
+      <c r="B3" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="G3" s="39" t="s">
-        <v>178</v>
-      </c>
-      <c r="H3" s="32" t="s">
+      <c r="F3" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="J3" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="32" t="s">
+      <c r="I3" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="J3" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56">
+      <c r="A4" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="52"/>
+      <c r="C4" s="53">
         <v>0.3</v>
       </c>
-      <c r="D4" s="26">
-        <f>$G$43*C4</f>
-        <v>311419.48346999998</v>
-      </c>
-      <c r="E4" s="33">
+      <c r="D4" s="24">
+        <f>$G$42*C4</f>
+        <v>283773.76941000001</v>
+      </c>
+      <c r="E4" s="31">
         <f>$E$2*C4</f>
-        <v>138232.99056000001</v>
-      </c>
-      <c r="F4" s="26" cm="1">
+        <v>125214.89765999999</v>
+      </c>
+      <c r="F4" s="24" cm="1">
         <f t="array" ref="F4">SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,GlobalETF!A:A))</f>
-        <v>63945.949500000002</v>
-      </c>
-      <c r="G4" s="40">
+        <v>97240.477199999994</v>
+      </c>
+      <c r="G4" s="38">
         <f>F4/E4</f>
-        <v>0.4625954284932024</v>
-      </c>
-      <c r="H4" s="33">
+        <v>0.77658872080892616</v>
+      </c>
+      <c r="H4" s="31">
         <f>$H$2*C4</f>
-        <v>173186.49290999994</v>
-      </c>
-      <c r="I4" s="26" cm="1">
+        <v>158558.87174999999</v>
+      </c>
+      <c r="I4" s="24" cm="1">
         <f t="array" ref="I4">SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,GlobalETF!A:A))</f>
-        <v>157365.62540000002</v>
-      </c>
-      <c r="J4" s="40">
+        <v>199446.71330000003</v>
+      </c>
+      <c r="J4" s="38">
         <f>I4/H4</f>
-        <v>0.90864837526202702</v>
-      </c>
-      <c r="K4" s="49">
-        <f t="shared" ref="K4:K24" si="0">F4+I4</f>
-        <v>221311.57490000001</v>
-      </c>
-      <c r="L4" s="40">
-        <f t="shared" ref="L4:L24" si="1">K4/D4</f>
-        <v>0.71065423535492966</v>
-      </c>
-      <c r="M4" s="17" t="s">
-        <v>169</v>
+        <v>1.2578716731440165</v>
+      </c>
+      <c r="K4" s="47">
+        <f t="shared" ref="K4:K23" si="0">F4+I4</f>
+        <v>296687.19050000003</v>
+      </c>
+      <c r="L4" s="38">
+        <f t="shared" ref="L4:L23" si="1">K4/D4</f>
+        <v>1.045506042073052</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
-        <v>170</v>
-      </c>
-      <c r="B5" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="57">
+      <c r="A5" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="54">
         <v>0.1</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="25">
         <f>$D$4*C5</f>
-        <v>31141.948346999998</v>
-      </c>
-      <c r="E5" s="34">
+        <v>28377.376941000002</v>
+      </c>
+      <c r="E5" s="32">
         <f>$E$4*C5</f>
-        <v>13823.299056000002</v>
-      </c>
-      <c r="F5" s="27">
+        <v>12521.489765999999</v>
+      </c>
+      <c r="F5" s="25">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"82846")</f>
         <v>9192.3216000000011</v>
       </c>
-      <c r="G5" s="41">
+      <c r="G5" s="39">
         <f>F5/E5</f>
-        <v>0.66498753754517625</v>
-      </c>
-      <c r="H5" s="34">
+        <v>0.73412363638711786</v>
+      </c>
+      <c r="H5" s="32">
         <f>$H$4*C5</f>
-        <v>17318.649290999994</v>
-      </c>
-      <c r="I5" s="27">
+        <v>15855.887175</v>
+      </c>
+      <c r="I5" s="25">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"82846")</f>
         <v>9192.3216000000011</v>
       </c>
-      <c r="J5" s="41">
+      <c r="J5" s="39">
         <f>I5/H5</f>
-        <v>0.53077589629215405</v>
-      </c>
-      <c r="K5" s="50">
+        <v>0.57974186486982249</v>
+      </c>
+      <c r="K5" s="48">
         <f t="shared" ref="K5:K7" si="2">F5+I5</f>
         <v>18384.643200000002</v>
       </c>
-      <c r="L5" s="41">
+      <c r="L5" s="39">
         <f t="shared" ref="L5:L7" si="3">K5/D5</f>
-        <v>0.59034980712024243</v>
-      </c>
-      <c r="M5" s="14"/>
+        <v>0.64786267026102862</v>
+      </c>
+      <c r="M5" s="12"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="47" t="s">
-        <v>171</v>
-      </c>
-      <c r="B6" s="55" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="57">
+      <c r="A6" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="54">
         <v>0.2</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="25">
         <f t="shared" ref="D6:D10" si="4">$D$4*C6</f>
-        <v>62283.896693999995</v>
-      </c>
-      <c r="E6" s="34">
+        <v>56754.753882000005</v>
+      </c>
+      <c r="E6" s="32">
         <f t="shared" ref="E6:E10" si="5">$E$4*C6</f>
-        <v>27646.598112000003</v>
-      </c>
-      <c r="F6" s="27">
+        <v>25042.979531999998</v>
+      </c>
+      <c r="F6" s="25">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"DHL")</f>
         <v>0</v>
       </c>
-      <c r="G6" s="41">
+      <c r="G6" s="39">
         <f t="shared" ref="G6:G7" si="6">F6/E6</f>
         <v>0</v>
       </c>
-      <c r="H6" s="34">
+      <c r="H6" s="32">
         <f t="shared" ref="H6:H10" si="7">$H$4*C6</f>
-        <v>34637.298581999989</v>
-      </c>
-      <c r="I6" s="27">
+        <v>31711.77435</v>
+      </c>
+      <c r="I6" s="25">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"DHL")</f>
         <v>56120.048000000003</v>
       </c>
-      <c r="J6" s="41">
+      <c r="J6" s="39">
         <f t="shared" ref="J6:J7" si="8">I6/H6</f>
-        <v>1.6202201181232991</v>
-      </c>
-      <c r="K6" s="50">
+        <v>1.7696911998870857</v>
+      </c>
+      <c r="K6" s="48">
         <f t="shared" si="2"/>
         <v>56120.048000000003</v>
       </c>
-      <c r="L6" s="41">
+      <c r="L6" s="39">
         <f t="shared" si="3"/>
-        <v>0.90103623855965687</v>
-      </c>
-      <c r="M6" s="14"/>
+        <v>0.98881669219604695</v>
+      </c>
+      <c r="M6" s="12"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="47" t="s">
-        <v>172</v>
-      </c>
-      <c r="B7" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="57">
+      <c r="A7" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="54">
         <v>0.2</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="25">
         <f t="shared" si="4"/>
-        <v>62283.896693999995</v>
-      </c>
-      <c r="E7" s="34">
+        <v>56754.753882000005</v>
+      </c>
+      <c r="E7" s="32">
         <f t="shared" si="5"/>
-        <v>27646.598112000003</v>
-      </c>
-      <c r="F7" s="27">
+        <v>25042.979531999998</v>
+      </c>
+      <c r="F7" s="25">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"ES3")</f>
         <v>19845.627899999999</v>
       </c>
-      <c r="G7" s="41">
+      <c r="G7" s="39">
         <f t="shared" si="6"/>
-        <v>0.71783254560299792</v>
-      </c>
-      <c r="H7" s="34">
+        <v>0.79246272891135794</v>
+      </c>
+      <c r="H7" s="32">
         <f t="shared" si="7"/>
-        <v>34637.298581999989</v>
-      </c>
-      <c r="I7" s="27">
+        <v>31711.77435</v>
+      </c>
+      <c r="I7" s="25">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"ES3")</f>
         <v>39691.255799999999</v>
       </c>
-      <c r="J7" s="41">
+      <c r="J7" s="39">
         <f t="shared" si="8"/>
-        <v>1.1459108367251944</v>
-      </c>
-      <c r="K7" s="50">
+        <v>1.2516251964311798</v>
+      </c>
+      <c r="K7" s="48">
         <f t="shared" si="2"/>
         <v>59536.883699999998</v>
       </c>
-      <c r="L7" s="41">
+      <c r="L7" s="39">
         <f t="shared" si="3"/>
-        <v>0.95589529332925272</v>
-      </c>
-      <c r="M7" s="14"/>
+        <v>1.0490202076073554</v>
+      </c>
+      <c r="M7" s="12"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="47" t="s">
-        <v>173</v>
-      </c>
-      <c r="B8" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="57">
+      <c r="A8" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="54">
         <v>0.25</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="25">
         <f t="shared" si="4"/>
-        <v>77854.870867499994</v>
-      </c>
-      <c r="E8" s="34">
+        <v>70943.442352500002</v>
+      </c>
+      <c r="E8" s="32">
         <f t="shared" si="5"/>
-        <v>34558.247640000001</v>
-      </c>
-      <c r="F8" s="27">
+        <v>31303.724414999997</v>
+      </c>
+      <c r="F8" s="25">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"VWRA")</f>
         <v>34908</v>
       </c>
-      <c r="G8" s="41">
+      <c r="G8" s="39">
         <f>F8/E8</f>
-        <v>1.0101206624723404</v>
-      </c>
-      <c r="H8" s="34">
+        <v>1.1151388741230075</v>
+      </c>
+      <c r="H8" s="32">
         <f t="shared" si="7"/>
-        <v>43296.623227499986</v>
-      </c>
-      <c r="I8" s="27">
+        <v>39639.717937499998</v>
+      </c>
+      <c r="I8" s="25">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"VWRA")</f>
         <v>52362</v>
       </c>
-      <c r="J8" s="41">
+      <c r="J8" s="39">
         <f>I8/H8</f>
-        <v>1.2093783786524515</v>
-      </c>
-      <c r="K8" s="50">
+        <v>1.3209478453544812</v>
+      </c>
+      <c r="K8" s="48">
         <f>F8+I8</f>
         <v>87270</v>
       </c>
-      <c r="L8" s="41">
+      <c r="L8" s="39">
         <f>K8/D8</f>
-        <v>1.1209317930604941</v>
-      </c>
-      <c r="M8" s="14"/>
+        <v>1.2301348384869382</v>
+      </c>
+      <c r="M8" s="12"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="47" t="s">
-        <v>181</v>
-      </c>
-      <c r="B9" s="55" t="s">
-        <v>183</v>
-      </c>
-      <c r="C9" s="57">
+      <c r="A9" s="45" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="54">
         <v>0.15</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="25">
         <f t="shared" ref="D9" si="9">$D$4*C9</f>
-        <v>46712.922520499997</v>
-      </c>
-      <c r="E9" s="34">
+        <v>42566.0654115</v>
+      </c>
+      <c r="E9" s="32">
         <f t="shared" ref="E9" si="10">$E$4*C9</f>
-        <v>20734.948584000002</v>
-      </c>
-      <c r="F9" s="27">
+        <v>18782.234648999998</v>
+      </c>
+      <c r="F9" s="25">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"WORLD")</f>
         <v>20804.541300000001</v>
       </c>
-      <c r="G9" s="41">
+      <c r="G9" s="39">
         <f>F9/E9</f>
-        <v>1.0033563003890784</v>
-      </c>
-      <c r="H9" s="34">
+        <v>1.1076712483254847</v>
+      </c>
+      <c r="H9" s="32">
         <f t="shared" ref="H9" si="11">$H$4*C9</f>
-        <v>25977.973936499991</v>
-      </c>
-      <c r="I9" s="27">
+        <v>23783.830762499998</v>
+      </c>
+      <c r="I9" s="25">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"WORLD")</f>
         <v>25427.772700000001</v>
       </c>
-      <c r="J9" s="41">
+      <c r="J9" s="39">
         <f>I9/H9</f>
-        <v>0.97882047161010743</v>
-      </c>
-      <c r="K9" s="50">
+        <v>1.0691201494795368</v>
+      </c>
+      <c r="K9" s="48">
         <f>F9+I9</f>
         <v>46232.313999999998</v>
       </c>
-      <c r="L9" s="41">
+      <c r="L9" s="39">
         <f>K9/D9</f>
-        <v>0.98971144397379374</v>
-      </c>
-      <c r="M9" s="14"/>
+        <v>1.0861307840660672</v>
+      </c>
+      <c r="M9" s="12"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="47" t="s">
-        <v>182</v>
-      </c>
-      <c r="B10" s="55" t="s">
-        <v>183</v>
-      </c>
-      <c r="C10" s="57">
+      <c r="A10" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="54">
         <v>0.1</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="25">
         <f t="shared" si="4"/>
-        <v>31141.948346999998</v>
-      </c>
-      <c r="E10" s="34">
+        <v>28377.376941000002</v>
+      </c>
+      <c r="E10" s="32">
         <f t="shared" si="5"/>
-        <v>13823.299056000002</v>
-      </c>
-      <c r="F10" s="27">
+        <v>12521.489765999999</v>
+      </c>
+      <c r="F10" s="25">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"XMME")</f>
         <v>12489.9864</v>
       </c>
-      <c r="G10" s="41">
+      <c r="G10" s="39">
         <f>F10/E10</f>
-        <v>0.90354598778492912</v>
-      </c>
-      <c r="H10" s="34">
+        <v>0.99748405608368251</v>
+      </c>
+      <c r="H10" s="32">
         <f t="shared" si="7"/>
-        <v>17318.649290999994</v>
-      </c>
-      <c r="I10" s="27">
+        <v>15855.887175</v>
+      </c>
+      <c r="I10" s="25">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"XMME")</f>
         <v>16653.315200000001</v>
       </c>
-      <c r="J10" s="41">
+      <c r="J10" s="39">
         <f>I10/H10</f>
-        <v>0.96158279552749248</v>
-      </c>
-      <c r="K10" s="50">
+        <v>1.0502922363283025</v>
+      </c>
+      <c r="K10" s="48">
         <f>F10+I10</f>
         <v>29143.301599999999</v>
       </c>
-      <c r="L10" s="41">
+      <c r="L10" s="39">
         <f>K10/D10</f>
-        <v>0.93582139676265519</v>
-      </c>
-      <c r="M10" s="14"/>
+        <v>1.0269906785462393</v>
+      </c>
+      <c r="M10" s="12"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="46" t="s">
-        <v>188</v>
-      </c>
-      <c r="B11" s="55"/>
-      <c r="C11" s="56">
+      <c r="A11" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" s="52"/>
+      <c r="C11" s="53">
         <v>0.3</v>
       </c>
-      <c r="D11" s="26">
-        <f>$G$43*C11</f>
-        <v>311419.48346999998</v>
-      </c>
-      <c r="E11" s="33">
+      <c r="D11" s="24">
+        <f>$G$42*C11</f>
+        <v>283773.76941000001</v>
+      </c>
+      <c r="E11" s="31">
         <f>$E$2*C11</f>
-        <v>138232.99056000001</v>
-      </c>
-      <c r="F11" s="26">
+        <v>125214.89765999999</v>
+      </c>
+      <c r="F11" s="24">
         <f>F12+F13+F15+F18+F16</f>
         <v>73102.326799999995</v>
       </c>
-      <c r="G11" s="40">
+      <c r="G11" s="38">
         <f>F11/E11</f>
-        <v>0.52883415531887767</v>
-      </c>
-      <c r="H11" s="33">
+        <v>0.58381493070015578</v>
+      </c>
+      <c r="H11" s="31">
         <f>$H$2*C11</f>
-        <v>173186.49290999994</v>
-      </c>
-      <c r="I11" s="26">
+        <v>158558.87174999999</v>
+      </c>
+      <c r="I11" s="24">
         <f>I12+I13+I15+I18+I16</f>
         <v>85799.421000000002</v>
       </c>
-      <c r="J11" s="40">
+      <c r="J11" s="38">
         <f>I11/H11</f>
-        <v>0.49541635469567191</v>
-      </c>
-      <c r="K11" s="49">
+        <v>0.5411202795090525</v>
+      </c>
+      <c r="K11" s="47">
         <f>F11+I11</f>
         <v>158901.74780000001</v>
       </c>
-      <c r="L11" s="41">
+      <c r="L11" s="39">
         <f>K11/D11</f>
-        <v>0.51024985986564808</v>
+        <v>0.55995925250729117</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="47" t="s">
-        <v>184</v>
-      </c>
-      <c r="B12" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="57">
+      <c r="A12" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="54">
         <v>0.25</v>
       </c>
-      <c r="D12" s="27">
-        <f>$D$11*C12</f>
-        <v>77854.870867499994</v>
-      </c>
-      <c r="E12" s="34">
-        <f t="shared" ref="E12:E18" si="12">$E$11*C12</f>
-        <v>34558.247640000001</v>
-      </c>
-      <c r="F12" s="27">
+      <c r="D12" s="25">
+        <f t="shared" ref="D12:D18" si="12">$D$11*C12</f>
+        <v>70943.442352500002</v>
+      </c>
+      <c r="E12" s="32">
+        <f t="shared" ref="E12:E18" si="13">$E$11*C12</f>
+        <v>31303.724414999997</v>
+      </c>
+      <c r="F12" s="25">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"CSNDX")</f>
         <v>21996</v>
       </c>
-      <c r="G12" s="41">
+      <c r="G12" s="39">
         <f>F12/E12</f>
-        <v>0.63649060650113443</v>
-      </c>
-      <c r="H12" s="34">
-        <f t="shared" ref="H12:H18" si="13">$H$11*C12</f>
-        <v>43296.623227499986</v>
-      </c>
-      <c r="I12" s="27">
+        <v>0.70266399321673179</v>
+      </c>
+      <c r="H12" s="32">
+        <f t="shared" ref="H12:H18" si="14">$H$11*C12</f>
+        <v>39639.717937499998</v>
+      </c>
+      <c r="I12" s="25">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"CSNDX")</f>
         <v>29328</v>
       </c>
-      <c r="J12" s="41">
+      <c r="J12" s="39">
         <f>I12/H12</f>
-        <v>0.67737384150947433</v>
-      </c>
-      <c r="K12" s="50">
+        <v>0.73986399313540785</v>
+      </c>
+      <c r="K12" s="48">
         <f t="shared" si="0"/>
         <v>51324</v>
       </c>
-      <c r="L12" s="41">
+      <c r="L12" s="39">
         <f t="shared" si="1"/>
-        <v>0.6592265766819847</v>
-      </c>
-      <c r="M12" s="14"/>
+        <v>0.72344952962648812</v>
+      </c>
+      <c r="M12" s="12"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="47" t="s">
-        <v>185</v>
-      </c>
-      <c r="B13" s="55" t="s">
-        <v>183</v>
-      </c>
-      <c r="C13" s="57">
+      <c r="A13" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" s="54">
         <v>0.25</v>
       </c>
-      <c r="D13" s="27">
-        <f>$D$11*C13</f>
-        <v>77854.870867499994</v>
-      </c>
-      <c r="E13" s="34">
+      <c r="D13" s="25">
         <f t="shared" si="12"/>
-        <v>34558.247640000001</v>
-      </c>
-      <c r="F13" s="27">
+        <v>70943.442352500002</v>
+      </c>
+      <c r="E13" s="32">
+        <f t="shared" si="13"/>
+        <v>31303.724414999997</v>
+      </c>
+      <c r="F13" s="25">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"EQCH")</f>
         <v>21460.376799999998</v>
       </c>
-      <c r="G13" s="41">
-        <f t="shared" ref="G13:G18" si="14">F13/E13</f>
-        <v>0.62099146413779205</v>
-      </c>
-      <c r="H13" s="34">
-        <f t="shared" si="13"/>
-        <v>43296.623227499986</v>
-      </c>
-      <c r="I13" s="27">
+      <c r="G13" s="39">
+        <f t="shared" ref="G13:G18" si="15">F13/E13</f>
+        <v>0.6855534669132437</v>
+      </c>
+      <c r="H13" s="32">
+        <f t="shared" si="14"/>
+        <v>39639.717937499998</v>
+      </c>
+      <c r="I13" s="25">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"EQCH")</f>
         <v>26825.471000000001</v>
       </c>
-      <c r="J13" s="41">
-        <f t="shared" ref="J13:J18" si="15">I13/H13</f>
-        <v>0.61957420695482135</v>
-      </c>
-      <c r="K13" s="50">
+      <c r="J13" s="39">
+        <f t="shared" ref="J13:J18" si="16">I13/H13</f>
+        <v>0.67673213624516104</v>
+      </c>
+      <c r="K13" s="48">
         <f t="shared" si="0"/>
         <v>48285.847800000003</v>
       </c>
-      <c r="L13" s="41">
+      <c r="L13" s="39">
         <f t="shared" si="1"/>
-        <v>0.62020329957488396</v>
-      </c>
-      <c r="M13" s="14"/>
+        <v>0.68062453975773896</v>
+      </c>
+      <c r="M13" s="12"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="47" t="s">
-        <v>190</v>
-      </c>
-      <c r="B14" s="55" t="s">
-        <v>183</v>
-      </c>
-      <c r="C14" s="57">
+      <c r="A14" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="54">
         <v>0.2</v>
       </c>
-      <c r="D14" s="27">
-        <f>$D$11*C14</f>
-        <v>62283.896693999995</v>
-      </c>
-      <c r="E14" s="34">
-        <f t="shared" ref="E14" si="16">$E$11*C14</f>
-        <v>27646.598112000003</v>
-      </c>
-      <c r="F14" s="27">
-        <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"EQCH")</f>
-        <v>21460.376799999998</v>
-      </c>
-      <c r="G14" s="41">
-        <f t="shared" ref="G14" si="17">F14/E14</f>
-        <v>0.77623933017224001</v>
-      </c>
-      <c r="H14" s="34">
-        <f t="shared" ref="H14" si="18">$H$11*C14</f>
-        <v>34637.298581999989</v>
-      </c>
-      <c r="I14" s="27">
-        <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"EQCH")</f>
-        <v>26825.471000000001</v>
-      </c>
-      <c r="J14" s="41">
-        <f t="shared" ref="J14" si="19">I14/H14</f>
-        <v>0.77446775869352669</v>
-      </c>
-      <c r="K14" s="50">
-        <f t="shared" ref="K14" si="20">F14+I14</f>
-        <v>48285.847800000003</v>
-      </c>
-      <c r="L14" s="41">
-        <f t="shared" ref="L14" si="21">K14/D14</f>
-        <v>0.77525412446860498</v>
-      </c>
-      <c r="M14" s="14"/>
+      <c r="D14" s="25">
+        <f t="shared" si="12"/>
+        <v>56754.753882000005</v>
+      </c>
+      <c r="E14" s="32">
+        <f t="shared" ref="E14" si="17">$E$11*C14</f>
+        <v>25042.979531999998</v>
+      </c>
+      <c r="F14" s="25">
+        <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"CBUK")</f>
+        <v>21933.266199999998</v>
+      </c>
+      <c r="G14" s="39">
+        <f t="shared" ref="G14" si="18">F14/E14</f>
+        <v>0.87582494614802531</v>
+      </c>
+      <c r="H14" s="32">
+        <f t="shared" ref="H14" si="19">$H$11*C14</f>
+        <v>31711.77435</v>
+      </c>
+      <c r="I14" s="25">
+        <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"CBUK")</f>
+        <v>21933.266199999998</v>
+      </c>
+      <c r="J14" s="39">
+        <f t="shared" ref="J14" si="20">I14/H14</f>
+        <v>0.69164424411969239</v>
+      </c>
+      <c r="K14" s="48">
+        <f t="shared" ref="K14" si="21">F14+I14</f>
+        <v>43866.532399999996</v>
+      </c>
+      <c r="L14" s="39">
+        <f t="shared" ref="L14" si="22">K14/D14</f>
+        <v>0.7729137983965858</v>
+      </c>
+      <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="47" t="s">
-        <v>168</v>
-      </c>
-      <c r="B15" s="55" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="57">
+      <c r="A15" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="54">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="D15" s="27">
-        <f>$D$11*C15</f>
-        <v>23356.461260249998</v>
-      </c>
-      <c r="E15" s="34">
+      <c r="D15" s="25">
         <f t="shared" si="12"/>
-        <v>10367.474292000001</v>
-      </c>
-      <c r="F15" s="27">
+        <v>21283.03270575</v>
+      </c>
+      <c r="E15" s="32">
+        <f t="shared" si="13"/>
+        <v>9391.1173244999991</v>
+      </c>
+      <c r="F15" s="25">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"HEAL")</f>
         <v>9372.5</v>
       </c>
-      <c r="G15" s="41">
+      <c r="G15" s="39">
+        <f t="shared" si="15"/>
+        <v>0.99801756022668042</v>
+      </c>
+      <c r="H15" s="32">
         <f t="shared" si="14"/>
-        <v>0.90402924917134675</v>
-      </c>
-      <c r="H15" s="34">
-        <f t="shared" si="13"/>
-        <v>12988.986968249996</v>
-      </c>
-      <c r="I15" s="27">
+        <v>11891.915381249999</v>
+      </c>
+      <c r="I15" s="25">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"HEAL")</f>
         <v>9372.5</v>
       </c>
-      <c r="J15" s="41">
-        <f t="shared" si="15"/>
-        <v>0.72157282341647888</v>
-      </c>
-      <c r="K15" s="50">
+      <c r="J15" s="39">
+        <f t="shared" si="16"/>
+        <v>0.78814048868676234</v>
+      </c>
+      <c r="K15" s="48">
         <f t="shared" si="0"/>
         <v>18745</v>
       </c>
-      <c r="L15" s="41">
+      <c r="L15" s="39">
         <f t="shared" si="1"/>
-        <v>0.80256164626710069</v>
-      </c>
-      <c r="M15" s="14"/>
+        <v>0.88074854082875587</v>
+      </c>
+      <c r="M15" s="12"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="57">
+      <c r="A16" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="54">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="D16" s="27">
-        <f>$D$11*C16</f>
-        <v>23356.461260249998</v>
-      </c>
-      <c r="E16" s="34">
+      <c r="D16" s="25">
+        <f t="shared" si="12"/>
+        <v>21283.03270575</v>
+      </c>
+      <c r="E16" s="32">
         <f>$E$11*C16</f>
-        <v>10367.474292000001</v>
-      </c>
-      <c r="F16" s="27">
+        <v>9391.1173244999991</v>
+      </c>
+      <c r="F16" s="25">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"INRA")</f>
         <v>10423.450000000001</v>
       </c>
-      <c r="G16" s="41">
+      <c r="G16" s="39">
         <f>F16/E16</f>
-        <v>1.0053991653534355</v>
-      </c>
-      <c r="H16" s="34">
+        <v>1.1099265018025919</v>
+      </c>
+      <c r="H16" s="32">
         <f>$H$11*C16</f>
-        <v>12988.986968249996</v>
-      </c>
-      <c r="I16" s="27">
+        <v>11891.915381249999</v>
+      </c>
+      <c r="I16" s="25">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"INRA")</f>
         <v>10423.450000000001</v>
       </c>
-      <c r="J16" s="41">
+      <c r="J16" s="39">
         <f>I16/H16</f>
-        <v>0.80248367524571862</v>
-      </c>
-      <c r="K16" s="50">
+        <v>0.87651565503355922</v>
+      </c>
+      <c r="K16" s="48">
         <f>F16+I16</f>
         <v>20846.900000000001</v>
       </c>
-      <c r="L16" s="41">
+      <c r="L16" s="39">
         <f>K16/D16</f>
-        <v>0.89255387482345283</v>
-      </c>
-      <c r="M16" s="14"/>
+        <v>0.97950796243280835</v>
+      </c>
+      <c r="M16" s="12"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="47" t="s">
-        <v>186</v>
-      </c>
-      <c r="B17" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="57">
+      <c r="A17" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="54">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="D17" s="27">
-        <f>$D$11*C17</f>
-        <v>23356.461260249998</v>
-      </c>
-      <c r="E17" s="34">
+      <c r="D17" s="25">
+        <f t="shared" si="12"/>
+        <v>21283.03270575</v>
+      </c>
+      <c r="E17" s="32">
         <f>$E$11*C17</f>
-        <v>10367.474292000001</v>
-      </c>
-      <c r="F17" s="27">
+        <v>9391.1173244999991</v>
+      </c>
+      <c r="F17" s="25">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"GRID")</f>
         <v>0</v>
       </c>
-      <c r="G17" s="41">
+      <c r="G17" s="39">
         <f>F17/E17</f>
         <v>0</v>
       </c>
-      <c r="H17" s="34">
+      <c r="H17" s="32">
         <f>$H$11*C17</f>
-        <v>12988.986968249996</v>
-      </c>
-      <c r="I17" s="27">
+        <v>11891.915381249999</v>
+      </c>
+      <c r="I17" s="25">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"GRID")</f>
         <v>0</v>
       </c>
-      <c r="J17" s="41">
+      <c r="J17" s="39">
         <f>I17/H17</f>
         <v>0</v>
       </c>
-      <c r="K17" s="50">
+      <c r="K17" s="48">
         <f>F17+I17</f>
         <v>0</v>
       </c>
-      <c r="L17" s="41">
+      <c r="L17" s="39">
         <f>K17/D17</f>
         <v>0</v>
       </c>
-      <c r="M17" s="14"/>
+      <c r="M17" s="12"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="57">
+      <c r="A18" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="54">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="D18" s="27">
-        <f>$D$11*C18</f>
-        <v>23356.461260249998</v>
-      </c>
-      <c r="E18" s="34">
+      <c r="D18" s="25">
         <f t="shared" si="12"/>
-        <v>10367.474292000001</v>
-      </c>
-      <c r="F18" s="27">
+        <v>21283.03270575</v>
+      </c>
+      <c r="E18" s="32">
+        <f t="shared" si="13"/>
+        <v>9391.1173244999991</v>
+      </c>
+      <c r="F18" s="25">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"LOCK")</f>
         <v>9850</v>
       </c>
-      <c r="G18" s="41">
+      <c r="G18" s="39">
+        <f t="shared" si="15"/>
+        <v>1.0488634802062207</v>
+      </c>
+      <c r="H18" s="32">
         <f t="shared" si="14"/>
-        <v>0.95008675426383193</v>
-      </c>
-      <c r="H18" s="34">
-        <f t="shared" si="13"/>
-        <v>12988.986968249996</v>
-      </c>
-      <c r="I18" s="27">
+        <v>11891.915381249999</v>
+      </c>
+      <c r="I18" s="25">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"LOCK")</f>
         <v>9850</v>
       </c>
-      <c r="J18" s="41">
-        <f t="shared" si="15"/>
-        <v>0.75833473573244248</v>
-      </c>
-      <c r="K18" s="50">
+      <c r="J18" s="39">
+        <f t="shared" si="16"/>
+        <v>0.82829381846514905</v>
+      </c>
+      <c r="K18" s="48">
         <f t="shared" si="0"/>
         <v>19700</v>
       </c>
-      <c r="L18" s="41">
+      <c r="L18" s="39">
         <f t="shared" si="1"/>
-        <v>0.84344968959519251</v>
-      </c>
-      <c r="M18" s="14"/>
+        <v>0.92561996555489412</v>
+      </c>
+      <c r="M18" s="12"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="46" t="s">
-        <v>187</v>
-      </c>
-      <c r="B19" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="56">
+      <c r="A19" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="53">
         <v>0.25</v>
       </c>
-      <c r="D19" s="26">
-        <f>$G$43*C19</f>
-        <v>259516.23622499997</v>
-      </c>
-      <c r="E19" s="33">
+      <c r="D19" s="24">
+        <f>$G$42*C19</f>
+        <v>236478.141175</v>
+      </c>
+      <c r="E19" s="31">
         <f>$E$2*C19</f>
-        <v>115194.1588</v>
-      </c>
-      <c r="F19" s="26" cm="1">
+        <v>104345.74804999999</v>
+      </c>
+      <c r="F19" s="24" cm="1">
         <f t="array" ref="F19">SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,IncomeStrategy!A:A))</f>
         <v>89228</v>
       </c>
-      <c r="G19" s="40">
+      <c r="G19" s="38">
         <f>F19/E19</f>
-        <v>0.77458788648231347</v>
-      </c>
-      <c r="H19" s="33">
+        <v>0.85511869594575207</v>
+      </c>
+      <c r="H19" s="31">
         <f>$H$2*C19</f>
-        <v>144322.07742499997</v>
-      </c>
-      <c r="I19" s="26" cm="1">
+        <v>132132.393125</v>
+      </c>
+      <c r="I19" s="24" cm="1">
         <f t="array" ref="I19">SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,IncomeStrategy!A:A))</f>
         <v>64467</v>
       </c>
-      <c r="J19" s="40">
-        <f t="shared" ref="J19:J24" si="22">I19/H19</f>
-        <v>0.44668841489966526</v>
-      </c>
-      <c r="K19" s="49">
+      <c r="J19" s="38">
+        <f t="shared" ref="J19:J23" si="23">I19/H19</f>
+        <v>0.48789701355830944</v>
+      </c>
+      <c r="K19" s="47">
         <f t="shared" si="0"/>
         <v>153695</v>
       </c>
-      <c r="L19" s="40">
+      <c r="L19" s="38">
         <f t="shared" si="1"/>
-        <v>0.59223654841675033</v>
+        <v>0.64993322104245432</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="46" t="s">
-        <v>191</v>
-      </c>
-      <c r="B20" s="55"/>
-      <c r="C20" s="56">
-        <v>0.05</v>
+      <c r="A20" s="44" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="55">
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D20" s="26">
-        <f>$G$43*C20</f>
-        <v>51903.247244999999</v>
+        <f>$G$42*C20</f>
+        <v>23647.814117500002</v>
       </c>
       <c r="E20" s="33">
         <f>$E$2*C20</f>
-        <v>23038.831760000001</v>
-      </c>
-      <c r="F20" s="26">
-        <f>F21+F22</f>
-        <v>94379.890700000018</v>
-      </c>
-      <c r="G20" s="40">
-        <f>F20/E20</f>
-        <v>4.0965571381037771</v>
+        <v>10434.574805</v>
+      </c>
+      <c r="F20" s="26" cm="1">
+        <f t="array" ref="F20">SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK")-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,GlobalETF!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,GrowthEngine!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,IncomeStrategy!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,Gold!A:A))</f>
+        <v>7890.0000000000255</v>
+      </c>
+      <c r="G20" s="38">
+        <f t="shared" ref="G20:G21" si="24">F20/E20</f>
+        <v>0.75614005816694374</v>
       </c>
       <c r="H20" s="33">
         <f>$H$2*C20</f>
-        <v>28864.415484999994</v>
-      </c>
-      <c r="I20" s="26">
-        <f>I21+I22</f>
-        <v>103378.02509999994</v>
+        <v>13213.239312500002</v>
+      </c>
+      <c r="I20" s="26" cm="1">
+        <f t="array" ref="I20">SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK")-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,GlobalETF!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,GrowthEngine!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,IncomeStrategy!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,Gold!A:A))</f>
+        <v>3606.4799999999341</v>
       </c>
       <c r="J20" s="40">
         <f>I20/H20</f>
-        <v>3.581504193414986</v>
+        <v>0.27294442450521034</v>
       </c>
       <c r="K20" s="49">
-        <f>F20+I20</f>
-        <v>197757.91579999996</v>
+        <f t="shared" si="0"/>
+        <v>11496.47999999996</v>
       </c>
       <c r="L20" s="40">
         <f t="shared" si="1"/>
-        <v>3.8101260768236536</v>
-      </c>
+        <v>0.48615402433716964</v>
+      </c>
+      <c r="M20" s="13"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="47" t="s">
-        <v>166</v>
-      </c>
-      <c r="B21" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="58">
-        <v>0.5</v>
-      </c>
-      <c r="D21" s="28">
-        <f>$D$20*C21</f>
-        <v>25951.623622499999</v>
-      </c>
-      <c r="E21" s="35">
-        <f>$E$20*C21</f>
-        <v>11519.41588</v>
-      </c>
-      <c r="F21" s="28" cm="1">
-        <f t="array" ref="F21">SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK")-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,GlobalETF!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,GrowthEngine!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,IncomeStrategy!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,Gold!A:A))</f>
-        <v>84578.170700000017</v>
-      </c>
-      <c r="G21" s="42">
-        <f t="shared" ref="G21:G24" si="23">F21/H21</f>
-        <v>5.8603764724737184</v>
-      </c>
-      <c r="H21" s="35">
-        <f>$H$20*C21</f>
-        <v>14432.207742499997</v>
-      </c>
-      <c r="I21" s="28" cm="1">
-        <f t="array" ref="I21">SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK")-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,GlobalETF!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,GrowthEngine!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,IncomeStrategy!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,Gold!A:A))</f>
-        <v>94446.30509999994</v>
-      </c>
-      <c r="J21" s="42">
-        <f>I21/H21</f>
-        <v>6.5441342575657533</v>
-      </c>
-      <c r="K21" s="51">
-        <f t="shared" si="0"/>
-        <v>179024.47579999996</v>
-      </c>
-      <c r="L21" s="42">
-        <f t="shared" si="1"/>
-        <v>6.8983921161983153</v>
-      </c>
-      <c r="M21" s="15"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="47" t="s">
-        <v>189</v>
-      </c>
-      <c r="B22" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="58">
-        <v>0.5</v>
-      </c>
-      <c r="D22" s="28">
-        <f>$D$20*C22</f>
-        <v>25951.623622499999</v>
-      </c>
-      <c r="E22" s="35">
-        <f>$E$20*C22</f>
-        <v>11519.41588</v>
-      </c>
-      <c r="F22" s="28">
+      <c r="A21" s="44" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="55">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D21" s="26">
+        <f>$G$42*C21</f>
+        <v>23647.814117500002</v>
+      </c>
+      <c r="E21" s="33">
+        <f>$E$2*C21</f>
+        <v>10434.574805</v>
+      </c>
+      <c r="F21" s="26">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"OPT",[1]PositionsHK!T:T,"Long")+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"FOP",[1]PositionsHK!T:T,"Long")</f>
         <v>9801.7200000000012</v>
       </c>
-      <c r="G22" s="42">
-        <f t="shared" si="23"/>
-        <v>0.67915596663259459</v>
-      </c>
-      <c r="H22" s="35">
-        <f>$H$20*C22</f>
-        <v>14432.207742499997</v>
-      </c>
-      <c r="I22" s="28">
+      <c r="G21" s="38">
+        <f t="shared" si="24"/>
+        <v>0.93935020670926139</v>
+      </c>
+      <c r="H21" s="33">
+        <f>H2*C21</f>
+        <v>13213.239312500002</v>
+      </c>
+      <c r="I21" s="26">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"OPT",[1]PositionsAL!T:T,"Long")+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"FOP",[1]PositionsAL!T:T,"Long")</f>
         <v>8931.7200000000012</v>
       </c>
-      <c r="J22" s="42">
-        <f>I22/H22</f>
-        <v>0.6188741292642187</v>
-      </c>
-      <c r="K22" s="51">
+      <c r="J21" s="40">
+        <f>I21/H21</f>
+        <v>0.67596747389191736</v>
+      </c>
+      <c r="K21" s="49">
         <f t="shared" si="0"/>
         <v>18733.440000000002</v>
       </c>
-      <c r="L22" s="42">
+      <c r="L21" s="40">
         <f t="shared" si="1"/>
-        <v>0.7218600374489923</v>
-      </c>
-      <c r="M22" s="15"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="46" t="s">
-        <v>167</v>
-      </c>
-      <c r="B23" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="56">
+        <v>0.79218484663818323</v>
+      </c>
+      <c r="M21" s="13"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B22" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="53">
         <v>0.05</v>
       </c>
-      <c r="D23" s="26">
-        <f>$G$43*C23</f>
-        <v>51903.247244999999</v>
-      </c>
-      <c r="E23" s="33">
-        <f>$E$2*C23</f>
-        <v>23038.831760000001</v>
-      </c>
-      <c r="F23" s="26">
+      <c r="D22" s="24">
+        <f>$G$42*C22</f>
+        <v>47295.628235000004</v>
+      </c>
+      <c r="E22" s="31">
+        <f>$E$2*C22</f>
+        <v>20869.14961</v>
+      </c>
+      <c r="F22" s="24">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"GSD")</f>
         <v>25314.1482</v>
       </c>
-      <c r="G23" s="40">
-        <f t="shared" si="23"/>
-        <v>0.87700193385710634</v>
-      </c>
-      <c r="H23" s="33">
-        <f>$H$2*C23</f>
-        <v>28864.415484999994</v>
-      </c>
-      <c r="I23" s="26">
+      <c r="G22" s="38">
+        <f t="shared" ref="G22:G23" si="25">F22/H22</f>
+        <v>0.95790848864942169</v>
+      </c>
+      <c r="H22" s="31">
+        <f>$H$2*C22</f>
+        <v>26426.478625000003</v>
+      </c>
+      <c r="I22" s="24">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"GSD")</f>
         <v>25314.1482</v>
       </c>
-      <c r="J23" s="40">
-        <f t="shared" si="22"/>
-        <v>0.87700193385710634</v>
-      </c>
-      <c r="K23" s="49">
+      <c r="J22" s="38">
+        <f t="shared" si="23"/>
+        <v>0.95790848864942169</v>
+      </c>
+      <c r="K22" s="47">
         <f t="shared" si="0"/>
         <v>50628.296399999999</v>
       </c>
-      <c r="L23" s="40">
+      <c r="L22" s="38">
         <f t="shared" si="1"/>
-        <v>0.97543601002492542</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="45" t="s">
-        <v>165</v>
-      </c>
-      <c r="B24" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="56">
+        <v>1.0704646135249714</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="53">
         <v>0.05</v>
       </c>
-      <c r="D24" s="26">
-        <f>$G$43*C24</f>
-        <v>51903.247244999999</v>
-      </c>
-      <c r="E24" s="36">
-        <f>$E$2*C24</f>
-        <v>23038.831760000001</v>
-      </c>
-      <c r="F24" s="59" t="str">
+      <c r="D23" s="24">
+        <f>$G$42*C23</f>
+        <v>47295.628235000004</v>
+      </c>
+      <c r="E23" s="34">
+        <f>$E$2*C23</f>
+        <v>20869.14961</v>
+      </c>
+      <c r="F23" s="56" t="str">
         <f>[1]Summary!$C$2</f>
         <v>$134,409.76</v>
       </c>
-      <c r="G24" s="43">
-        <f t="shared" si="23"/>
-        <v>4.6565903983002492</v>
-      </c>
-      <c r="H24" s="36">
-        <f>$H$2*C24</f>
-        <v>28864.415484999994</v>
-      </c>
-      <c r="I24" s="59" t="str">
+      <c r="G23" s="41">
+        <f t="shared" si="25"/>
+        <v>5.0861774626622234</v>
+      </c>
+      <c r="H23" s="34">
+        <f>$H$2*C23</f>
+        <v>26426.478625000003</v>
+      </c>
+      <c r="I23" s="56" t="str">
         <f>[1]Summary!$C$3</f>
         <v>$158,827.53</v>
       </c>
-      <c r="J24" s="43">
-        <f t="shared" si="22"/>
-        <v>5.5025375477476093</v>
-      </c>
-      <c r="K24" s="52">
+      <c r="J23" s="41">
+        <f t="shared" si="23"/>
+        <v>6.0101662523339687</v>
+      </c>
+      <c r="K23" s="50">
         <f t="shared" si="0"/>
         <v>293237.29000000004</v>
       </c>
-      <c r="L24" s="43">
+      <c r="L23" s="41">
         <f t="shared" si="1"/>
-        <v>5.6496906371931956</v>
-      </c>
+        <v>6.2000929249312042</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="8">
+        <f>C4+C11+C19+C20+C21+C22+C23</f>
+        <v>1</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="10">
-        <f>C4+C11+C19+C20+C23+C24</f>
-        <v>1</v>
-      </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
+      <c r="F25" s="4"/>
+      <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F26" s="6"/>
-      <c r="I26" s="6"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+    </row>
+    <row r="41" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G41" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="H41" s="17"/>
     </row>
     <row r="42" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G42" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="H42" s="19"/>
+      <c r="G42" s="22">
+        <f>E2+H2</f>
+        <v>945912.56469999999</v>
+      </c>
+      <c r="H42" s="17"/>
     </row>
     <row r="43" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G43" s="24">
-        <f>E2+H2</f>
-        <v>1038064.9448999999</v>
-      </c>
-      <c r="H43" s="19"/>
+      <c r="G43" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="H43" s="23">
+        <f>G44/G42</f>
+        <v>0.68999535375343979</v>
+      </c>
     </row>
     <row r="44" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G44" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="H44" s="25">
-        <f>G45/G43</f>
-        <v>0.71751546814034017</v>
-      </c>
+      <c r="G44" s="22">
+        <f>G42-G46</f>
+        <v>652675.27469999995</v>
+      </c>
+      <c r="H44" s="17"/>
     </row>
     <row r="45" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G45" s="24">
-        <f>G43-G47</f>
-        <v>744827.65489999985</v>
-      </c>
-      <c r="H45" s="19"/>
+      <c r="G45" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="H45" s="23">
+        <f>G46/G42</f>
+        <v>0.31000464624656027</v>
+      </c>
     </row>
     <row r="46" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G46" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="H46" s="25">
-        <f>G47/G43</f>
-        <v>0.28248453185965983</v>
-      </c>
-    </row>
-    <row r="47" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G47" s="24">
-        <f>F24+I24</f>
+      <c r="G46" s="22">
+        <f>F23+I23</f>
         <v>293237.29000000004</v>
       </c>
-      <c r="H47" s="19"/>
+      <c r="H46" s="17"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="17"/>
+      <c r="B51" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="19"/>
-      <c r="B52" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="E52" s="23"/>
-      <c r="F52" s="23"/>
+      <c r="A52" s="18" t="str">
+        <f>A4</f>
+        <v>Global Triads (the strategic core)</v>
+      </c>
+      <c r="B52" s="19">
+        <f>D4</f>
+        <v>283773.76941000001</v>
+      </c>
+      <c r="C52" s="20">
+        <f>K4</f>
+        <v>296687.19050000003</v>
+      </c>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="20" t="str">
-        <f>A4</f>
-        <v>Global Traids (The strategic core)</v>
-      </c>
-      <c r="B53" s="21">
-        <f>D4</f>
-        <v>311419.48346999998</v>
-      </c>
-      <c r="C53" s="22">
-        <f>K4</f>
-        <v>221311.57490000001</v>
-      </c>
-      <c r="E53" s="23"/>
-      <c r="F53" s="23"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="20" t="str">
+      <c r="A53" s="18" t="str">
         <f>A11</f>
-        <v>Four Horsemen (The growth engine)</v>
-      </c>
-      <c r="B54" s="21">
+        <v>Four Horsemen (growth engine)</v>
+      </c>
+      <c r="B53" s="19">
         <f>D11</f>
-        <v>311419.48346999998</v>
-      </c>
-      <c r="C54" s="22">
+        <v>283773.76941000001</v>
+      </c>
+      <c r="C53" s="20">
         <f>K11</f>
         <v>158901.74780000001</v>
       </c>
-      <c r="E54" s="23"/>
-      <c r="F54" s="23"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="20" t="str">
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="18" t="str">
         <f>A19</f>
-        <v>Cash Cow (The Income Strategy)</v>
-      </c>
-      <c r="B55" s="21">
+        <v>Cash Cow (income Strategy)</v>
+      </c>
+      <c r="B54" s="19">
         <f>D19</f>
-        <v>259516.23622499997</v>
-      </c>
-      <c r="C55" s="22">
+        <v>236478.141175</v>
+      </c>
+      <c r="C54" s="20">
         <f>K19</f>
         <v>153695</v>
       </c>
-      <c r="E55" s="23"/>
-      <c r="F55" s="23"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="18" t="str">
+        <f>A20</f>
+        <v>The Alpha (theme, buy calls)</v>
+      </c>
+      <c r="B55" s="19">
+        <f>D20</f>
+        <v>23647.814117500002</v>
+      </c>
+      <c r="C55" s="20">
+        <f>K20</f>
+        <v>11496.47999999996</v>
+      </c>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="20" t="str">
+      <c r="A56" s="18" t="str">
         <f>A21</f>
-        <v>The Sniper (theme stocks)</v>
-      </c>
-      <c r="B56" s="21">
+        <v>The Omega (insurance, bear spreads)</v>
+      </c>
+      <c r="B56" s="19">
         <f>D21</f>
-        <v>25951.623622499999</v>
-      </c>
-      <c r="C56" s="22">
+        <v>23647.814117500002</v>
+      </c>
+      <c r="C56" s="20">
         <f>K21</f>
-        <v>179024.47579999996</v>
-      </c>
-      <c r="E56" s="23"/>
-      <c r="F56" s="23"/>
+        <v>18733.440000000002</v>
+      </c>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="20" t="str">
+      <c r="A57" s="18" t="str">
         <f>A22</f>
-        <v>The Hedge (bear spreads 4xQQQ, 4xSPY)</v>
-      </c>
-      <c r="B57" s="21">
+        <v>The Vault (Gold)</v>
+      </c>
+      <c r="B57" s="19">
         <f>D22</f>
-        <v>25951.623622499999</v>
-      </c>
-      <c r="C57" s="22">
+        <v>47295.628235000004</v>
+      </c>
+      <c r="C57" s="20">
         <f>K22</f>
-        <v>18733.440000000002</v>
-      </c>
-      <c r="E57" s="23"/>
-      <c r="F57" s="23"/>
+        <v>50628.296399999999</v>
+      </c>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="20" t="str">
+      <c r="A58" s="18" t="str">
         <f>A23</f>
-        <v>Reserve: Gold</v>
-      </c>
-      <c r="B58" s="21">
+        <v>The War Chest (Cash)</v>
+      </c>
+      <c r="B58" s="19">
         <f>D23</f>
-        <v>51903.247244999999</v>
-      </c>
-      <c r="C58" s="22">
+        <v>47295.628235000004</v>
+      </c>
+      <c r="C58" s="20">
         <f>K23</f>
-        <v>50628.296399999999</v>
-      </c>
-      <c r="E58" s="23"/>
-      <c r="F58" s="23"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="20" t="str">
-        <f>A24</f>
-        <v>Reserve: Cash</v>
-      </c>
-      <c r="B59" s="21">
-        <f>D24</f>
-        <v>51903.247244999999</v>
-      </c>
-      <c r="C59" s="22">
-        <f>K24</f>
         <v>293237.29000000004</v>
       </c>
-      <c r="E59" s="23"/>
-      <c r="F59" s="23"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G4:G24">
-    <cfRule type="expression" dxfId="39" priority="149">
-      <formula>AND(G4&gt;=120%)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="150">
-      <formula>AND(G4&lt;50%)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="151">
+  <conditionalFormatting sqref="G4:G23 L16:L23">
+    <cfRule type="expression" dxfId="31" priority="151">
       <formula>AND(G4&gt;=50%, G4&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="152">
+    <cfRule type="expression" dxfId="30" priority="152">
       <formula>AND(G4&gt;=80%, G4&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J10">
-    <cfRule type="expression" dxfId="35" priority="85">
+    <cfRule type="expression" dxfId="29" priority="85">
       <formula>AND(J4&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="86">
+    <cfRule type="expression" dxfId="28" priority="86">
       <formula>AND(J4&lt;50%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="87">
+    <cfRule type="expression" dxfId="27" priority="87">
       <formula>AND(J4&gt;=50%, J4&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="88">
+    <cfRule type="expression" dxfId="26" priority="88">
       <formula>AND(J4&gt;=80%, J4&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:J10">
-    <cfRule type="expression" dxfId="31" priority="81">
+    <cfRule type="expression" dxfId="25" priority="81">
       <formula>AND(J8&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="82">
+    <cfRule type="expression" dxfId="24" priority="82">
       <formula>AND(J8&lt;50%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="83">
+    <cfRule type="expression" dxfId="23" priority="83">
       <formula>AND(J8&gt;=50%, J8&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="84">
+    <cfRule type="expression" dxfId="22" priority="84">
       <formula>AND(J8&gt;=80%, J8&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J11:J18">
-    <cfRule type="expression" dxfId="27" priority="125">
+  <conditionalFormatting sqref="J11:J23">
+    <cfRule type="expression" dxfId="21" priority="125">
       <formula>AND(J11&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="126">
+    <cfRule type="expression" dxfId="20" priority="126">
       <formula>AND(J11&lt;50%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="127">
+    <cfRule type="expression" dxfId="19" priority="127">
       <formula>AND(J11&gt;=50%, J11&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="128">
+    <cfRule type="expression" dxfId="18" priority="128">
       <formula>AND(J11&gt;=80%, J11&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:J17">
-    <cfRule type="expression" dxfId="23" priority="121">
+    <cfRule type="expression" dxfId="17" priority="121">
       <formula>AND(J16&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="122">
+    <cfRule type="expression" dxfId="16" priority="122">
       <formula>AND(J16&lt;50%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="123">
+    <cfRule type="expression" dxfId="15" priority="123">
       <formula>AND(J16&gt;=50%, J16&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="124">
+    <cfRule type="expression" dxfId="14" priority="124">
       <formula>AND(J16&gt;=80%, J16&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J19:J24">
-    <cfRule type="expression" dxfId="19" priority="97">
-      <formula>AND(J19&gt;=120%)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="98">
-      <formula>AND(J19&lt;50%)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="99">
-      <formula>AND(J19&gt;=50%, J19&lt;80%)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="100">
-      <formula>AND(J19&gt;=80%, J19&lt;=120%)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="L4:L9">
-    <cfRule type="expression" dxfId="15" priority="61">
+    <cfRule type="expression" dxfId="13" priority="61">
       <formula>AND(L4&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="62">
+    <cfRule type="expression" dxfId="12" priority="62">
       <formula>AND(L4&lt;50%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="63">
+    <cfRule type="expression" dxfId="11" priority="63">
       <formula>AND(L4&gt;=50%, L4&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="64">
+    <cfRule type="expression" dxfId="10" priority="64">
       <formula>AND(L4&gt;=80%, L4&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:L11">
-    <cfRule type="expression" dxfId="11" priority="53">
+    <cfRule type="expression" dxfId="9" priority="53">
       <formula>AND(L8&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="54">
+    <cfRule type="expression" dxfId="8" priority="54">
       <formula>AND(L8&lt;50%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="55">
+    <cfRule type="expression" dxfId="7" priority="55">
       <formula>AND(L8&gt;=50%, L8&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="56">
+    <cfRule type="expression" dxfId="6" priority="56">
       <formula>AND(L8&gt;=80%, L8&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:L17">
-    <cfRule type="expression" dxfId="7" priority="33">
+    <cfRule type="expression" dxfId="5" priority="33">
       <formula>AND(L10&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="34">
+    <cfRule type="expression" dxfId="4" priority="34">
       <formula>AND(L10&lt;50%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="35">
+    <cfRule type="expression" dxfId="3" priority="35">
       <formula>AND(L10&gt;=50%, L10&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="36">
+    <cfRule type="expression" dxfId="2" priority="36">
       <formula>AND(L10&gt;=80%, L10&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L16:L24">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>AND(L16&gt;=120%)</formula>
+  <conditionalFormatting sqref="L16:L23 G4:G23">
+    <cfRule type="expression" dxfId="1" priority="149">
+      <formula>AND(G4&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>AND(L16&lt;50%)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>AND(L16&gt;=50%, L16&lt;80%)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="4">
-      <formula>AND(L16&gt;=80%, L16&lt;=120%)</formula>
+    <cfRule type="expression" dxfId="0" priority="150">
+      <formula>AND(G4&lt;50%)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6061,145 +5975,184 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="75.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="7" style="58" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" style="58" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.83203125" style="58" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="58" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.5" style="58" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="58" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="58" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="57" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="57" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="57" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" s="59">
+        <v>82846</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="60">
+        <v>3.8E-3</v>
+      </c>
+      <c r="E2" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="G2" s="61">
+        <v>-6.3500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>183</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>161</v>
+      </c>
+      <c r="F3" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="G3" s="62" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A4" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" s="59" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="G4" s="62" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
-        <v>82846</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="4">
-        <v>3.8E-3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="4">
-        <v>2.8E-3</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="4">
-        <v>1.9E-3</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="4">
-        <v>1.9E-3</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E7" s="4"/>
+      <c r="C5" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="F5" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="G5" s="62" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="59" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>174</v>
+      </c>
+      <c r="E6" s="59" t="s">
+        <v>175</v>
+      </c>
+      <c r="F6" s="59" t="s">
+        <v>176</v>
+      </c>
+      <c r="G6" s="62" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="59" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>180</v>
+      </c>
+      <c r="F7" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="G7" s="62" t="s">
+        <v>182</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6208,260 +6161,159 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="68.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="68.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="4">
-        <v>3.3E-3</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="J2" s="6">
-        <f>Dashboard!$E$11*GrowthEngine!I2</f>
-        <v>55293.196224000007</v>
-      </c>
-      <c r="K2" s="6">
-        <f>Dashboard!$H$11*GrowthEngine!I2</f>
-        <v>69274.597163999977</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>184</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>51</v>
+        <v>138</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="4">
-        <v>4.4999999999999997E-3</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.35499999999999998</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="J3" s="6">
-        <f>Dashboard!$E$11*GrowthEngine!I3</f>
-        <v>27646.598112000003</v>
-      </c>
-      <c r="K3" s="6">
-        <f>Dashboard!$H$11*GrowthEngine!I3</f>
-        <v>34637.298581999989</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>185</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>187</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="4">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.185</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="J4" s="6">
-        <f>Dashboard!$E$11*GrowthEngine!I4</f>
-        <v>20734.948584000002</v>
-      </c>
-      <c r="K4" s="6">
-        <f>Dashboard!$H$11*GrowthEngine!I4</f>
-        <v>25977.973936499991</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>52</v>
+        <v>191</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="4">
-        <v>6.4999999999999997E-3</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.46</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="J5" s="6">
-        <f>Dashboard!$E$11*GrowthEngine!I5</f>
-        <v>13823.299056000002</v>
-      </c>
-      <c r="K5" s="6">
-        <f>Dashboard!$H$11*GrowthEngine!I5</f>
-        <v>17318.649290999994</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>189</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" s="4">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.115</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="J6" s="6">
-        <f>Dashboard!$E$11*GrowthEngine!I6</f>
-        <v>20734.948584000002</v>
-      </c>
-      <c r="K6" s="6">
-        <f>Dashboard!$H$11*GrowthEngine!I6</f>
-        <v>25977.973936499991</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I7" s="3">
-        <f>SUM(I2:I6)</f>
-        <v>1</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6473,7 +6325,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6488,394 +6340,394 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E11" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="7" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E12" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="7" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="B13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="E13" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="7" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="C14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E14" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="C15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E15" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="E16" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="7" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="B17" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E17" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="B18" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="D18" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="E18" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="7" t="s">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="B19" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D19" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E19" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="B20" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E20" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="8" t="s">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="B21" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="D21" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E21" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="D22" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E22" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B23" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D12" s="7" t="s">
+      <c r="C23" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E23" s="5" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -6907,37 +6759,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>71</v>
+      <c r="C1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>161</v>
+      <c r="A2" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -6957,17 +6809,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>162</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>163</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>164</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update fetch IBKR positions dashboard Excel file
</commit_message>
<xml_diff>
--- a/projects/fetch-ibkr-positions-dashboard.xlsx
+++ b/projects/fetch-ibkr-positions-dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hongkiatkoh/Developer/timeless-workspace/projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A22F24-6172-EF42-9284-C2214DC5EBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86B8931-3F59-C148-AF2E-FBE9876FDC6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13360" yWindow="2220" windowWidth="31840" windowHeight="22560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4400" yWindow="1500" windowWidth="39780" windowHeight="23580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId7"/>
-    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">IncomeStrategy!$A$1:$E$1</definedName>
@@ -278,7 +277,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="197">
   <si>
     <t>HK</t>
   </si>
@@ -304,9 +303,6 @@
     <t>Actual %</t>
   </si>
   <si>
-    <t>Remarks</t>
-  </si>
-  <si>
     <t>Security (LOCK)</t>
   </si>
   <si>
@@ -644,9 +640,6 @@
   </si>
   <si>
     <t>Biotic (HEAL)</t>
-  </si>
-  <si>
-    <t>VWRA/VT: The concrete foundation. ES3/DHL: The income pillars (Stability/Cash Flow). 82846: The growth pillar (China exposure).</t>
   </si>
   <si>
     <t>82846 (china etf)</t>
@@ -888,7 +881,7 @@
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -993,6 +986,14 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1121,7 +1122,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1132,13 +1133,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1193,6 +1188,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -1200,7 +1196,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="34">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1587,25 +1588,25 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>282356.97500999999</c:v>
+                  <c:v>303025.54100999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>282356.97500999999</c:v>
+                  <c:v>303025.54100999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>235297.47917500001</c:v>
+                  <c:v>252521.28417499998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23529.747917500004</c:v>
+                  <c:v>25252.1284175</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23529.747917500004</c:v>
+                  <c:v>25252.1284175</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>47059.495835000009</c:v>
+                  <c:v>50504.256835</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>47059.495835000009</c:v>
+                  <c:v>50504.256835</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1737,7 +1738,7 @@
                   <c:v>295003.50795</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>163928.95999999999</c:v>
+                  <c:v>207257.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>149223.32</c:v>
@@ -2185,10 +2186,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.6600869661654335</c:v>
+                  <c:v>0.68327152991756324</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.3399130338345665</c:v>
+                  <c:v>0.31672847008243676</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2571,6 +2572,28 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.2048192771084338E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-27AB-6144-B7D4-D5E33E9380E8}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -4384,15 +4407,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4420,14 +4443,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4477,9 +4500,6 @@
           <cell r="F1" t="str">
             <v>Symbol</v>
           </cell>
-          <cell r="T1" t="str">
-            <v>Side</v>
-          </cell>
           <cell r="V1" t="str">
             <v>PositionValueUSD</v>
           </cell>
@@ -4491,9 +4511,6 @@
           <cell r="F2" t="str">
             <v>EQCH</v>
           </cell>
-          <cell r="T2" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V2">
             <v>26620.23</v>
           </cell>
@@ -4505,9 +4522,6 @@
           <cell r="F3" t="str">
             <v>WORLD</v>
           </cell>
-          <cell r="T3" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V3">
             <v>20620.006874999999</v>
           </cell>
@@ -4519,9 +4533,6 @@
           <cell r="F4" t="str">
             <v>XMME</v>
           </cell>
-          <cell r="T4" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V4">
             <v>12303.125249999999</v>
           </cell>
@@ -4533,9 +4544,6 @@
           <cell r="F5" t="str">
             <v>82846</v>
           </cell>
-          <cell r="T5" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V5">
             <v>9076.0920000000006</v>
           </cell>
@@ -4547,9 +4555,6 @@
           <cell r="F6" t="str">
             <v>CBUK</v>
           </cell>
-          <cell r="T6" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V6">
             <v>21664.17</v>
           </cell>
@@ -4561,9 +4566,6 @@
           <cell r="F7" t="str">
             <v>ES3</v>
           </cell>
-          <cell r="T7" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V7">
             <v>19632.5314</v>
           </cell>
@@ -4575,9 +4577,6 @@
           <cell r="F8" t="str">
             <v>GSD</v>
           </cell>
-          <cell r="T8" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V8">
             <v>11690.70875</v>
           </cell>
@@ -4589,9 +4588,6 @@
           <cell r="F9" t="str">
             <v>BITO</v>
           </cell>
-          <cell r="T9" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V9">
             <v>1160</v>
           </cell>
@@ -4603,9 +4599,6 @@
           <cell r="F10" t="str">
             <v>CELH</v>
           </cell>
-          <cell r="T10" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V10">
             <v>2624</v>
           </cell>
@@ -4617,9 +4610,6 @@
           <cell r="F11" t="str">
             <v>CHA</v>
           </cell>
-          <cell r="T11" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V11">
             <v>1172</v>
           </cell>
@@ -4631,9 +4621,6 @@
           <cell r="F12" t="str">
             <v>CSNDX</v>
           </cell>
-          <cell r="T12" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V12">
             <v>22122</v>
           </cell>
@@ -4645,9 +4632,6 @@
           <cell r="F13" t="str">
             <v>GOOGL</v>
           </cell>
-          <cell r="T13" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V13">
             <v>33800</v>
           </cell>
@@ -4659,9 +4643,6 @@
           <cell r="F14" t="str">
             <v>HEAL</v>
           </cell>
-          <cell r="T14" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V14">
             <v>9292.5</v>
           </cell>
@@ -4673,9 +4654,6 @@
           <cell r="F15" t="str">
             <v>INRA</v>
           </cell>
-          <cell r="T15" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V15">
             <v>10418.75</v>
           </cell>
@@ -4687,9 +4665,6 @@
           <cell r="F16" t="str">
             <v>LKNCY</v>
           </cell>
-          <cell r="T16" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V16">
             <v>3337</v>
           </cell>
@@ -4701,9 +4676,6 @@
           <cell r="F17" t="str">
             <v>LOCK</v>
           </cell>
-          <cell r="T17" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V17">
             <v>9824</v>
           </cell>
@@ -4715,9 +4687,6 @@
           <cell r="F18" t="str">
             <v>NVDA</v>
           </cell>
-          <cell r="T18" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V18">
             <v>38226</v>
           </cell>
@@ -4729,9 +4698,6 @@
           <cell r="F19" t="str">
             <v>ORCL</v>
           </cell>
-          <cell r="T19" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V19">
             <v>16458</v>
           </cell>
@@ -4743,9 +4709,6 @@
           <cell r="F20" t="str">
             <v>SE</v>
           </cell>
-          <cell r="T20" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V20">
             <v>2329.8000000000002</v>
           </cell>
@@ -4757,9 +4720,6 @@
           <cell r="F21" t="str">
             <v>VWRA</v>
           </cell>
-          <cell r="T21" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V21">
             <v>34940</v>
           </cell>
@@ -4771,9 +4731,6 @@
           <cell r="F22" t="str">
             <v>QQQ   261218P00560000</v>
           </cell>
-          <cell r="T22" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V22">
             <v>5162.9399999999996</v>
           </cell>
@@ -4785,9 +4742,6 @@
           <cell r="F23" t="str">
             <v>SPY   261218P00620000</v>
           </cell>
-          <cell r="T23" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V23">
             <v>4235.1400000000003</v>
           </cell>
@@ -4799,9 +4753,6 @@
           <cell r="F24" t="str">
             <v>EW2G6 P6525</v>
           </cell>
-          <cell r="T24" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V24">
             <v>875</v>
           </cell>
@@ -4813,9 +4764,6 @@
           <cell r="F25" t="str">
             <v>EW2G6 C7300</v>
           </cell>
-          <cell r="T25" t="str">
-            <v>Long</v>
-          </cell>
           <cell r="V25">
             <v>25</v>
           </cell>
@@ -4827,9 +4775,6 @@
           <cell r="F26" t="str">
             <v>GOOGL 260227P00310000</v>
           </cell>
-          <cell r="T26" t="str">
-            <v>Short</v>
-          </cell>
           <cell r="V26">
             <v>-420.01</v>
           </cell>
@@ -4841,9 +4786,6 @@
           <cell r="F27" t="str">
             <v>GOOGL 260227C00370000</v>
           </cell>
-          <cell r="T27" t="str">
-            <v>Short</v>
-          </cell>
           <cell r="V27">
             <v>-422.62</v>
           </cell>
@@ -4855,9 +4797,6 @@
           <cell r="F28" t="str">
             <v>ORCL  260213C00175000</v>
           </cell>
-          <cell r="T28" t="str">
-            <v>Short</v>
-          </cell>
           <cell r="V28">
             <v>-330</v>
           </cell>
@@ -4869,9 +4808,6 @@
           <cell r="F29" t="str">
             <v>ORCL  260220C00200000</v>
           </cell>
-          <cell r="T29" t="str">
-            <v>Short</v>
-          </cell>
           <cell r="V29">
             <v>-74.5</v>
           </cell>
@@ -4883,9 +4819,6 @@
           <cell r="F30" t="str">
             <v>QQQ   261218P00425000</v>
           </cell>
-          <cell r="T30" t="str">
-            <v>Short</v>
-          </cell>
           <cell r="V30">
             <v>-1433.36</v>
           </cell>
@@ -4897,9 +4830,6 @@
           <cell r="F31" t="str">
             <v>SPY   261218P00505000</v>
           </cell>
-          <cell r="T31" t="str">
-            <v>Short</v>
-          </cell>
           <cell r="V31">
             <v>-1573</v>
           </cell>
@@ -4911,9 +4841,6 @@
           <cell r="F32" t="str">
             <v>EW2G6 P6625</v>
           </cell>
-          <cell r="T32" t="str">
-            <v>Short</v>
-          </cell>
           <cell r="V32">
             <v>-1350</v>
           </cell>
@@ -4924,9 +4851,6 @@
           </cell>
           <cell r="F33" t="str">
             <v>EW2G6 C7200</v>
-          </cell>
-          <cell r="T33" t="str">
-            <v>Short</v>
           </cell>
           <cell r="V33">
             <v>-215</v>
@@ -5212,19 +5136,6 @@
         </row>
       </sheetData>
       <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="PositionsHK"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5242,11 +5153,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D0B6ABF8-99C7-D448-B31B-76226AD3E31D}" name="Query__2" displayName="Query__2" ref="J41:K46" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D0B6ABF8-99C7-D448-B31B-76226AD3E31D}" name="Query__2" displayName="Query__2" ref="J41:K46" tableType="queryTable" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="J41:K46" xr:uid="{D0B6ABF8-99C7-D448-B31B-76226AD3E31D}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{7DA33D05-B373-C040-923A-8735B8E52F38}" uniqueName="1" name="CurrencyPrimary" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{6E5A9362-71B1-D549-A253-709ADB40623F}" uniqueName="2" name="Total Value USD" queryTableFieldId="2" dataDxfId="32" dataCellStyle="Currency"/>
+    <tableColumn id="2" xr3:uid="{6E5A9362-71B1-D549-A253-709ADB40623F}" uniqueName="2" name="Total Value USD" queryTableFieldId="2" dataDxfId="33" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5537,1059 +5448,1038 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M58"/>
+  <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="38.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="62.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="17.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="17.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="153.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="38.6640625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="38.6640625" style="1"/>
+    <col min="3" max="3" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="38.6640625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="38.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="41"/>
-      <c r="E1" s="26" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="37"/>
+      <c r="E1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="26" t="s">
+      <c r="G1" s="30"/>
+      <c r="H1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="34"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="34"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="41" t="s">
+      <c r="J1" s="30"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="30"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="37" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="9">
         <v>1</v>
       </c>
-      <c r="E2" s="27">
-        <f>F4+F11+F19+F22+F23+F20-F21</f>
-        <v>415458.09427500004</v>
-      </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="27">
-        <f>I4+I11+I19+I22+I23+I20-I21</f>
-        <v>525731.82242500002</v>
-      </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="34"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
+      <c r="E2" s="23">
+        <f>F4+F11+F19+F22+F23+F20+F21</f>
+        <v>449905.70427499997</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="23">
+        <f>I4+I11+I19+I22+I23+I20+I21</f>
+        <v>560179.43242499989</v>
+      </c>
+      <c r="I2" s="24"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="30"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="50" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="15" t="s">
+      <c r="B3" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="G3" s="36" t="s">
-        <v>131</v>
-      </c>
-      <c r="H3" s="29" t="s">
+      <c r="F3" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="J3" s="36" t="s">
+      <c r="I3" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="J3" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="36" t="s">
+      <c r="L3" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="43" t="s">
-        <v>140</v>
-      </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="52">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="47"/>
+      <c r="C4" s="48">
         <v>0.3</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="19">
         <f>$G$42*C4</f>
-        <v>282356.97500999999</v>
-      </c>
-      <c r="E4" s="30">
+        <v>303025.54100999999</v>
+      </c>
+      <c r="E4" s="26">
         <f>$E$2*C4</f>
-        <v>124637.42828250001</v>
-      </c>
-      <c r="F4" s="23" cm="1">
+        <v>134971.71128249998</v>
+      </c>
+      <c r="F4" s="19" cm="1">
         <f t="array" ref="F4">SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,GlobalETF!A:A))</f>
         <v>96571.755525</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="33">
         <f>F4/E4</f>
-        <v>0.77482147101200549</v>
-      </c>
-      <c r="H4" s="30">
+        <v>0.71549626664266208</v>
+      </c>
+      <c r="H4" s="26">
         <f>$H$2*C4</f>
-        <v>157719.54672750001</v>
-      </c>
-      <c r="I4" s="23" cm="1">
+        <v>168053.82972749995</v>
+      </c>
+      <c r="I4" s="19" cm="1">
         <f t="array" ref="I4">SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,GlobalETF!A:A))</f>
         <v>198431.75242500001</v>
       </c>
-      <c r="J4" s="37">
+      <c r="J4" s="33">
         <f>I4/H4</f>
-        <v>1.2581303747203922</v>
-      </c>
-      <c r="K4" s="46">
+        <v>1.1807630492370094</v>
+      </c>
+      <c r="K4" s="42">
         <f t="shared" ref="K4:K23" si="0">F4+I4</f>
         <v>295003.50795</v>
       </c>
-      <c r="L4" s="37">
+      <c r="L4" s="33">
         <f t="shared" ref="L4:L23" si="1">K4/D4</f>
-        <v>1.0447891642823843</v>
-      </c>
-      <c r="M4" s="14" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="B5" s="51" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="53">
+        <v>0.97352687488565437</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="40" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="49">
         <v>0.1</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="20">
         <f>$D$4*C5</f>
-        <v>28235.697501000002</v>
-      </c>
-      <c r="E5" s="31">
+        <v>30302.554101000002</v>
+      </c>
+      <c r="E5" s="27">
         <f>$E$4*C5</f>
-        <v>12463.742828250002</v>
-      </c>
-      <c r="F5" s="24">
+        <v>13497.171128249998</v>
+      </c>
+      <c r="F5" s="20">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"82846")</f>
         <v>9076.0920000000006</v>
       </c>
-      <c r="G5" s="38">
+      <c r="G5" s="34">
         <f>F5/E5</f>
-        <v>0.72819955651109569</v>
-      </c>
-      <c r="H5" s="31">
+        <v>0.6724440191028962</v>
+      </c>
+      <c r="H5" s="27">
         <f>$H$4*C5</f>
-        <v>15771.954672750002</v>
-      </c>
-      <c r="I5" s="24">
+        <v>16805.382972749994</v>
+      </c>
+      <c r="I5" s="20">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"82846")</f>
         <v>9076.0920000000006</v>
       </c>
-      <c r="J5" s="38">
+      <c r="J5" s="34">
         <f>I5/H5</f>
-        <v>0.57545765178245289</v>
-      </c>
-      <c r="K5" s="47">
+        <v>0.54007052470728723</v>
+      </c>
+      <c r="K5" s="43">
         <f t="shared" ref="K5:K7" si="2">F5+I5</f>
         <v>18152.184000000001</v>
       </c>
-      <c r="L5" s="38">
+      <c r="L5" s="34">
         <f t="shared" ref="L5:L7" si="3">K5/D5</f>
-        <v>0.64288066548939049</v>
-      </c>
-      <c r="M5" s="11"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="44" t="s">
-        <v>124</v>
-      </c>
-      <c r="B6" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="53">
+        <v>0.59903148558031838</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="49">
         <v>0.2</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="20">
         <f t="shared" ref="D6:D10" si="4">$D$4*C6</f>
-        <v>56471.395002000005</v>
-      </c>
-      <c r="E6" s="31">
+        <v>60605.108202000003</v>
+      </c>
+      <c r="E6" s="27">
         <f t="shared" ref="E6:E10" si="5">$E$4*C6</f>
-        <v>24927.485656500005</v>
-      </c>
-      <c r="F6" s="24">
+        <v>26994.342256499996</v>
+      </c>
+      <c r="F6" s="20">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"DHL")</f>
         <v>0</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G6" s="34">
         <f t="shared" ref="G6:G7" si="6">F6/E6</f>
         <v>0</v>
       </c>
-      <c r="H6" s="31">
+      <c r="H6" s="27">
         <f t="shared" ref="H6:H10" si="7">$H$4*C6</f>
-        <v>31543.909345500004</v>
-      </c>
-      <c r="I6" s="24">
+        <v>33610.765945499988</v>
+      </c>
+      <c r="I6" s="20">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"DHL")</f>
         <v>56074.2</v>
       </c>
-      <c r="J6" s="38">
+      <c r="J6" s="34">
         <f t="shared" ref="J6:J7" si="8">I6/H6</f>
-        <v>1.7776553751096624</v>
-      </c>
-      <c r="K6" s="47">
+        <v>1.6683404386238794</v>
+      </c>
+      <c r="K6" s="43">
         <f t="shared" si="2"/>
         <v>56074.2</v>
       </c>
-      <c r="L6" s="38">
+      <c r="L6" s="34">
         <f t="shared" si="3"/>
-        <v>0.9929664389911752</v>
-      </c>
-      <c r="M6" s="11"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="44" t="s">
-        <v>125</v>
-      </c>
-      <c r="B7" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="53">
+        <v>0.92523883982026311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="49">
         <v>0.2</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="20">
         <f t="shared" si="4"/>
-        <v>56471.395002000005</v>
-      </c>
-      <c r="E7" s="31">
+        <v>60605.108202000003</v>
+      </c>
+      <c r="E7" s="27">
         <f t="shared" si="5"/>
-        <v>24927.485656500005</v>
-      </c>
-      <c r="F7" s="24">
+        <v>26994.342256499996</v>
+      </c>
+      <c r="F7" s="20">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"ES3")</f>
         <v>19632.5314</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G7" s="34">
         <f t="shared" si="6"/>
-        <v>0.78758570641803538</v>
-      </c>
-      <c r="H7" s="31">
+        <v>0.72728319191673074</v>
+      </c>
+      <c r="H7" s="27">
         <f t="shared" si="7"/>
-        <v>31543.909345500004</v>
-      </c>
-      <c r="I7" s="24">
+        <v>33610.765945499988</v>
+      </c>
+      <c r="I7" s="20">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"ES3")</f>
         <v>39265.0628</v>
       </c>
-      <c r="J7" s="38">
+      <c r="J7" s="34">
         <f t="shared" si="8"/>
-        <v>1.2447747794964255</v>
-      </c>
-      <c r="K7" s="47">
+        <v>1.1682287414594621</v>
+      </c>
+      <c r="K7" s="43">
         <f t="shared" si="2"/>
         <v>58897.5942</v>
       </c>
-      <c r="L7" s="38">
+      <c r="L7" s="34">
         <f t="shared" si="3"/>
-        <v>1.0429633303358996</v>
-      </c>
-      <c r="M7" s="11"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="B8" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="53">
+        <v>0.97182557621531229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="49">
         <v>0.25</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="20">
         <f t="shared" si="4"/>
-        <v>70589.243752499999</v>
-      </c>
-      <c r="E8" s="31">
+        <v>75756.385252499997</v>
+      </c>
+      <c r="E8" s="27">
         <f t="shared" si="5"/>
-        <v>31159.357070625003</v>
-      </c>
-      <c r="F8" s="24">
+        <v>33742.927820624995</v>
+      </c>
+      <c r="F8" s="20">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"VWRA")</f>
         <v>34940</v>
       </c>
-      <c r="G8" s="38">
+      <c r="G8" s="34">
         <f>F8/E8</f>
-        <v>1.1213325076254266</v>
-      </c>
-      <c r="H8" s="31">
+        <v>1.0354762392208097</v>
+      </c>
+      <c r="H8" s="27">
         <f t="shared" si="7"/>
-        <v>39429.886681875003</v>
-      </c>
-      <c r="I8" s="24">
+        <v>42013.457431874987</v>
+      </c>
+      <c r="I8" s="20">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"VWRA")</f>
         <v>52410</v>
       </c>
-      <c r="J8" s="38">
+      <c r="J8" s="34">
         <f>I8/H8</f>
-        <v>1.329194791322889</v>
-      </c>
-      <c r="K8" s="47">
+        <v>1.2474574387262236</v>
+      </c>
+      <c r="K8" s="43">
         <f>F8+I8</f>
         <v>87350</v>
       </c>
-      <c r="L8" s="38">
+      <c r="L8" s="34">
         <f>K8/D8</f>
-        <v>1.2374406546451548</v>
-      </c>
-      <c r="M8" s="11"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="44" t="s">
+        <v>1.1530381196100881</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="B9" s="51" t="s">
-        <v>135</v>
-      </c>
-      <c r="C9" s="53">
+      <c r="C9" s="49">
         <v>0.15</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="20">
         <f t="shared" ref="D9" si="9">$D$4*C9</f>
-        <v>42353.546251499996</v>
-      </c>
-      <c r="E9" s="31">
+        <v>45453.831151499995</v>
+      </c>
+      <c r="E9" s="27">
         <f t="shared" ref="E9" si="10">$E$4*C9</f>
-        <v>18695.614242375003</v>
-      </c>
-      <c r="F9" s="24">
+        <v>20245.756692374995</v>
+      </c>
+      <c r="F9" s="20">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"WORLD")</f>
         <v>20620.006874999999</v>
       </c>
-      <c r="G9" s="38">
+      <c r="G9" s="34">
         <f>F9/E9</f>
-        <v>1.1029328380269645</v>
-      </c>
-      <c r="H9" s="31">
+        <v>1.0184853640351192</v>
+      </c>
+      <c r="H9" s="27">
         <f t="shared" ref="H9" si="11">$H$4*C9</f>
-        <v>23657.932009125001</v>
-      </c>
-      <c r="I9" s="24">
+        <v>25208.074459124993</v>
+      </c>
+      <c r="I9" s="20">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"WORLD")</f>
         <v>25202.230625</v>
       </c>
-      <c r="J9" s="38">
+      <c r="J9" s="34">
         <f>I9/H9</f>
-        <v>1.0652761456613939</v>
-      </c>
-      <c r="K9" s="47">
+        <v>0.999768176100302</v>
+      </c>
+      <c r="K9" s="43">
         <f>F9+I9</f>
         <v>45822.237500000003</v>
       </c>
-      <c r="L9" s="38">
+      <c r="L9" s="34">
         <f>K9/D9</f>
-        <v>1.0818984844362864</v>
-      </c>
-      <c r="M9" s="11"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="44" t="s">
-        <v>134</v>
-      </c>
-      <c r="B10" s="51" t="s">
-        <v>135</v>
-      </c>
-      <c r="C10" s="53">
+        <v>1.0081050670354297</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="49">
         <v>0.1</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="20">
         <f t="shared" si="4"/>
-        <v>28235.697501000002</v>
-      </c>
-      <c r="E10" s="31">
+        <v>30302.554101000002</v>
+      </c>
+      <c r="E10" s="27">
         <f t="shared" si="5"/>
-        <v>12463.742828250002</v>
-      </c>
-      <c r="F10" s="24">
+        <v>13497.171128249998</v>
+      </c>
+      <c r="F10" s="20">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"XMME")</f>
         <v>12303.125249999999</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G10" s="34">
         <f>F10/E10</f>
-        <v>0.98711321466887525</v>
-      </c>
-      <c r="H10" s="31">
+        <v>0.91153361938555966</v>
+      </c>
+      <c r="H10" s="27">
         <f t="shared" si="7"/>
-        <v>15771.954672750002</v>
-      </c>
-      <c r="I10" s="24">
+        <v>16805.382972749994</v>
+      </c>
+      <c r="I10" s="20">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"XMME")</f>
         <v>16404.167000000001</v>
       </c>
-      <c r="J10" s="38">
+      <c r="J10" s="34">
         <f>I10/H10</f>
-        <v>1.0400845894099799</v>
-      </c>
-      <c r="K10" s="47">
+        <v>0.97612574653011086</v>
+      </c>
+      <c r="K10" s="43">
         <f>F10+I10</f>
         <v>28707.292249999999</v>
       </c>
-      <c r="L10" s="38">
+      <c r="L10" s="34">
         <f>K10/D10</f>
-        <v>1.0167020754129872</v>
-      </c>
-      <c r="M10" s="11"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="43" t="s">
-        <v>141</v>
-      </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="52">
+        <v>0.94735553162671005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="47"/>
+      <c r="C11" s="48">
         <v>0.3</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="19">
         <f>$G$42*C11</f>
-        <v>282356.97500999999</v>
-      </c>
-      <c r="E11" s="30">
+        <v>303025.54100999999</v>
+      </c>
+      <c r="E11" s="26">
         <f>$E$2*C11</f>
-        <v>124637.42828250001</v>
-      </c>
-      <c r="F11" s="23">
-        <f>F12+F13+F15+F18+F16</f>
-        <v>78277.48</v>
-      </c>
-      <c r="G11" s="37">
+        <v>134971.71128249998</v>
+      </c>
+      <c r="F11" s="19" cm="1">
+        <f t="array" ref="F11">SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,GrowthEngine!A:A))</f>
+        <v>99941.65</v>
+      </c>
+      <c r="G11" s="33">
         <f>F11/E11</f>
-        <v>0.62804152074269581</v>
-      </c>
-      <c r="H11" s="30">
+        <v>0.74046367976189487</v>
+      </c>
+      <c r="H11" s="26">
         <f>$H$2*C11</f>
-        <v>157719.54672750001</v>
-      </c>
-      <c r="I11" s="23">
-        <f>I12+I13+I15+I18+I16</f>
-        <v>85651.48</v>
-      </c>
-      <c r="J11" s="37">
+        <v>168053.82972749995</v>
+      </c>
+      <c r="I11" s="19" cm="1">
+        <f t="array" ref="I11">SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,GrowthEngine!A:A))</f>
+        <v>107315.65</v>
+      </c>
+      <c r="J11" s="33">
         <f>I11/H11</f>
-        <v>0.54306192084094917</v>
-      </c>
-      <c r="K11" s="46">
+        <v>0.63857902062697891</v>
+      </c>
+      <c r="K11" s="42">
         <f>F11+I11</f>
-        <v>163928.95999999999</v>
-      </c>
-      <c r="L11" s="38">
+        <v>207257.3</v>
+      </c>
+      <c r="L11" s="34">
         <f>K11/D11</f>
-        <v>0.58057343897452596</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="44" t="s">
-        <v>136</v>
-      </c>
-      <c r="B12" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="53">
+        <v>0.68395983820109874</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="49">
         <v>0.25</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="20">
         <f t="shared" ref="D12:D18" si="12">$D$11*C12</f>
-        <v>70589.243752499999</v>
-      </c>
-      <c r="E12" s="31">
+        <v>75756.385252499997</v>
+      </c>
+      <c r="E12" s="27">
         <f t="shared" ref="E12:E18" si="13">$E$11*C12</f>
-        <v>31159.357070625003</v>
-      </c>
-      <c r="F12" s="24">
+        <v>33742.927820624995</v>
+      </c>
+      <c r="F12" s="20">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"CSNDX")</f>
         <v>22122</v>
       </c>
-      <c r="G12" s="38">
+      <c r="G12" s="34">
         <f>F12/E12</f>
-        <v>0.70996330090697446</v>
-      </c>
-      <c r="H12" s="31">
+        <v>0.65560404590849319</v>
+      </c>
+      <c r="H12" s="27">
         <f t="shared" ref="H12:H18" si="14">$H$11*C12</f>
-        <v>39429.886681875003</v>
-      </c>
-      <c r="I12" s="24">
+        <v>42013.457431874987</v>
+      </c>
+      <c r="I12" s="20">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"CSNDX")</f>
         <v>29496</v>
       </c>
-      <c r="J12" s="38">
+      <c r="J12" s="34">
         <f>I12/H12</f>
-        <v>0.74806200276397505</v>
-      </c>
-      <c r="K12" s="47">
+        <v>0.70206076345485013</v>
+      </c>
+      <c r="K12" s="43">
         <f t="shared" si="0"/>
         <v>51618</v>
       </c>
-      <c r="L12" s="38">
+      <c r="L12" s="34">
         <f t="shared" si="1"/>
-        <v>0.73124455307926273</v>
-      </c>
-      <c r="M12" s="11"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="B13" s="51" t="s">
+        <v>0.68136830747605637</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="C13" s="53">
+      <c r="B13" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="49">
         <v>0.25</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="20">
         <f t="shared" si="12"/>
-        <v>70589.243752499999</v>
-      </c>
-      <c r="E13" s="31">
+        <v>75756.385252499997</v>
+      </c>
+      <c r="E13" s="27">
         <f t="shared" si="13"/>
-        <v>31159.357070625003</v>
-      </c>
-      <c r="F13" s="24">
+        <v>33742.927820624995</v>
+      </c>
+      <c r="F13" s="20">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"EQCH")</f>
         <v>26620.23</v>
       </c>
-      <c r="G13" s="38">
+      <c r="G13" s="34">
         <f t="shared" ref="G13:G18" si="15">F13/E13</f>
-        <v>0.85432539380267913</v>
-      </c>
-      <c r="H13" s="31">
+        <v>0.78891286913545999</v>
+      </c>
+      <c r="H13" s="27">
         <f t="shared" si="14"/>
-        <v>39429.886681875003</v>
-      </c>
-      <c r="I13" s="24">
+        <v>42013.457431874987</v>
+      </c>
+      <c r="I13" s="20">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"EQCH")</f>
         <v>26620.23</v>
       </c>
-      <c r="J13" s="38">
+      <c r="J13" s="34">
         <f t="shared" ref="J13:J18" si="16">I13/H13</f>
-        <v>0.67512824002704264</v>
-      </c>
-      <c r="K13" s="47">
+        <v>0.63361198118876139</v>
+      </c>
+      <c r="K13" s="43">
         <f t="shared" si="0"/>
         <v>53240.46</v>
       </c>
-      <c r="L13" s="38">
+      <c r="L13" s="34">
         <f t="shared" si="1"/>
-        <v>0.75422907471103806</v>
-      </c>
-      <c r="M13" s="11"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="44" t="s">
-        <v>139</v>
-      </c>
-      <c r="B14" s="51" t="s">
-        <v>135</v>
-      </c>
-      <c r="C14" s="53">
+        <v>0.70278511603407101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="49">
         <v>0.2</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="20">
         <f t="shared" si="12"/>
-        <v>56471.395002000005</v>
-      </c>
-      <c r="E14" s="31">
+        <v>60605.108202000003</v>
+      </c>
+      <c r="E14" s="27">
         <f t="shared" ref="E14" si="17">$E$11*C14</f>
-        <v>24927.485656500005</v>
-      </c>
-      <c r="F14" s="24">
+        <v>26994.342256499996</v>
+      </c>
+      <c r="F14" s="20">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"CBUK")</f>
         <v>21664.17</v>
       </c>
-      <c r="G14" s="38">
+      <c r="G14" s="34">
         <f t="shared" ref="G14" si="18">F14/E14</f>
-        <v>0.86908765282353795</v>
-      </c>
-      <c r="H14" s="31">
+        <v>0.8025448367716187</v>
+      </c>
+      <c r="H14" s="27">
         <f t="shared" ref="H14" si="19">$H$11*C14</f>
-        <v>31543.909345500004</v>
-      </c>
-      <c r="I14" s="24">
+        <v>33610.765945499988</v>
+      </c>
+      <c r="I14" s="20">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"CBUK")</f>
         <v>21664.17</v>
       </c>
-      <c r="J14" s="38">
+      <c r="J14" s="34">
         <f t="shared" ref="J14" si="20">I14/H14</f>
-        <v>0.68679407370572376</v>
-      </c>
-      <c r="K14" s="47">
+        <v>0.64456043742438207</v>
+      </c>
+      <c r="K14" s="43">
         <f t="shared" ref="K14" si="21">F14+I14</f>
         <v>43328.34</v>
       </c>
-      <c r="L14" s="38">
+      <c r="L14" s="34">
         <f t="shared" ref="L14" si="22">K14/D14</f>
-        <v>0.76726172602014642</v>
-      </c>
-      <c r="M14" s="11"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="B15" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="53">
+        <v>0.71492884486872577</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="49">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="20">
         <f t="shared" si="12"/>
-        <v>21176.773125749998</v>
-      </c>
-      <c r="E15" s="31">
+        <v>22726.915575749998</v>
+      </c>
+      <c r="E15" s="27">
         <f t="shared" si="13"/>
-        <v>9347.8071211875013</v>
-      </c>
-      <c r="F15" s="24">
+        <v>10122.878346187497</v>
+      </c>
+      <c r="F15" s="20">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"HEAL")</f>
         <v>9292.5</v>
       </c>
-      <c r="G15" s="38">
+      <c r="G15" s="34">
         <f t="shared" si="15"/>
-        <v>0.99408341224091545</v>
-      </c>
-      <c r="H15" s="31">
+        <v>0.91797013479864287</v>
+      </c>
+      <c r="H15" s="27">
         <f t="shared" si="14"/>
-        <v>11828.966004562501</v>
-      </c>
-      <c r="I15" s="24">
+        <v>12604.037229562497</v>
+      </c>
+      <c r="I15" s="20">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"HEAL")</f>
         <v>9292.5</v>
       </c>
-      <c r="J15" s="38">
+      <c r="J15" s="34">
         <f t="shared" si="16"/>
-        <v>0.78557162108808398</v>
-      </c>
-      <c r="K15" s="47">
+        <v>0.73726376959635143</v>
+      </c>
+      <c r="K15" s="43">
         <f t="shared" si="0"/>
         <v>18585</v>
       </c>
-      <c r="L15" s="38">
+      <c r="L15" s="34">
         <f t="shared" si="1"/>
-        <v>0.87761246199504683</v>
-      </c>
-      <c r="M15" s="11"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="53">
+        <v>0.81775285071373738</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="49">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="20">
         <f t="shared" si="12"/>
-        <v>21176.773125749998</v>
-      </c>
-      <c r="E16" s="31">
+        <v>22726.915575749998</v>
+      </c>
+      <c r="E16" s="27">
         <f>$E$11*C16</f>
-        <v>9347.8071211875013</v>
-      </c>
-      <c r="F16" s="24">
+        <v>10122.878346187497</v>
+      </c>
+      <c r="F16" s="20">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"INRA")</f>
         <v>10418.75</v>
       </c>
-      <c r="G16" s="38">
+      <c r="G16" s="34">
         <f>F16/E16</f>
-        <v>1.1145662148275532</v>
-      </c>
-      <c r="H16" s="31">
+        <v>1.029228016350106</v>
+      </c>
+      <c r="H16" s="27">
         <f>$H$11*C16</f>
-        <v>11828.966004562501</v>
-      </c>
-      <c r="I16" s="24">
+        <v>12604.037229562497</v>
+      </c>
+      <c r="I16" s="20">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"INRA")</f>
         <v>10418.75</v>
       </c>
-      <c r="J16" s="38">
+      <c r="J16" s="34">
         <f>I16/H16</f>
-        <v>0.88078281702571704</v>
-      </c>
-      <c r="K16" s="47">
+        <v>0.8266200591317715</v>
+      </c>
+      <c r="K16" s="43">
         <f>F16+I16</f>
         <v>20837.5</v>
       </c>
-      <c r="L16" s="38">
+      <c r="L16" s="34">
         <f>K16/D16</f>
-        <v>0.98397899794575139</v>
-      </c>
-      <c r="M16" s="11"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="44" t="s">
-        <v>138</v>
-      </c>
-      <c r="B17" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="53">
+        <v>0.91686440821885939</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="49">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="20">
         <f t="shared" si="12"/>
-        <v>21176.773125749998</v>
-      </c>
-      <c r="E17" s="31">
+        <v>22726.915575749998</v>
+      </c>
+      <c r="E17" s="27">
         <f>$E$11*C17</f>
-        <v>9347.8071211875013</v>
-      </c>
-      <c r="F17" s="24">
+        <v>10122.878346187497</v>
+      </c>
+      <c r="F17" s="20">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"GRID")</f>
         <v>0</v>
       </c>
-      <c r="G17" s="38">
+      <c r="G17" s="34">
         <f>F17/E17</f>
         <v>0</v>
       </c>
-      <c r="H17" s="31">
+      <c r="H17" s="27">
         <f>$H$11*C17</f>
-        <v>11828.966004562501</v>
-      </c>
-      <c r="I17" s="24">
+        <v>12604.037229562497</v>
+      </c>
+      <c r="I17" s="20">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"GRID")</f>
         <v>0</v>
       </c>
-      <c r="J17" s="38">
+      <c r="J17" s="34">
         <f>I17/H17</f>
         <v>0</v>
       </c>
-      <c r="K17" s="47">
+      <c r="K17" s="43">
         <f>F17+I17</f>
         <v>0</v>
       </c>
-      <c r="L17" s="38">
+      <c r="L17" s="34">
         <f>K17/D17</f>
         <v>0</v>
       </c>
-      <c r="M17" s="11"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="53">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="49">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="20">
         <f t="shared" si="12"/>
-        <v>21176.773125749998</v>
-      </c>
-      <c r="E18" s="31">
+        <v>22726.915575749998</v>
+      </c>
+      <c r="E18" s="27">
         <f t="shared" si="13"/>
-        <v>9347.8071211875013</v>
-      </c>
-      <c r="F18" s="24">
+        <v>10122.878346187497</v>
+      </c>
+      <c r="F18" s="20">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"LOCK")</f>
         <v>9824</v>
       </c>
-      <c r="G18" s="38">
+      <c r="G18" s="34">
         <f t="shared" si="15"/>
-        <v>1.0509416671352976</v>
-      </c>
-      <c r="H18" s="31">
+        <v>0.97047496413902257</v>
+      </c>
+      <c r="H18" s="27">
         <f t="shared" si="14"/>
-        <v>11828.966004562501</v>
-      </c>
-      <c r="I18" s="24">
+        <v>12604.037229562497</v>
+      </c>
+      <c r="I18" s="20">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"LOCK")</f>
         <v>9824</v>
       </c>
-      <c r="J18" s="38">
+      <c r="J18" s="34">
         <f t="shared" si="16"/>
-        <v>0.83050369712879613</v>
-      </c>
-      <c r="K18" s="47">
+        <v>0.77943279768787266</v>
+      </c>
+      <c r="K18" s="43">
         <f t="shared" si="0"/>
         <v>19648</v>
       </c>
-      <c r="L18" s="38">
+      <c r="L18" s="34">
         <f t="shared" si="1"/>
-        <v>0.92780896708521288</v>
-      </c>
-      <c r="M18" s="11"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="43" t="s">
-        <v>187</v>
-      </c>
-      <c r="B19" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="52">
+        <v>0.8645255857316928</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="48">
         <v>0.25</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="19">
         <f>$G$42*C19</f>
-        <v>235297.47917500001</v>
-      </c>
-      <c r="E19" s="30">
+        <v>252521.28417499998</v>
+      </c>
+      <c r="E19" s="26">
         <f>$E$2*C19</f>
-        <v>103864.52356875001</v>
-      </c>
-      <c r="F19" s="23" cm="1">
+        <v>112476.42606874999</v>
+      </c>
+      <c r="F19" s="19" cm="1">
         <f t="array" ref="F19">SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,IncomeStrategy!A:A))+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"OPT")-SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"OPT",[1]PositionsHK!F:F,"SPY*")-SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"OPT",[1]PositionsHK!F:F,"QQQ*")+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"FOP")-SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"FOP",[1]PositionsHK!F:F,"SPY*")-SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"FOP",[1]PositionsHK!F:F,"QQQ*")</f>
         <v>86571.87</v>
       </c>
-      <c r="G19" s="37">
+      <c r="G19" s="33">
         <f>F19/E19</f>
-        <v>0.83350760226321496</v>
-      </c>
-      <c r="H19" s="30">
+        <v>0.76968901863119199</v>
+      </c>
+      <c r="H19" s="26">
         <f>$H$2*C19</f>
-        <v>131432.95560625001</v>
-      </c>
-      <c r="I19" s="23" cm="1">
+        <v>140044.85810624997</v>
+      </c>
+      <c r="I19" s="19" cm="1">
         <f t="array" ref="I19">SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,IncomeStrategy!A:A))+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"OPT")-SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"OPT",[1]PositionsAL!F:F,"SPY*")-SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"OPT",[1]PositionsAL!F:F,"QQQ*")+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"FOP")-SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"FOP",[1]PositionsAL!F:F,"SPY*")-SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"FOP",[1]PositionsAL!F:F,"QQQ*")</f>
         <v>62651.45</v>
       </c>
-      <c r="J19" s="37">
+      <c r="J19" s="33">
         <f t="shared" ref="J19:J23" si="23">I19/H19</f>
-        <v>0.47667991418904637</v>
-      </c>
-      <c r="K19" s="46">
+        <v>0.44736701402108792</v>
+      </c>
+      <c r="K19" s="42">
         <f t="shared" si="0"/>
         <v>149223.32</v>
       </c>
-      <c r="L19" s="37">
+      <c r="L19" s="33">
         <f t="shared" si="1"/>
-        <v>0.63419004964781933</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="43" t="s">
-        <v>186</v>
-      </c>
-      <c r="B20" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="54">
+        <v>0.59093363352527006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="B20" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="50">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="21">
         <f>$G$42*C20</f>
-        <v>23529.747917500004</v>
-      </c>
-      <c r="E20" s="32">
+        <v>25252.1284175</v>
+      </c>
+      <c r="E20" s="28">
         <f>$E$2*C20</f>
-        <v>10386.452356875001</v>
-      </c>
-      <c r="F20" s="25" cm="1">
+        <v>11247.642606875001</v>
+      </c>
+      <c r="F20" s="21" cm="1">
         <f t="array" ref="F20">SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK")-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,GlobalETF!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,GrowthEngine!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,IncomeStrategy!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,Gold!A:A))</f>
         <v>10622.800000000008</v>
       </c>
-      <c r="G20" s="37">
+      <c r="G20" s="33">
         <f t="shared" ref="G20:G21" si="24">F20/E20</f>
-        <v>1.0227553773901021</v>
-      </c>
-      <c r="H20" s="32">
+        <v>0.94444679398925213</v>
+      </c>
+      <c r="H20" s="28">
         <f>$H$2*C20</f>
-        <v>13143.295560625002</v>
-      </c>
-      <c r="I20" s="25" cm="1">
+        <v>14004.485810624998</v>
+      </c>
+      <c r="I20" s="21" cm="1">
         <f t="array" ref="I20">SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK")-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,GlobalETF!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,GrowthEngine!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,IncomeStrategy!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,Gold!A:A))</f>
         <v>3581.3399999999965</v>
       </c>
-      <c r="J20" s="39">
+      <c r="J20" s="35">
         <f>I20/H20</f>
-        <v>0.27248417137700687</v>
-      </c>
-      <c r="K20" s="48">
+        <v>0.25572806088195588</v>
+      </c>
+      <c r="K20" s="44">
         <f t="shared" si="0"/>
         <v>14204.140000000005</v>
       </c>
-      <c r="L20" s="39">
+      <c r="L20" s="35">
         <f t="shared" si="1"/>
-        <v>0.60366732571052428</v>
-      </c>
-      <c r="M20" s="12"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="43" t="s">
-        <v>185</v>
-      </c>
-      <c r="B21" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="54">
+        <v>0.56249278338678099</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="39" t="s">
+        <v>183</v>
+      </c>
+      <c r="B21" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="50">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="21">
         <f>$G$42*C21</f>
-        <v>23529.747917500004</v>
-      </c>
-      <c r="E21" s="32">
+        <v>25252.1284175</v>
+      </c>
+      <c r="E21" s="28">
         <f>$E$2*C21</f>
-        <v>10386.452356875001</v>
-      </c>
-      <c r="F21" s="25">
+        <v>11247.642606875001</v>
+      </c>
+      <c r="F21" s="21">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"SPY*")+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"QQQ*")</f>
         <v>6391.72</v>
       </c>
-      <c r="G21" s="37">
+      <c r="G21" s="33">
         <f t="shared" si="24"/>
-        <v>0.61539010437661057</v>
-      </c>
-      <c r="H21" s="32">
+        <v>0.56827196803827407</v>
+      </c>
+      <c r="H21" s="28">
         <f>H2*C21</f>
-        <v>13143.295560625002</v>
-      </c>
-      <c r="I21" s="25">
+        <v>14004.485810624998</v>
+      </c>
+      <c r="I21" s="21">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"SPY*")+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"QQQ*")</f>
         <v>6391.72</v>
       </c>
-      <c r="J21" s="39">
+      <c r="J21" s="35">
         <f>I21/H21</f>
-        <v>0.48631029946161047</v>
-      </c>
-      <c r="K21" s="48">
+        <v>0.45640518948226549</v>
+      </c>
+      <c r="K21" s="44">
         <f t="shared" si="0"/>
         <v>12783.44</v>
       </c>
-      <c r="L21" s="39">
+      <c r="L21" s="35">
         <f t="shared" si="1"/>
-        <v>0.54328843831312146</v>
-      </c>
-      <c r="M21" s="12"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="43" t="s">
-        <v>142</v>
-      </c>
-      <c r="B22" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="52">
+        <v>0.50623217927012198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="48">
         <v>0.05</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="19">
         <f>$G$42*C22</f>
-        <v>47059.495835000009</v>
-      </c>
-      <c r="E22" s="30">
+        <v>50504.256835</v>
+      </c>
+      <c r="E22" s="26">
         <f>$E$2*C22</f>
-        <v>20772.904713750002</v>
-      </c>
-      <c r="F22" s="23">
+        <v>22495.285213750001</v>
+      </c>
+      <c r="F22" s="19">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"GSD")</f>
         <v>11690.70875</v>
       </c>
-      <c r="G22" s="37">
+      <c r="G22" s="33">
         <f t="shared" ref="G22:G23" si="25">F22/H22</f>
-        <v>0.44474038859109671</v>
-      </c>
-      <c r="H22" s="30">
+        <v>0.41739157396019605</v>
+      </c>
+      <c r="H22" s="26">
         <f>$H$2*C22</f>
-        <v>26286.591121250003</v>
-      </c>
-      <c r="I22" s="23">
+        <v>28008.971621249995</v>
+      </c>
+      <c r="I22" s="19">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"GSD")</f>
         <v>0</v>
       </c>
-      <c r="J22" s="37">
+      <c r="J22" s="33">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="K22" s="46">
+      <c r="K22" s="42">
         <f t="shared" si="0"/>
         <v>11690.70875</v>
       </c>
-      <c r="L22" s="37">
+      <c r="L22" s="33">
         <f t="shared" si="1"/>
-        <v>0.2484240118294076</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="42" t="s">
-        <v>143</v>
-      </c>
-      <c r="B23" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="52">
+        <v>0.23147967087594509</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="48">
         <v>0.05</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="19">
         <f>$G$42*C23</f>
-        <v>47059.495835000009</v>
-      </c>
-      <c r="E23" s="33">
+        <v>50504.256835</v>
+      </c>
+      <c r="E23" s="29">
         <f>$E$2*C23</f>
-        <v>20772.904713750002</v>
-      </c>
-      <c r="F23" s="55" t="str">
+        <v>22495.285213750001</v>
+      </c>
+      <c r="F23" s="51" t="str">
         <f>[1]Summary!$C$2</f>
         <v>$138,115.20</v>
       </c>
-      <c r="G23" s="40">
+      <c r="G23" s="36">
         <f t="shared" si="25"/>
-        <v>5.2542073395111357</v>
-      </c>
-      <c r="H23" s="33">
+        <v>4.9311057138282806</v>
+      </c>
+      <c r="H23" s="29">
         <f>$H$2*C23</f>
-        <v>26286.591121250003</v>
-      </c>
-      <c r="I23" s="55" t="str">
+        <v>28008.971621249995</v>
+      </c>
+      <c r="I23" s="51" t="str">
         <f>[1]Summary!$C$3</f>
         <v>$181,807.52</v>
       </c>
-      <c r="J23" s="40">
+      <c r="J23" s="36">
         <f t="shared" si="23"/>
-        <v>6.9163597197290185</v>
-      </c>
-      <c r="K23" s="49">
+        <v>6.4910458855285249</v>
+      </c>
+      <c r="K23" s="45">
         <f t="shared" si="0"/>
         <v>319922.71999999997</v>
       </c>
-      <c r="L23" s="40">
+      <c r="L23" s="36">
         <f t="shared" si="1"/>
-        <v>6.7982606766913296</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+        <v>6.3345694016487348</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="7">
@@ -6606,343 +6496,330 @@
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F25" s="3"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
     </row>
     <row r="41" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G41" s="17" t="s">
+      <c r="G41" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="H41" s="12"/>
+      <c r="J41" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="K41" s="53" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="42" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G42" s="17">
+        <f>E2+H2</f>
+        <v>1010085.1366999999</v>
+      </c>
+      <c r="H42" s="12"/>
+      <c r="J42" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="52">
+        <v>365115.64</v>
+      </c>
+    </row>
+    <row r="43" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G43" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="H43" s="18">
+        <f>G44/G42</f>
+        <v>0.68327152991756324</v>
+      </c>
+      <c r="J43" t="s">
+        <v>133</v>
+      </c>
+      <c r="K43" s="52">
+        <v>127769.98974999999</v>
+      </c>
+    </row>
+    <row r="44" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G44" s="17">
+        <f>G42-G46</f>
+        <v>690162.41669999994</v>
+      </c>
+      <c r="H44" s="12"/>
+      <c r="J44" t="s">
+        <v>13</v>
+      </c>
+      <c r="K44" s="52">
+        <v>99402.54</v>
+      </c>
+    </row>
+    <row r="45" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G45" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="H41" s="16"/>
-      <c r="J41" t="s">
-        <v>182</v>
-      </c>
-      <c r="K41" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="42" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G42" s="21">
-        <f>E2+H2</f>
-        <v>941189.91670000006</v>
-      </c>
-      <c r="H42" s="16"/>
-      <c r="J42" t="s">
-        <v>18</v>
-      </c>
-      <c r="K42" s="56">
-        <v>365115.64</v>
-      </c>
-    </row>
-    <row r="43" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G43" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="H43" s="22">
-        <f>G44/G42</f>
-        <v>0.6600869661654335</v>
-      </c>
-      <c r="J43" t="s">
-        <v>135</v>
-      </c>
-      <c r="K43" s="56">
-        <v>127769.98974999999</v>
-      </c>
-    </row>
-    <row r="44" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G44" s="21">
-        <f>G42-G46</f>
-        <v>621267.19670000009</v>
-      </c>
-      <c r="H44" s="16"/>
-      <c r="J44" t="s">
-        <v>14</v>
-      </c>
-      <c r="K44" s="56">
-        <v>99402.54</v>
-      </c>
-    </row>
-    <row r="45" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G45" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="H45" s="22">
+      <c r="H45" s="18">
         <f>G46/G42</f>
-        <v>0.3399130338345665</v>
+        <v>0.31672847008243676</v>
       </c>
       <c r="J45" t="s">
-        <v>16</v>
-      </c>
-      <c r="K45" s="56">
+        <v>15</v>
+      </c>
+      <c r="K45" s="52">
         <v>70588.302949999998</v>
       </c>
     </row>
     <row r="46" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G46" s="21">
+      <c r="G46" s="17">
         <f>F23+I23</f>
         <v>319922.71999999997</v>
       </c>
-      <c r="H46" s="16"/>
+      <c r="H46" s="12"/>
       <c r="J46" t="s">
-        <v>184</v>
-      </c>
-      <c r="K46" s="56">
+        <v>182</v>
+      </c>
+      <c r="K46" s="52">
         <v>18152.184000000001</v>
       </c>
     </row>
-    <row r="48" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="H48" s="1">
-        <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"OPT",[1]PositionsHK!T:T,"Long")+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"FOP",[1]PositionsHK!T:T,"Long")</f>
-        <v>10298.08</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="16"/>
-      <c r="B51" s="16" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="12"/>
+      <c r="B51" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C51" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="H51" s="1" t="e">
-        <f>SUMIFS([2]PositionsHK!V:V, [2]PositionsHK!D:D, "OPT", [2]PositionsHK!T:T, "Long", [2]PositionsHK!F:F, "SPY")
-+SUMIFS([2]PositionsHK!V:V, [2]PositionsHK!D:D, "OPT", [2]PositionsHK!T:T, "Short", [2]PositionsHK!F:F, "SPY")
-+SUMIFS([2]PositionsHK!V:V, [2]PositionsHK!D:D, "OPT", [2]PositionsHK!T:T, "Long", [2]PositionsHK!F:F, "QQQ")
-+SUMIFS([2]PositionsHK!V:V, [2]PositionsHK!D:D, "OPT", [2]PositionsHK!T:T, "Short", [2]PositionsHK!F:F, "QQQ")</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="17" t="str">
+      <c r="C51" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="13" t="str">
         <f>A4</f>
         <v>Global Triads (the strategic core)</v>
       </c>
-      <c r="B52" s="18">
+      <c r="B52" s="14">
         <f>D4</f>
-        <v>282356.97500999999</v>
-      </c>
-      <c r="C52" s="19">
+        <v>303025.54100999999</v>
+      </c>
+      <c r="C52" s="15">
         <f>K4</f>
         <v>295003.50795</v>
       </c>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="17" t="str">
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="13" t="str">
         <f>A11</f>
         <v>Four Horsemen (growth engine)</v>
       </c>
-      <c r="B53" s="18">
+      <c r="B53" s="14">
         <f>D11</f>
-        <v>282356.97500999999</v>
-      </c>
-      <c r="C53" s="19">
+        <v>303025.54100999999</v>
+      </c>
+      <c r="C53" s="15">
         <f>K11</f>
-        <v>163928.95999999999</v>
-      </c>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="17" t="str">
+        <v>207257.3</v>
+      </c>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="13" t="str">
         <f>A19</f>
         <v>Cash Cow (income Strategy, wheel/CSPs/CC/callOpts)</v>
       </c>
-      <c r="B54" s="18">
+      <c r="B54" s="14">
         <f>D19</f>
-        <v>235297.47917500001</v>
-      </c>
-      <c r="C54" s="19">
+        <v>252521.28417499998</v>
+      </c>
+      <c r="C54" s="15">
         <f>K19</f>
         <v>149223.32</v>
       </c>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="17" t="str">
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="13" t="str">
         <f>A20</f>
         <v>The Alpha (theme stocks)</v>
       </c>
-      <c r="B55" s="18">
+      <c r="B55" s="14">
         <f>D20</f>
-        <v>23529.747917500004</v>
-      </c>
-      <c r="C55" s="19">
+        <v>25252.1284175</v>
+      </c>
+      <c r="C55" s="15">
         <f>K20</f>
         <v>14204.140000000005</v>
       </c>
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="17" t="str">
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="13" t="str">
         <f>A21</f>
         <v>The Omega (insurance, SPY and QQQ bear spreads)</v>
       </c>
-      <c r="B56" s="18">
+      <c r="B56" s="14">
         <f>D21</f>
-        <v>23529.747917500004</v>
-      </c>
-      <c r="C56" s="19">
+        <v>25252.1284175</v>
+      </c>
+      <c r="C56" s="15">
         <f>K21</f>
         <v>12783.44</v>
       </c>
-      <c r="E56" s="20"/>
-      <c r="F56" s="20"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="17" t="str">
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="13" t="str">
         <f>A22</f>
         <v>The Vault (Gold)</v>
       </c>
-      <c r="B57" s="18">
+      <c r="B57" s="14">
         <f>D22</f>
-        <v>47059.495835000009</v>
-      </c>
-      <c r="C57" s="19">
+        <v>50504.256835</v>
+      </c>
+      <c r="C57" s="15">
         <f>K22</f>
         <v>11690.70875</v>
       </c>
-      <c r="E57" s="20"/>
-      <c r="F57" s="20"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="17" t="str">
+      <c r="E57" s="16"/>
+      <c r="F57" s="16"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="13" t="str">
         <f>A23</f>
         <v>The War Chest (Cash)</v>
       </c>
-      <c r="B58" s="18">
+      <c r="B58" s="14">
         <f>D23</f>
-        <v>47059.495835000009</v>
-      </c>
-      <c r="C58" s="19">
+        <v>50504.256835</v>
+      </c>
+      <c r="C58" s="15">
         <f>K23</f>
         <v>319922.71999999997</v>
       </c>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G4:G23 L16:L23">
-    <cfRule type="expression" dxfId="31" priority="151">
+    <cfRule type="expression" dxfId="32" priority="151">
       <formula>AND(G4&gt;=50%, G4&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="152">
+    <cfRule type="expression" dxfId="31" priority="152">
       <formula>AND(G4&gt;=80%, G4&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J10">
-    <cfRule type="expression" dxfId="29" priority="85">
+    <cfRule type="expression" dxfId="30" priority="85">
       <formula>AND(J4&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="86">
+    <cfRule type="expression" dxfId="29" priority="86">
       <formula>AND(J4&lt;50%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="87">
+    <cfRule type="expression" dxfId="28" priority="87">
       <formula>AND(J4&gt;=50%, J4&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="88">
+    <cfRule type="expression" dxfId="27" priority="88">
       <formula>AND(J4&gt;=80%, J4&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:J10">
-    <cfRule type="expression" dxfId="25" priority="81">
+    <cfRule type="expression" dxfId="26" priority="81">
       <formula>AND(J8&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="82">
+    <cfRule type="expression" dxfId="25" priority="82">
       <formula>AND(J8&lt;50%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="83">
+    <cfRule type="expression" dxfId="24" priority="83">
       <formula>AND(J8&gt;=50%, J8&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="84">
+    <cfRule type="expression" dxfId="23" priority="84">
       <formula>AND(J8&gt;=80%, J8&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:J23">
-    <cfRule type="expression" dxfId="21" priority="125">
+    <cfRule type="expression" dxfId="22" priority="125">
       <formula>AND(J11&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="126">
+    <cfRule type="expression" dxfId="21" priority="126">
       <formula>AND(J11&lt;50%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="127">
+    <cfRule type="expression" dxfId="20" priority="127">
       <formula>AND(J11&gt;=50%, J11&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="128">
+    <cfRule type="expression" dxfId="19" priority="128">
       <formula>AND(J11&gt;=80%, J11&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:J17">
-    <cfRule type="expression" dxfId="17" priority="121">
+    <cfRule type="expression" dxfId="18" priority="121">
       <formula>AND(J16&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="122">
+    <cfRule type="expression" dxfId="17" priority="122">
       <formula>AND(J16&lt;50%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="123">
+    <cfRule type="expression" dxfId="16" priority="123">
       <formula>AND(J16&gt;=50%, J16&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="124">
+    <cfRule type="expression" dxfId="15" priority="124">
       <formula>AND(J16&gt;=80%, J16&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:L9">
-    <cfRule type="expression" dxfId="13" priority="61">
+    <cfRule type="expression" dxfId="14" priority="61">
       <formula>AND(L4&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="62">
+    <cfRule type="expression" dxfId="13" priority="62">
       <formula>AND(L4&lt;50%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="63">
+    <cfRule type="expression" dxfId="12" priority="63">
       <formula>AND(L4&gt;=50%, L4&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="64">
+    <cfRule type="expression" dxfId="11" priority="64">
       <formula>AND(L4&gt;=80%, L4&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:L11">
-    <cfRule type="expression" dxfId="9" priority="53">
+    <cfRule type="expression" dxfId="10" priority="53">
       <formula>AND(L8&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="54">
+    <cfRule type="expression" dxfId="9" priority="54">
       <formula>AND(L8&lt;50%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="55">
+    <cfRule type="expression" dxfId="8" priority="55">
       <formula>AND(L8&gt;=50%, L8&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="56">
+    <cfRule type="expression" dxfId="7" priority="56">
       <formula>AND(L8&gt;=80%, L8&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:L17">
-    <cfRule type="expression" dxfId="5" priority="33">
+    <cfRule type="expression" dxfId="6" priority="33">
       <formula>AND(L10&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="34">
+    <cfRule type="expression" dxfId="5" priority="34">
       <formula>AND(L10&lt;50%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="35">
+    <cfRule type="expression" dxfId="4" priority="35">
       <formula>AND(L10&gt;=50%, L10&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="36">
+    <cfRule type="expression" dxfId="3" priority="36">
       <formula>AND(L10&gt;=80%, L10&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16:L23 G4:G23">
-    <cfRule type="expression" dxfId="1" priority="149">
+    <cfRule type="expression" dxfId="2" priority="149">
       <formula>AND(G4&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="150">
+    <cfRule type="expression" dxfId="1" priority="150">
       <formula>AND(G4&lt;50%)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6976,25 +6853,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -7002,19 +6879,19 @@
         <v>82846</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D2" s="1">
         <v>3.8E-3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G2" s="1">
         <v>-6.3500000000000001E-2</v>
@@ -7022,117 +6899,117 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -7163,135 +7040,135 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -7322,393 +7199,393 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -7741,36 +7618,36 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhance market pulse signals deduplication with fuzzy matching and update risk signal documentation
</commit_message>
<xml_diff>
--- a/projects/fetch-ibkr-positions-dashboard.xlsx
+++ b/projects/fetch-ibkr-positions-dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hongkiatkoh/Developer/timeless-workspace/projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86B8931-3F59-C148-AF2E-FBE9876FDC6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96A9371-C299-8145-8C08-C325E094E9C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4400" yWindow="1500" windowWidth="39780" windowHeight="23580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="980" windowWidth="39780" windowHeight="23580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -1122,7 +1122,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1189,6 +1189,7 @@
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -1198,9 +1199,11 @@
   </cellStyles>
   <dxfs count="34">
     <dxf>
-      <font>
-        <b/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7E79"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1213,6 +1216,27 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF7E79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7E79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFD78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1303,14 +1327,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFD78"/>
+          <bgColor rgb="FFFF7E79"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1324,7 +1341,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF7E79"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFD78"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1387,28 +1411,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFFD78"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7E79"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7E79"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1420,14 +1423,12 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFD78"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <font>
+        <b/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -5153,11 +5154,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D0B6ABF8-99C7-D448-B31B-76226AD3E31D}" name="Query__2" displayName="Query__2" ref="J41:K46" tableType="queryTable" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D0B6ABF8-99C7-D448-B31B-76226AD3E31D}" name="Query__2" displayName="Query__2" ref="J41:K46" tableType="queryTable" totalsRowShown="0" headerRowDxfId="33">
   <autoFilter ref="J41:K46" xr:uid="{D0B6ABF8-99C7-D448-B31B-76226AD3E31D}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{7DA33D05-B373-C040-923A-8735B8E52F38}" uniqueName="1" name="CurrencyPrimary" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{6E5A9362-71B1-D549-A253-709ADB40623F}" uniqueName="2" name="Total Value USD" queryTableFieldId="2" dataDxfId="33" dataCellStyle="Currency"/>
+    <tableColumn id="2" xr3:uid="{6E5A9362-71B1-D549-A253-709ADB40623F}" uniqueName="2" name="Total Value USD" queryTableFieldId="2" dataDxfId="32" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5448,10 +5449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L58"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="38.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5470,7 +5471,7 @@
     <col min="14" max="16384" width="38.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="37"/>
       <c r="E1" s="22" t="s">
         <v>0</v>
@@ -5483,7 +5484,7 @@
       <c r="K1" s="41"/>
       <c r="L1" s="30"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
         <v>2</v>
       </c>
@@ -5505,7 +5506,7 @@
       <c r="K2" s="41"/>
       <c r="L2" s="30"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
         <v>3</v>
       </c>
@@ -5543,7 +5544,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="s">
         <v>138</v>
       </c>
@@ -5587,8 +5588,12 @@
         <f t="shared" ref="L4:L23" si="1">K4/D4</f>
         <v>0.97352687488565437</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="54">
+        <f t="shared" ref="M4:M21" si="2">K4/$G$42</f>
+        <v>0.29205806246569632</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="40" t="s">
         <v>121</v>
       </c>
@@ -5627,15 +5632,16 @@
         <v>0.54007052470728723</v>
       </c>
       <c r="K5" s="43">
-        <f t="shared" ref="K5:K7" si="2">F5+I5</f>
+        <f t="shared" ref="K5:K7" si="3">F5+I5</f>
         <v>18152.184000000001</v>
       </c>
       <c r="L5" s="34">
-        <f t="shared" ref="L5:L7" si="3">K5/D5</f>
+        <f t="shared" ref="L5:L7" si="4">K5/D5</f>
         <v>0.59903148558031838</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="54"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="40" t="s">
         <v>122</v>
       </c>
@@ -5646,11 +5652,11 @@
         <v>0.2</v>
       </c>
       <c r="D6" s="20">
-        <f t="shared" ref="D6:D10" si="4">$D$4*C6</f>
+        <f t="shared" ref="D6:D10" si="5">$D$4*C6</f>
         <v>60605.108202000003</v>
       </c>
       <c r="E6" s="27">
-        <f t="shared" ref="E6:E10" si="5">$E$4*C6</f>
+        <f t="shared" ref="E6:E10" si="6">$E$4*C6</f>
         <v>26994.342256499996</v>
       </c>
       <c r="F6" s="20">
@@ -5658,11 +5664,11 @@
         <v>0</v>
       </c>
       <c r="G6" s="34">
-        <f t="shared" ref="G6:G7" si="6">F6/E6</f>
+        <f t="shared" ref="G6:G7" si="7">F6/E6</f>
         <v>0</v>
       </c>
       <c r="H6" s="27">
-        <f t="shared" ref="H6:H10" si="7">$H$4*C6</f>
+        <f t="shared" ref="H6:H10" si="8">$H$4*C6</f>
         <v>33610.765945499988</v>
       </c>
       <c r="I6" s="20">
@@ -5670,19 +5676,20 @@
         <v>56074.2</v>
       </c>
       <c r="J6" s="34">
-        <f t="shared" ref="J6:J7" si="8">I6/H6</f>
+        <f t="shared" ref="J6:J7" si="9">I6/H6</f>
         <v>1.6683404386238794</v>
       </c>
       <c r="K6" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>56074.2</v>
       </c>
       <c r="L6" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.92523883982026311</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="54"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="40" t="s">
         <v>123</v>
       </c>
@@ -5693,11 +5700,11 @@
         <v>0.2</v>
       </c>
       <c r="D7" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>60605.108202000003</v>
       </c>
       <c r="E7" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>26994.342256499996</v>
       </c>
       <c r="F7" s="20">
@@ -5705,11 +5712,11 @@
         <v>19632.5314</v>
       </c>
       <c r="G7" s="34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.72728319191673074</v>
       </c>
       <c r="H7" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>33610.765945499988</v>
       </c>
       <c r="I7" s="20">
@@ -5717,19 +5724,20 @@
         <v>39265.0628</v>
       </c>
       <c r="J7" s="34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.1682287414594621</v>
       </c>
       <c r="K7" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>58897.5942</v>
       </c>
       <c r="L7" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.97182557621531229</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="54"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="40" t="s">
         <v>124</v>
       </c>
@@ -5740,11 +5748,11 @@
         <v>0.25</v>
       </c>
       <c r="D8" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75756.385252499997</v>
       </c>
       <c r="E8" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>33742.927820624995</v>
       </c>
       <c r="F8" s="20">
@@ -5756,7 +5764,7 @@
         <v>1.0354762392208097</v>
       </c>
       <c r="H8" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>42013.457431874987</v>
       </c>
       <c r="I8" s="20">
@@ -5775,8 +5783,9 @@
         <f>K8/D8</f>
         <v>1.1530381196100881</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="54"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="40" t="s">
         <v>131</v>
       </c>
@@ -5787,11 +5796,11 @@
         <v>0.15</v>
       </c>
       <c r="D9" s="20">
-        <f t="shared" ref="D9" si="9">$D$4*C9</f>
+        <f t="shared" ref="D9" si="10">$D$4*C9</f>
         <v>45453.831151499995</v>
       </c>
       <c r="E9" s="27">
-        <f t="shared" ref="E9" si="10">$E$4*C9</f>
+        <f t="shared" ref="E9" si="11">$E$4*C9</f>
         <v>20245.756692374995</v>
       </c>
       <c r="F9" s="20">
@@ -5803,7 +5812,7 @@
         <v>1.0184853640351192</v>
       </c>
       <c r="H9" s="27">
-        <f t="shared" ref="H9" si="11">$H$4*C9</f>
+        <f t="shared" ref="H9" si="12">$H$4*C9</f>
         <v>25208.074459124993</v>
       </c>
       <c r="I9" s="20">
@@ -5822,8 +5831,9 @@
         <f>K9/D9</f>
         <v>1.0081050670354297</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="54"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="40" t="s">
         <v>132</v>
       </c>
@@ -5834,11 +5844,11 @@
         <v>0.1</v>
       </c>
       <c r="D10" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30302.554101000002</v>
       </c>
       <c r="E10" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>13497.171128249998</v>
       </c>
       <c r="F10" s="20">
@@ -5850,7 +5860,7 @@
         <v>0.91153361938555966</v>
       </c>
       <c r="H10" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>16805.382972749994</v>
       </c>
       <c r="I10" s="20">
@@ -5869,8 +5879,9 @@
         <f>K10/D10</f>
         <v>0.94735553162671005</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="54"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="39" t="s">
         <v>139</v>
       </c>
@@ -5914,8 +5925,12 @@
         <f>K11/D11</f>
         <v>0.68395983820109874</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="54">
+        <f t="shared" si="2"/>
+        <v>0.20518795146032962</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="40" t="s">
         <v>134</v>
       </c>
@@ -5926,11 +5941,11 @@
         <v>0.25</v>
       </c>
       <c r="D12" s="20">
-        <f t="shared" ref="D12:D18" si="12">$D$11*C12</f>
+        <f t="shared" ref="D12:D18" si="13">$D$11*C12</f>
         <v>75756.385252499997</v>
       </c>
       <c r="E12" s="27">
-        <f t="shared" ref="E12:E18" si="13">$E$11*C12</f>
+        <f t="shared" ref="E12:E18" si="14">$E$11*C12</f>
         <v>33742.927820624995</v>
       </c>
       <c r="F12" s="20">
@@ -5942,7 +5957,7 @@
         <v>0.65560404590849319</v>
       </c>
       <c r="H12" s="27">
-        <f t="shared" ref="H12:H18" si="14">$H$11*C12</f>
+        <f t="shared" ref="H12:H18" si="15">$H$11*C12</f>
         <v>42013.457431874987</v>
       </c>
       <c r="I12" s="20">
@@ -5961,8 +5976,9 @@
         <f t="shared" si="1"/>
         <v>0.68136830747605637</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="54"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
         <v>135</v>
       </c>
@@ -5973,11 +5989,11 @@
         <v>0.25</v>
       </c>
       <c r="D13" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>75756.385252499997</v>
       </c>
       <c r="E13" s="27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>33742.927820624995</v>
       </c>
       <c r="F13" s="20">
@@ -5985,11 +6001,11 @@
         <v>26620.23</v>
       </c>
       <c r="G13" s="34">
-        <f t="shared" ref="G13:G18" si="15">F13/E13</f>
+        <f t="shared" ref="G13:G18" si="16">F13/E13</f>
         <v>0.78891286913545999</v>
       </c>
       <c r="H13" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>42013.457431874987</v>
       </c>
       <c r="I13" s="20">
@@ -5997,7 +6013,7 @@
         <v>26620.23</v>
       </c>
       <c r="J13" s="34">
-        <f t="shared" ref="J13:J18" si="16">I13/H13</f>
+        <f t="shared" ref="J13:J18" si="17">I13/H13</f>
         <v>0.63361198118876139</v>
       </c>
       <c r="K13" s="43">
@@ -6008,8 +6024,9 @@
         <f t="shared" si="1"/>
         <v>0.70278511603407101</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="54"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
         <v>137</v>
       </c>
@@ -6020,11 +6037,11 @@
         <v>0.2</v>
       </c>
       <c r="D14" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>60605.108202000003</v>
       </c>
       <c r="E14" s="27">
-        <f t="shared" ref="E14" si="17">$E$11*C14</f>
+        <f t="shared" ref="E14" si="18">$E$11*C14</f>
         <v>26994.342256499996</v>
       </c>
       <c r="F14" s="20">
@@ -6032,11 +6049,11 @@
         <v>21664.17</v>
       </c>
       <c r="G14" s="34">
-        <f t="shared" ref="G14" si="18">F14/E14</f>
+        <f t="shared" ref="G14" si="19">F14/E14</f>
         <v>0.8025448367716187</v>
       </c>
       <c r="H14" s="27">
-        <f t="shared" ref="H14" si="19">$H$11*C14</f>
+        <f t="shared" ref="H14" si="20">$H$11*C14</f>
         <v>33610.765945499988</v>
       </c>
       <c r="I14" s="20">
@@ -6044,19 +6061,20 @@
         <v>21664.17</v>
       </c>
       <c r="J14" s="34">
-        <f t="shared" ref="J14" si="20">I14/H14</f>
+        <f t="shared" ref="J14" si="21">I14/H14</f>
         <v>0.64456043742438207</v>
       </c>
       <c r="K14" s="43">
-        <f t="shared" ref="K14" si="21">F14+I14</f>
+        <f t="shared" ref="K14" si="22">F14+I14</f>
         <v>43328.34</v>
       </c>
       <c r="L14" s="34">
-        <f t="shared" ref="L14" si="22">K14/D14</f>
+        <f t="shared" ref="L14" si="23">K14/D14</f>
         <v>0.71492884486872577</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="54"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
         <v>120</v>
       </c>
@@ -6067,11 +6085,11 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="D15" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>22726.915575749998</v>
       </c>
       <c r="E15" s="27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>10122.878346187497</v>
       </c>
       <c r="F15" s="20">
@@ -6079,11 +6097,11 @@
         <v>9292.5</v>
       </c>
       <c r="G15" s="34">
+        <f t="shared" si="16"/>
+        <v>0.91797013479864287</v>
+      </c>
+      <c r="H15" s="27">
         <f t="shared" si="15"/>
-        <v>0.91797013479864287</v>
-      </c>
-      <c r="H15" s="27">
-        <f t="shared" si="14"/>
         <v>12604.037229562497</v>
       </c>
       <c r="I15" s="20">
@@ -6091,7 +6109,7 @@
         <v>9292.5</v>
       </c>
       <c r="J15" s="34">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.73726376959635143</v>
       </c>
       <c r="K15" s="43">
@@ -6102,8 +6120,9 @@
         <f t="shared" si="1"/>
         <v>0.81775285071373738</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M15" s="54"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="40" t="s">
         <v>9</v>
       </c>
@@ -6114,7 +6133,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="D16" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>22726.915575749998</v>
       </c>
       <c r="E16" s="27">
@@ -6149,8 +6168,9 @@
         <f>K16/D16</f>
         <v>0.91686440821885939</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M16" s="54"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="40" t="s">
         <v>136</v>
       </c>
@@ -6161,7 +6181,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="D17" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>22726.915575749998</v>
       </c>
       <c r="E17" s="27">
@@ -6196,8 +6216,9 @@
         <f>K17/D17</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="54"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="40" t="s">
         <v>8</v>
       </c>
@@ -6208,11 +6229,11 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="D18" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>22726.915575749998</v>
       </c>
       <c r="E18" s="27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>10122.878346187497</v>
       </c>
       <c r="F18" s="20">
@@ -6220,11 +6241,11 @@
         <v>9824</v>
       </c>
       <c r="G18" s="34">
+        <f t="shared" si="16"/>
+        <v>0.97047496413902257</v>
+      </c>
+      <c r="H18" s="27">
         <f t="shared" si="15"/>
-        <v>0.97047496413902257</v>
-      </c>
-      <c r="H18" s="27">
-        <f t="shared" si="14"/>
         <v>12604.037229562497</v>
       </c>
       <c r="I18" s="20">
@@ -6232,7 +6253,7 @@
         <v>9824</v>
       </c>
       <c r="J18" s="34">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.77943279768787266</v>
       </c>
       <c r="K18" s="43">
@@ -6243,8 +6264,9 @@
         <f t="shared" si="1"/>
         <v>0.8645255857316928</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="54"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="39" t="s">
         <v>185</v>
       </c>
@@ -6279,7 +6301,7 @@
         <v>62651.45</v>
       </c>
       <c r="J19" s="33">
-        <f t="shared" ref="J19:J23" si="23">I19/H19</f>
+        <f t="shared" ref="J19:J23" si="24">I19/H19</f>
         <v>0.44736701402108792</v>
       </c>
       <c r="K19" s="42">
@@ -6290,8 +6312,12 @@
         <f t="shared" si="1"/>
         <v>0.59093363352527006</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M19" s="54">
+        <f t="shared" si="2"/>
+        <v>0.14773340838131752</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="39" t="s">
         <v>184</v>
       </c>
@@ -6314,7 +6340,7 @@
         <v>10622.800000000008</v>
       </c>
       <c r="G20" s="33">
-        <f t="shared" ref="G20:G21" si="24">F20/E20</f>
+        <f t="shared" ref="G20:G21" si="25">F20/E20</f>
         <v>0.94444679398925213</v>
       </c>
       <c r="H20" s="28">
@@ -6337,8 +6363,12 @@
         <f t="shared" si="1"/>
         <v>0.56249278338678099</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M20" s="54">
+        <f t="shared" si="2"/>
+        <v>1.4062319584669527E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="39" t="s">
         <v>183</v>
       </c>
@@ -6357,11 +6387,11 @@
         <v>11247.642606875001</v>
       </c>
       <c r="F21" s="21">
-        <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"SPY*")+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"QQQ*")</f>
+        <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"SPY*",[1]PositionsHK!D:D,"OPT")+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"SPY*",[1]PositionsHK!D:D,"FOP")+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"QQQ*",[1]PositionsHK!D:D,"OPT")+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"QQQ*",[1]PositionsHK!D:D,"FOP")</f>
         <v>6391.72</v>
       </c>
       <c r="G21" s="33">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.56827196803827407</v>
       </c>
       <c r="H21" s="28">
@@ -6369,7 +6399,7 @@
         <v>14004.485810624998</v>
       </c>
       <c r="I21" s="21">
-        <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"SPY*")+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"QQQ*")</f>
+        <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"SPY*",[1]PositionsAL!D:D,"OPT")+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"SPY*",[1]PositionsAL!D:D,"FOP")+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"QQQ*",[1]PositionsAL!D:D,"OPT")+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"QQQ*",[1]PositionsAL!D:D,"FOP")</f>
         <v>6391.72</v>
       </c>
       <c r="J21" s="35">
@@ -6384,8 +6414,12 @@
         <f t="shared" si="1"/>
         <v>0.50623217927012198</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M21" s="54">
+        <f t="shared" si="2"/>
+        <v>1.2655804481753049E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="39" t="s">
         <v>140</v>
       </c>
@@ -6408,7 +6442,7 @@
         <v>11690.70875</v>
       </c>
       <c r="G22" s="33">
-        <f t="shared" ref="G22:G23" si="25">F22/H22</f>
+        <f t="shared" ref="G22:G23" si="26">F22/H22</f>
         <v>0.41739157396019605</v>
       </c>
       <c r="H22" s="26">
@@ -6420,7 +6454,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="33">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="K22" s="42">
@@ -6431,8 +6465,12 @@
         <f t="shared" si="1"/>
         <v>0.23147967087594509</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M22" s="54">
+        <f>K22/$G$42</f>
+        <v>1.1573983543797255E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="38" t="s">
         <v>141</v>
       </c>
@@ -6455,7 +6493,7 @@
         <v>$138,115.20</v>
       </c>
       <c r="G23" s="36">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>4.9311057138282806</v>
       </c>
       <c r="H23" s="29">
@@ -6467,7 +6505,7 @@
         <v>$181,807.52</v>
       </c>
       <c r="J23" s="36">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>6.4910458855285249</v>
       </c>
       <c r="K23" s="45">
@@ -6478,8 +6516,12 @@
         <f t="shared" si="1"/>
         <v>6.3345694016487348</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M23" s="54">
+        <f>K23/$G$42</f>
+        <v>0.31672847008243676</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="7">
@@ -6496,11 +6538,11 @@
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F25" s="3"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
     </row>
@@ -6710,116 +6752,116 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G4:G23 L16:L23">
-    <cfRule type="expression" dxfId="32" priority="151">
-      <formula>AND(G4&gt;=50%, G4&lt;80%)</formula>
-    </cfRule>
     <cfRule type="expression" dxfId="31" priority="152">
       <formula>AND(G4&gt;=80%, G4&lt;=120%)</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="30" priority="151">
+      <formula>AND(G4&gt;=50%, G4&lt;80%)</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J10">
-    <cfRule type="expression" dxfId="30" priority="85">
+    <cfRule type="expression" dxfId="29" priority="85">
       <formula>AND(J4&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="86">
+    <cfRule type="expression" dxfId="28" priority="86">
       <formula>AND(J4&lt;50%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="87">
+    <cfRule type="expression" dxfId="27" priority="87">
       <formula>AND(J4&gt;=50%, J4&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="88">
+    <cfRule type="expression" dxfId="26" priority="88">
       <formula>AND(J4&gt;=80%, J4&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:J10">
-    <cfRule type="expression" dxfId="26" priority="81">
+    <cfRule type="expression" dxfId="25" priority="81">
       <formula>AND(J8&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="82">
+    <cfRule type="expression" dxfId="24" priority="82">
       <formula>AND(J8&lt;50%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="83">
+    <cfRule type="expression" dxfId="23" priority="83">
       <formula>AND(J8&gt;=50%, J8&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="84">
+    <cfRule type="expression" dxfId="22" priority="84">
       <formula>AND(J8&gt;=80%, J8&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:J23">
-    <cfRule type="expression" dxfId="22" priority="125">
+    <cfRule type="expression" dxfId="21" priority="127">
+      <formula>AND(J11&gt;=50%, J11&lt;80%)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="128">
+      <formula>AND(J11&gt;=80%, J11&lt;=120%)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="125">
       <formula>AND(J11&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="126">
+    <cfRule type="expression" dxfId="18" priority="126">
       <formula>AND(J11&lt;50%)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="127">
-      <formula>AND(J11&gt;=50%, J11&lt;80%)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="128">
-      <formula>AND(J11&gt;=80%, J11&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:J17">
-    <cfRule type="expression" dxfId="18" priority="121">
+    <cfRule type="expression" dxfId="17" priority="121">
       <formula>AND(J16&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="122">
+    <cfRule type="expression" dxfId="16" priority="122">
       <formula>AND(J16&lt;50%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="123">
+    <cfRule type="expression" dxfId="15" priority="123">
       <formula>AND(J16&gt;=50%, J16&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="124">
+    <cfRule type="expression" dxfId="14" priority="124">
       <formula>AND(J16&gt;=80%, J16&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:L9">
-    <cfRule type="expression" dxfId="14" priority="61">
+    <cfRule type="expression" dxfId="13" priority="61">
       <formula>AND(L4&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="62">
+    <cfRule type="expression" dxfId="12" priority="62">
       <formula>AND(L4&lt;50%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="63">
+    <cfRule type="expression" dxfId="11" priority="63">
       <formula>AND(L4&gt;=50%, L4&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="64">
+    <cfRule type="expression" dxfId="10" priority="64">
       <formula>AND(L4&gt;=80%, L4&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:L11">
-    <cfRule type="expression" dxfId="10" priority="53">
+    <cfRule type="expression" dxfId="9" priority="53">
       <formula>AND(L8&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="54">
+    <cfRule type="expression" dxfId="8" priority="54">
       <formula>AND(L8&lt;50%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="55">
+    <cfRule type="expression" dxfId="7" priority="55">
       <formula>AND(L8&gt;=50%, L8&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="56">
+    <cfRule type="expression" dxfId="6" priority="56">
       <formula>AND(L8&gt;=80%, L8&lt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:L17">
-    <cfRule type="expression" dxfId="6" priority="33">
-      <formula>AND(L10&gt;=120%)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="34">
-      <formula>AND(L10&lt;50%)</formula>
+    <cfRule type="expression" dxfId="5" priority="36">
+      <formula>AND(L10&gt;=80%, L10&lt;=120%)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="35">
       <formula>AND(L10&gt;=50%, L10&lt;80%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="36">
-      <formula>AND(L10&gt;=80%, L10&lt;=120%)</formula>
+    <cfRule type="expression" dxfId="3" priority="34">
+      <formula>AND(L10&lt;50%)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="33">
+      <formula>AND(L10&gt;=120%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16:L23 G4:G23">
-    <cfRule type="expression" dxfId="2" priority="149">
+    <cfRule type="expression" dxfId="1" priority="149">
       <formula>AND(G4&gt;=120%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="150">
+    <cfRule type="expression" dxfId="0" priority="150">
       <formula>AND(G4&lt;50%)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Refactor portfolio risk analysis to exclude options from VaR/CVaR calculations
- Updated PortfolioRiskAnalyzer to calculate VaR/CVaR using only stocks from specific categories, excluding options.
- Adjusted historical data fetching to focus on VaR-eligible positions.
- Modified risk reporting to reflect changes in VaR/CVaR calculations and added detailed messaging for VaR base.
- Removed options theta summary from risk reporting.
- Updated portfolio risk JSON structure to include positions value for VaR.
- Adjusted risk history and risk report to reflect new calculations and data.
</commit_message>
<xml_diff>
--- a/projects/fetch-ibkr-positions-dashboard.xlsx
+++ b/projects/fetch-ibkr-positions-dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hongkiatkoh/Developer/timeless-workspace/projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96A9371-C299-8145-8C08-C325E094E9C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A879FF4-1134-F942-ABC5-209C5B0CBE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="980" windowWidth="39780" windowHeight="23580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1122,7 +1122,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1146,7 +1146,6 @@
     <xf numFmtId="10" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1155,7 +1154,6 @@
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
@@ -1164,7 +1162,6 @@
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1175,7 +1172,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1183,13 +1179,15 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="9" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -5452,7 +5450,7 @@
   <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="38.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5472,45 +5470,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="37"/>
-      <c r="E1" s="22" t="s">
+      <c r="A1" s="34"/>
+      <c r="E1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="22" t="s">
+      <c r="G1" s="28"/>
+      <c r="H1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="30"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="30"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="28"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="34" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="9">
         <v>1</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="22">
         <f>F4+F11+F19+F22+F23+F20+F21</f>
         <v>449905.70427499997</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="23">
+      <c r="F2" s="23"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="22">
         <f>I4+I11+I19+I22+I23+I20+I21</f>
         <v>560179.43242499989</v>
       </c>
-      <c r="I2" s="24"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="30"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="28"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="42" t="s">
         <v>130</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -5519,44 +5517,44 @@
       <c r="D3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="24" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="24" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="J3" s="32" t="s">
+      <c r="J3" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="K3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="32" t="s">
+      <c r="L3" s="30" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="48">
+      <c r="B4" s="43"/>
+      <c r="C4" s="44">
         <v>0.3</v>
       </c>
       <c r="D4" s="19">
         <f>$G$42*C4</f>
         <v>303025.54100999999</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="25">
         <f>$E$2*C4</f>
         <v>134971.71128249998</v>
       </c>
@@ -5564,11 +5562,11 @@
         <f t="array" ref="F4">SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,GlobalETF!A:A))</f>
         <v>96571.755525</v>
       </c>
-      <c r="G4" s="33">
+      <c r="G4" s="31">
         <f>F4/E4</f>
         <v>0.71549626664266208</v>
       </c>
-      <c r="H4" s="26">
+      <c r="H4" s="25">
         <f>$H$2*C4</f>
         <v>168053.82972749995</v>
       </c>
@@ -5576,38 +5574,38 @@
         <f t="array" ref="I4">SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,GlobalETF!A:A))</f>
         <v>198431.75242500001</v>
       </c>
-      <c r="J4" s="33">
+      <c r="J4" s="31">
         <f>I4/H4</f>
         <v>1.1807630492370094</v>
       </c>
-      <c r="K4" s="42">
+      <c r="K4" s="39">
         <f t="shared" ref="K4:K23" si="0">F4+I4</f>
         <v>295003.50795</v>
       </c>
-      <c r="L4" s="33">
+      <c r="L4" s="31">
         <f t="shared" ref="L4:L23" si="1">K4/D4</f>
         <v>0.97352687488565437</v>
       </c>
-      <c r="M4" s="54">
+      <c r="M4" s="49">
         <f t="shared" ref="M4:M21" si="2">K4/$G$42</f>
         <v>0.29205806246569632</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="49">
+      <c r="C5" s="45">
         <v>0.1</v>
       </c>
       <c r="D5" s="20">
         <f>$D$4*C5</f>
         <v>30302.554101000002</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="26">
         <f>$E$4*C5</f>
         <v>13497.171128249998</v>
       </c>
@@ -5615,11 +5613,11 @@
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"82846")</f>
         <v>9076.0920000000006</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="32">
         <f>F5/E5</f>
         <v>0.6724440191028962</v>
       </c>
-      <c r="H5" s="27">
+      <c r="H5" s="26">
         <f>$H$4*C5</f>
         <v>16805.382972749994</v>
       </c>
@@ -5627,35 +5625,35 @@
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"82846")</f>
         <v>9076.0920000000006</v>
       </c>
-      <c r="J5" s="34">
+      <c r="J5" s="32">
         <f>I5/H5</f>
         <v>0.54007052470728723</v>
       </c>
-      <c r="K5" s="43">
+      <c r="K5" s="40">
         <f t="shared" ref="K5:K7" si="3">F5+I5</f>
         <v>18152.184000000001</v>
       </c>
-      <c r="L5" s="34">
+      <c r="L5" s="32">
         <f t="shared" ref="L5:L7" si="4">K5/D5</f>
         <v>0.59903148558031838</v>
       </c>
-      <c r="M5" s="54"/>
+      <c r="M5" s="49"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="49">
+      <c r="C6" s="45">
         <v>0.2</v>
       </c>
       <c r="D6" s="20">
         <f t="shared" ref="D6:D10" si="5">$D$4*C6</f>
         <v>60605.108202000003</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="26">
         <f t="shared" ref="E6:E10" si="6">$E$4*C6</f>
         <v>26994.342256499996</v>
       </c>
@@ -5663,11 +5661,11 @@
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"DHL")</f>
         <v>0</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="32">
         <f t="shared" ref="G6:G7" si="7">F6/E6</f>
         <v>0</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="26">
         <f t="shared" ref="H6:H10" si="8">$H$4*C6</f>
         <v>33610.765945499988</v>
       </c>
@@ -5675,35 +5673,35 @@
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"DHL")</f>
         <v>56074.2</v>
       </c>
-      <c r="J6" s="34">
+      <c r="J6" s="32">
         <f t="shared" ref="J6:J7" si="9">I6/H6</f>
         <v>1.6683404386238794</v>
       </c>
-      <c r="K6" s="43">
+      <c r="K6" s="40">
         <f t="shared" si="3"/>
         <v>56074.2</v>
       </c>
-      <c r="L6" s="34">
+      <c r="L6" s="32">
         <f t="shared" si="4"/>
         <v>0.92523883982026311</v>
       </c>
-      <c r="M6" s="54"/>
+      <c r="M6" s="49"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C7" s="45">
         <v>0.2</v>
       </c>
       <c r="D7" s="20">
         <f t="shared" si="5"/>
         <v>60605.108202000003</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="26">
         <f t="shared" si="6"/>
         <v>26994.342256499996</v>
       </c>
@@ -5711,11 +5709,11 @@
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"ES3")</f>
         <v>19632.5314</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="32">
         <f t="shared" si="7"/>
         <v>0.72728319191673074</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7" s="26">
         <f t="shared" si="8"/>
         <v>33610.765945499988</v>
       </c>
@@ -5723,35 +5721,35 @@
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"ES3")</f>
         <v>39265.0628</v>
       </c>
-      <c r="J7" s="34">
+      <c r="J7" s="32">
         <f t="shared" si="9"/>
         <v>1.1682287414594621</v>
       </c>
-      <c r="K7" s="43">
+      <c r="K7" s="40">
         <f t="shared" si="3"/>
         <v>58897.5942</v>
       </c>
-      <c r="L7" s="34">
+      <c r="L7" s="32">
         <f t="shared" si="4"/>
         <v>0.97182557621531229</v>
       </c>
-      <c r="M7" s="54"/>
+      <c r="M7" s="49"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="49">
+      <c r="C8" s="45">
         <v>0.25</v>
       </c>
       <c r="D8" s="20">
         <f t="shared" si="5"/>
         <v>75756.385252499997</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="26">
         <f t="shared" si="6"/>
         <v>33742.927820624995</v>
       </c>
@@ -5759,11 +5757,11 @@
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"VWRA")</f>
         <v>34940</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="32">
         <f>F8/E8</f>
         <v>1.0354762392208097</v>
       </c>
-      <c r="H8" s="27">
+      <c r="H8" s="26">
         <f t="shared" si="8"/>
         <v>42013.457431874987</v>
       </c>
@@ -5771,35 +5769,35 @@
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"VWRA")</f>
         <v>52410</v>
       </c>
-      <c r="J8" s="34">
+      <c r="J8" s="32">
         <f>I8/H8</f>
         <v>1.2474574387262236</v>
       </c>
-      <c r="K8" s="43">
+      <c r="K8" s="40">
         <f>F8+I8</f>
         <v>87350</v>
       </c>
-      <c r="L8" s="34">
+      <c r="L8" s="32">
         <f>K8/D8</f>
         <v>1.1530381196100881</v>
       </c>
-      <c r="M8" s="54"/>
+      <c r="M8" s="49"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="C9" s="49">
+      <c r="C9" s="45">
         <v>0.15</v>
       </c>
       <c r="D9" s="20">
         <f t="shared" ref="D9" si="10">$D$4*C9</f>
         <v>45453.831151499995</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="26">
         <f t="shared" ref="E9" si="11">$E$4*C9</f>
         <v>20245.756692374995</v>
       </c>
@@ -5807,11 +5805,11 @@
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"WORLD")</f>
         <v>20620.006874999999</v>
       </c>
-      <c r="G9" s="34">
+      <c r="G9" s="32">
         <f>F9/E9</f>
         <v>1.0184853640351192</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="26">
         <f t="shared" ref="H9" si="12">$H$4*C9</f>
         <v>25208.074459124993</v>
       </c>
@@ -5819,35 +5817,35 @@
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"WORLD")</f>
         <v>25202.230625</v>
       </c>
-      <c r="J9" s="34">
+      <c r="J9" s="32">
         <f>I9/H9</f>
         <v>0.999768176100302</v>
       </c>
-      <c r="K9" s="43">
+      <c r="K9" s="40">
         <f>F9+I9</f>
         <v>45822.237500000003</v>
       </c>
-      <c r="L9" s="34">
+      <c r="L9" s="32">
         <f>K9/D9</f>
         <v>1.0081050670354297</v>
       </c>
-      <c r="M9" s="54"/>
+      <c r="M9" s="49"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="C10" s="49">
+      <c r="C10" s="45">
         <v>0.1</v>
       </c>
       <c r="D10" s="20">
         <f t="shared" si="5"/>
         <v>30302.554101000002</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="26">
         <f t="shared" si="6"/>
         <v>13497.171128249998</v>
       </c>
@@ -5855,11 +5853,11 @@
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"XMME")</f>
         <v>12303.125249999999</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="32">
         <f>F10/E10</f>
         <v>0.91153361938555966</v>
       </c>
-      <c r="H10" s="27">
+      <c r="H10" s="26">
         <f t="shared" si="8"/>
         <v>16805.382972749994</v>
       </c>
@@ -5867,33 +5865,33 @@
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"XMME")</f>
         <v>16404.167000000001</v>
       </c>
-      <c r="J10" s="34">
+      <c r="J10" s="32">
         <f>I10/H10</f>
         <v>0.97612574653011086</v>
       </c>
-      <c r="K10" s="43">
+      <c r="K10" s="40">
         <f>F10+I10</f>
         <v>28707.292249999999</v>
       </c>
-      <c r="L10" s="34">
+      <c r="L10" s="32">
         <f>K10/D10</f>
         <v>0.94735553162671005</v>
       </c>
-      <c r="M10" s="54"/>
+      <c r="M10" s="49"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="B11" s="47"/>
-      <c r="C11" s="48">
+      <c r="B11" s="43"/>
+      <c r="C11" s="44">
         <v>0.3</v>
       </c>
       <c r="D11" s="19">
         <f>$G$42*C11</f>
         <v>303025.54100999999</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="25">
         <f>$E$2*C11</f>
         <v>134971.71128249998</v>
       </c>
@@ -5901,11 +5899,11 @@
         <f t="array" ref="F11">SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,GrowthEngine!A:A))</f>
         <v>99941.65</v>
       </c>
-      <c r="G11" s="33">
+      <c r="G11" s="31">
         <f>F11/E11</f>
         <v>0.74046367976189487</v>
       </c>
-      <c r="H11" s="26">
+      <c r="H11" s="25">
         <f>$H$2*C11</f>
         <v>168053.82972749995</v>
       </c>
@@ -5913,38 +5911,38 @@
         <f t="array" ref="I11">SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,GrowthEngine!A:A))</f>
         <v>107315.65</v>
       </c>
-      <c r="J11" s="33">
+      <c r="J11" s="31">
         <f>I11/H11</f>
         <v>0.63857902062697891</v>
       </c>
-      <c r="K11" s="42">
+      <c r="K11" s="39">
         <f>F11+I11</f>
         <v>207257.3</v>
       </c>
-      <c r="L11" s="34">
+      <c r="L11" s="32">
         <f>K11/D11</f>
         <v>0.68395983820109874</v>
       </c>
-      <c r="M11" s="54">
+      <c r="M11" s="49">
         <f t="shared" si="2"/>
         <v>0.20518795146032962</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="49">
+      <c r="C12" s="45">
         <v>0.25</v>
       </c>
       <c r="D12" s="20">
         <f t="shared" ref="D12:D18" si="13">$D$11*C12</f>
         <v>75756.385252499997</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="26">
         <f t="shared" ref="E12:E18" si="14">$E$11*C12</f>
         <v>33742.927820624995</v>
       </c>
@@ -5952,11 +5950,11 @@
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"CSNDX")</f>
         <v>22122</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="32">
         <f>F12/E12</f>
         <v>0.65560404590849319</v>
       </c>
-      <c r="H12" s="27">
+      <c r="H12" s="26">
         <f t="shared" ref="H12:H18" si="15">$H$11*C12</f>
         <v>42013.457431874987</v>
       </c>
@@ -5964,35 +5962,35 @@
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"CSNDX")</f>
         <v>29496</v>
       </c>
-      <c r="J12" s="34">
+      <c r="J12" s="32">
         <f>I12/H12</f>
         <v>0.70206076345485013</v>
       </c>
-      <c r="K12" s="43">
+      <c r="K12" s="40">
         <f t="shared" si="0"/>
         <v>51618</v>
       </c>
-      <c r="L12" s="34">
+      <c r="L12" s="32">
         <f t="shared" si="1"/>
         <v>0.68136830747605637</v>
       </c>
-      <c r="M12" s="54"/>
+      <c r="M12" s="49"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="C13" s="49">
+      <c r="C13" s="45">
         <v>0.25</v>
       </c>
       <c r="D13" s="20">
         <f t="shared" si="13"/>
         <v>75756.385252499997</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="26">
         <f t="shared" si="14"/>
         <v>33742.927820624995</v>
       </c>
@@ -6000,11 +5998,11 @@
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"EQCH")</f>
         <v>26620.23</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="32">
         <f t="shared" ref="G13:G18" si="16">F13/E13</f>
         <v>0.78891286913545999</v>
       </c>
-      <c r="H13" s="27">
+      <c r="H13" s="26">
         <f t="shared" si="15"/>
         <v>42013.457431874987</v>
       </c>
@@ -6012,35 +6010,35 @@
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"EQCH")</f>
         <v>26620.23</v>
       </c>
-      <c r="J13" s="34">
+      <c r="J13" s="32">
         <f t="shared" ref="J13:J18" si="17">I13/H13</f>
         <v>0.63361198118876139</v>
       </c>
-      <c r="K13" s="43">
+      <c r="K13" s="40">
         <f t="shared" si="0"/>
         <v>53240.46</v>
       </c>
-      <c r="L13" s="34">
+      <c r="L13" s="32">
         <f t="shared" si="1"/>
         <v>0.70278511603407101</v>
       </c>
-      <c r="M13" s="54"/>
+      <c r="M13" s="49"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="C14" s="49">
+      <c r="C14" s="45">
         <v>0.2</v>
       </c>
       <c r="D14" s="20">
         <f t="shared" si="13"/>
         <v>60605.108202000003</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="26">
         <f t="shared" ref="E14" si="18">$E$11*C14</f>
         <v>26994.342256499996</v>
       </c>
@@ -6048,11 +6046,11 @@
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"CBUK")</f>
         <v>21664.17</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="32">
         <f t="shared" ref="G14" si="19">F14/E14</f>
         <v>0.8025448367716187</v>
       </c>
-      <c r="H14" s="27">
+      <c r="H14" s="26">
         <f t="shared" ref="H14" si="20">$H$11*C14</f>
         <v>33610.765945499988</v>
       </c>
@@ -6060,35 +6058,35 @@
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"CBUK")</f>
         <v>21664.17</v>
       </c>
-      <c r="J14" s="34">
+      <c r="J14" s="32">
         <f t="shared" ref="J14" si="21">I14/H14</f>
         <v>0.64456043742438207</v>
       </c>
-      <c r="K14" s="43">
+      <c r="K14" s="40">
         <f t="shared" ref="K14" si="22">F14+I14</f>
         <v>43328.34</v>
       </c>
-      <c r="L14" s="34">
+      <c r="L14" s="32">
         <f t="shared" ref="L14" si="23">K14/D14</f>
         <v>0.71492884486872577</v>
       </c>
-      <c r="M14" s="54"/>
+      <c r="M14" s="49"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="49">
+      <c r="C15" s="45">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="D15" s="20">
         <f t="shared" si="13"/>
         <v>22726.915575749998</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="26">
         <f t="shared" si="14"/>
         <v>10122.878346187497</v>
       </c>
@@ -6096,11 +6094,11 @@
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"HEAL")</f>
         <v>9292.5</v>
       </c>
-      <c r="G15" s="34">
+      <c r="G15" s="32">
         <f t="shared" si="16"/>
         <v>0.91797013479864287</v>
       </c>
-      <c r="H15" s="27">
+      <c r="H15" s="26">
         <f t="shared" si="15"/>
         <v>12604.037229562497</v>
       </c>
@@ -6108,35 +6106,35 @@
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"HEAL")</f>
         <v>9292.5</v>
       </c>
-      <c r="J15" s="34">
+      <c r="J15" s="32">
         <f t="shared" si="17"/>
         <v>0.73726376959635143</v>
       </c>
-      <c r="K15" s="43">
+      <c r="K15" s="40">
         <f t="shared" si="0"/>
         <v>18585</v>
       </c>
-      <c r="L15" s="34">
+      <c r="L15" s="32">
         <f t="shared" si="1"/>
         <v>0.81775285071373738</v>
       </c>
-      <c r="M15" s="54"/>
+      <c r="M15" s="49"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="49">
+      <c r="C16" s="45">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="D16" s="20">
         <f t="shared" si="13"/>
         <v>22726.915575749998</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="26">
         <f>$E$11*C16</f>
         <v>10122.878346187497</v>
       </c>
@@ -6144,11 +6142,11 @@
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"INRA")</f>
         <v>10418.75</v>
       </c>
-      <c r="G16" s="34">
+      <c r="G16" s="32">
         <f>F16/E16</f>
         <v>1.029228016350106</v>
       </c>
-      <c r="H16" s="27">
+      <c r="H16" s="26">
         <f>$H$11*C16</f>
         <v>12604.037229562497</v>
       </c>
@@ -6156,35 +6154,35 @@
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"INRA")</f>
         <v>10418.75</v>
       </c>
-      <c r="J16" s="34">
+      <c r="J16" s="32">
         <f>I16/H16</f>
         <v>0.8266200591317715</v>
       </c>
-      <c r="K16" s="43">
+      <c r="K16" s="40">
         <f>F16+I16</f>
         <v>20837.5</v>
       </c>
-      <c r="L16" s="34">
+      <c r="L16" s="32">
         <f>K16/D16</f>
         <v>0.91686440821885939</v>
       </c>
-      <c r="M16" s="54"/>
+      <c r="M16" s="49"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="49">
+      <c r="C17" s="45">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="D17" s="20">
         <f t="shared" si="13"/>
         <v>22726.915575749998</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="26">
         <f>$E$11*C17</f>
         <v>10122.878346187497</v>
       </c>
@@ -6192,11 +6190,11 @@
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"GRID")</f>
         <v>0</v>
       </c>
-      <c r="G17" s="34">
+      <c r="G17" s="32">
         <f>F17/E17</f>
         <v>0</v>
       </c>
-      <c r="H17" s="27">
+      <c r="H17" s="26">
         <f>$H$11*C17</f>
         <v>12604.037229562497</v>
       </c>
@@ -6204,35 +6202,35 @@
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"GRID")</f>
         <v>0</v>
       </c>
-      <c r="J17" s="34">
+      <c r="J17" s="32">
         <f>I17/H17</f>
         <v>0</v>
       </c>
-      <c r="K17" s="43">
+      <c r="K17" s="40">
         <f>F17+I17</f>
         <v>0</v>
       </c>
-      <c r="L17" s="34">
+      <c r="L17" s="32">
         <f>K17/D17</f>
         <v>0</v>
       </c>
-      <c r="M17" s="54"/>
+      <c r="M17" s="49"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="49">
+      <c r="C18" s="45">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="D18" s="20">
         <f t="shared" si="13"/>
         <v>22726.915575749998</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="26">
         <f t="shared" si="14"/>
         <v>10122.878346187497</v>
       </c>
@@ -6240,11 +6238,11 @@
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"LOCK")</f>
         <v>9824</v>
       </c>
-      <c r="G18" s="34">
+      <c r="G18" s="32">
         <f t="shared" si="16"/>
         <v>0.97047496413902257</v>
       </c>
-      <c r="H18" s="27">
+      <c r="H18" s="26">
         <f t="shared" si="15"/>
         <v>12604.037229562497</v>
       </c>
@@ -6252,35 +6250,35 @@
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"LOCK")</f>
         <v>9824</v>
       </c>
-      <c r="J18" s="34">
+      <c r="J18" s="32">
         <f t="shared" si="17"/>
         <v>0.77943279768787266</v>
       </c>
-      <c r="K18" s="43">
+      <c r="K18" s="40">
         <f t="shared" si="0"/>
         <v>19648</v>
       </c>
-      <c r="L18" s="34">
+      <c r="L18" s="32">
         <f t="shared" si="1"/>
         <v>0.8645255857316928</v>
       </c>
-      <c r="M18" s="54"/>
+      <c r="M18" s="49"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="48">
+      <c r="C19" s="44">
         <v>0.25</v>
       </c>
       <c r="D19" s="19">
         <f>$G$42*C19</f>
         <v>252521.28417499998</v>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="25">
         <f>$E$2*C19</f>
         <v>112476.42606874999</v>
       </c>
@@ -6288,11 +6286,11 @@
         <f t="array" ref="F19">SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,IncomeStrategy!A:A))+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"OPT")-SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"OPT",[1]PositionsHK!F:F,"SPY*")-SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"OPT",[1]PositionsHK!F:F,"QQQ*")+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"FOP")-SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"FOP",[1]PositionsHK!F:F,"SPY*")-SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"FOP",[1]PositionsHK!F:F,"QQQ*")</f>
         <v>86571.87</v>
       </c>
-      <c r="G19" s="33">
+      <c r="G19" s="31">
         <f>F19/E19</f>
         <v>0.76968901863119199</v>
       </c>
-      <c r="H19" s="26">
+      <c r="H19" s="25">
         <f>$H$2*C19</f>
         <v>140044.85810624997</v>
       </c>
@@ -6300,140 +6298,140 @@
         <f t="array" ref="I19">SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,IncomeStrategy!A:A))+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"OPT")-SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"OPT",[1]PositionsAL!F:F,"SPY*")-SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"OPT",[1]PositionsAL!F:F,"QQQ*")+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"FOP")-SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"FOP",[1]PositionsAL!F:F,"SPY*")-SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"FOP",[1]PositionsAL!F:F,"QQQ*")</f>
         <v>62651.45</v>
       </c>
-      <c r="J19" s="33">
+      <c r="J19" s="31">
         <f t="shared" ref="J19:J23" si="24">I19/H19</f>
         <v>0.44736701402108792</v>
       </c>
-      <c r="K19" s="42">
+      <c r="K19" s="39">
         <f t="shared" si="0"/>
         <v>149223.32</v>
       </c>
-      <c r="L19" s="33">
+      <c r="L19" s="31">
         <f t="shared" si="1"/>
         <v>0.59093363352527006</v>
       </c>
-      <c r="M19" s="54">
+      <c r="M19" s="49">
         <f t="shared" si="2"/>
         <v>0.14773340838131752</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="50">
+      <c r="C20" s="44">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="19">
         <f>$G$42*C20</f>
         <v>25252.1284175</v>
       </c>
-      <c r="E20" s="28">
+      <c r="E20" s="25">
         <f>$E$2*C20</f>
         <v>11247.642606875001</v>
       </c>
-      <c r="F20" s="21" cm="1">
+      <c r="F20" s="19" cm="1">
         <f t="array" ref="F20">SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK")-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,GlobalETF!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,GrowthEngine!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,IncomeStrategy!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,Gold!A:A))</f>
         <v>10622.800000000008</v>
       </c>
-      <c r="G20" s="33">
+      <c r="G20" s="31">
         <f t="shared" ref="G20:G21" si="25">F20/E20</f>
         <v>0.94444679398925213</v>
       </c>
-      <c r="H20" s="28">
+      <c r="H20" s="25">
         <f>$H$2*C20</f>
         <v>14004.485810624998</v>
       </c>
-      <c r="I20" s="21" cm="1">
+      <c r="I20" s="19" cm="1">
         <f t="array" ref="I20">SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK")-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,GlobalETF!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,GrowthEngine!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,IncomeStrategy!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,Gold!A:A))</f>
         <v>3581.3399999999965</v>
       </c>
-      <c r="J20" s="35">
+      <c r="J20" s="31">
         <f>I20/H20</f>
         <v>0.25572806088195588</v>
       </c>
-      <c r="K20" s="44">
+      <c r="K20" s="39">
         <f t="shared" si="0"/>
         <v>14204.140000000005</v>
       </c>
-      <c r="L20" s="35">
+      <c r="L20" s="31">
         <f t="shared" si="1"/>
         <v>0.56249278338678099</v>
       </c>
-      <c r="M20" s="54">
+      <c r="M20" s="49">
         <f t="shared" si="2"/>
         <v>1.4062319584669527E-2</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="50">
+      <c r="C21" s="44">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="19">
         <f>$G$42*C21</f>
         <v>25252.1284175</v>
       </c>
-      <c r="E21" s="28">
+      <c r="E21" s="25">
         <f>$E$2*C21</f>
         <v>11247.642606875001</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="19">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"SPY*",[1]PositionsHK!D:D,"OPT")+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"SPY*",[1]PositionsHK!D:D,"FOP")+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"QQQ*",[1]PositionsHK!D:D,"OPT")+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"QQQ*",[1]PositionsHK!D:D,"FOP")</f>
         <v>6391.72</v>
       </c>
-      <c r="G21" s="33">
+      <c r="G21" s="31">
         <f t="shared" si="25"/>
         <v>0.56827196803827407</v>
       </c>
-      <c r="H21" s="28">
+      <c r="H21" s="25">
         <f>H2*C21</f>
         <v>14004.485810624998</v>
       </c>
-      <c r="I21" s="21">
+      <c r="I21" s="19">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"SPY*",[1]PositionsAL!D:D,"OPT")+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"SPY*",[1]PositionsAL!D:D,"FOP")+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"QQQ*",[1]PositionsAL!D:D,"OPT")+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"QQQ*",[1]PositionsAL!D:D,"FOP")</f>
         <v>6391.72</v>
       </c>
-      <c r="J21" s="35">
+      <c r="J21" s="31">
         <f>I21/H21</f>
         <v>0.45640518948226549</v>
       </c>
-      <c r="K21" s="44">
+      <c r="K21" s="39">
         <f t="shared" si="0"/>
         <v>12783.44</v>
       </c>
-      <c r="L21" s="35">
+      <c r="L21" s="31">
         <f t="shared" si="1"/>
         <v>0.50623217927012198</v>
       </c>
-      <c r="M21" s="54">
+      <c r="M21" s="49">
         <f t="shared" si="2"/>
         <v>1.2655804481753049E-2</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="48">
+      <c r="C22" s="44">
         <v>0.05</v>
       </c>
       <c r="D22" s="19">
         <f>$G$42*C22</f>
         <v>50504.256835</v>
       </c>
-      <c r="E22" s="26">
+      <c r="E22" s="25">
         <f>$E$2*C22</f>
         <v>22495.285213750001</v>
       </c>
@@ -6441,11 +6439,11 @@
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"GSD")</f>
         <v>11690.70875</v>
       </c>
-      <c r="G22" s="33">
+      <c r="G22" s="31">
         <f t="shared" ref="G22:G23" si="26">F22/H22</f>
         <v>0.41739157396019605</v>
       </c>
-      <c r="H22" s="26">
+      <c r="H22" s="25">
         <f>$H$2*C22</f>
         <v>28008.971621249995</v>
       </c>
@@ -6453,70 +6451,70 @@
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"GSD")</f>
         <v>0</v>
       </c>
-      <c r="J22" s="33">
+      <c r="J22" s="31">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="K22" s="42">
+      <c r="K22" s="39">
         <f t="shared" si="0"/>
         <v>11690.70875</v>
       </c>
-      <c r="L22" s="33">
+      <c r="L22" s="31">
         <f t="shared" si="1"/>
         <v>0.23147967087594509</v>
       </c>
-      <c r="M22" s="54">
+      <c r="M22" s="49">
         <f>K22/$G$42</f>
         <v>1.1573983543797255E-2</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="48">
+      <c r="C23" s="44">
         <v>0.05</v>
       </c>
       <c r="D23" s="19">
         <f>$G$42*C23</f>
         <v>50504.256835</v>
       </c>
-      <c r="E23" s="29">
+      <c r="E23" s="27">
         <f>$E$2*C23</f>
         <v>22495.285213750001</v>
       </c>
-      <c r="F23" s="51" t="str">
+      <c r="F23" s="46" t="str">
         <f>[1]Summary!$C$2</f>
         <v>$138,115.20</v>
       </c>
-      <c r="G23" s="36">
+      <c r="G23" s="33">
         <f t="shared" si="26"/>
         <v>4.9311057138282806</v>
       </c>
-      <c r="H23" s="29">
+      <c r="H23" s="27">
         <f>$H$2*C23</f>
         <v>28008.971621249995</v>
       </c>
-      <c r="I23" s="51" t="str">
+      <c r="I23" s="46" t="str">
         <f>[1]Summary!$C$3</f>
         <v>$181,807.52</v>
       </c>
-      <c r="J23" s="36">
+      <c r="J23" s="33">
         <f t="shared" si="24"/>
         <v>6.4910458855285249</v>
       </c>
-      <c r="K23" s="45">
+      <c r="K23" s="41">
         <f t="shared" si="0"/>
         <v>319922.71999999997</v>
       </c>
-      <c r="L23" s="36">
+      <c r="L23" s="33">
         <f t="shared" si="1"/>
         <v>6.3345694016487348</v>
       </c>
-      <c r="M23" s="54">
+      <c r="M23" s="49">
         <f>K23/$G$42</f>
         <v>0.31672847008243676</v>
       </c>
@@ -6551,10 +6549,10 @@
         <v>126</v>
       </c>
       <c r="H41" s="12"/>
-      <c r="J41" s="53" t="s">
+      <c r="J41" s="48" t="s">
         <v>180</v>
       </c>
-      <c r="K41" s="53" t="s">
+      <c r="K41" s="48" t="s">
         <v>181</v>
       </c>
     </row>
@@ -6567,7 +6565,7 @@
       <c r="J42" t="s">
         <v>17</v>
       </c>
-      <c r="K42" s="52">
+      <c r="K42" s="47">
         <v>365115.64</v>
       </c>
     </row>
@@ -6582,7 +6580,7 @@
       <c r="J43" t="s">
         <v>133</v>
       </c>
-      <c r="K43" s="52">
+      <c r="K43" s="47">
         <v>127769.98974999999</v>
       </c>
     </row>
@@ -6595,7 +6593,7 @@
       <c r="J44" t="s">
         <v>13</v>
       </c>
-      <c r="K44" s="52">
+      <c r="K44" s="47">
         <v>99402.54</v>
       </c>
     </row>
@@ -6610,7 +6608,7 @@
       <c r="J45" t="s">
         <v>15</v>
       </c>
-      <c r="K45" s="52">
+      <c r="K45" s="47">
         <v>70588.302949999998</v>
       </c>
     </row>
@@ -6623,7 +6621,7 @@
       <c r="J46" t="s">
         <v>182</v>
       </c>
-      <c r="K46" s="52">
+      <c r="K46" s="47">
         <v>18152.184000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Add auto-categorization script for uncategorized IBKR positions
</commit_message>
<xml_diff>
--- a/projects/fetch-ibkr-positions-dashboard.xlsx
+++ b/projects/fetch-ibkr-positions-dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hongkiatkoh/Developer/timeless-workspace/projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A879FF4-1134-F942-ABC5-209C5B0CBE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC20290E-CB6B-7A46-8978-7F1A2CA703F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="980" windowWidth="39780" windowHeight="23580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="980" windowWidth="18980" windowHeight="22080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -681,18 +681,9 @@
     <t>CHF</t>
   </si>
   <si>
-    <t>Nasdaq (CSNDX)</t>
-  </si>
-  <si>
     <t>Nasdaq (EQCH, hedged)</t>
   </si>
   <si>
-    <t>Energy (GRID)</t>
-  </si>
-  <si>
-    <t>China Tech (CBUK, unhedged)</t>
-  </si>
-  <si>
     <t>Global Triads (the strategic core)</t>
   </si>
   <si>
@@ -868,6 +859,15 @@
   </si>
   <si>
     <t>MSCI World Index, CHF-hedged, Large &amp; Mid-Cap stocks 23 developed countries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">China Tech (CBUK, unhedged) </t>
+  </si>
+  <si>
+    <t>Nasdaq (CSNDX), what about SOXX?</t>
+  </si>
+  <si>
+    <t>Energy (GRDU) - need to change scripts</t>
   </si>
 </sst>
 </file>
@@ -1596,10 +1596,10 @@
                   <c:v>252521.28417499998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25252.1284175</c:v>
+                  <c:v>30302.554100999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25252.1284175</c:v>
+                  <c:v>20201.702733999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>50504.256835</c:v>
@@ -5450,12 +5450,12 @@
   <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="38.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="61" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -5544,7 +5544,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="44">
@@ -5881,7 +5881,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B11" s="43"/>
       <c r="C11" s="44">
@@ -5930,7 +5930,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="37" t="s">
-        <v>134</v>
+        <v>195</v>
       </c>
       <c r="B12" s="43" t="s">
         <v>17</v>
@@ -5978,7 +5978,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B13" s="43" t="s">
         <v>133</v>
@@ -6026,7 +6026,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="37" t="s">
-        <v>137</v>
+        <v>194</v>
       </c>
       <c r="B14" s="43" t="s">
         <v>133</v>
@@ -6170,7 +6170,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="37" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="B17" s="43" t="s">
         <v>17</v>
@@ -6266,7 +6266,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="36" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B19" s="43" t="s">
         <v>17</v>
@@ -6317,21 +6317,21 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="36" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B20" s="50" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="44">
-        <v>2.5000000000000001E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D20" s="19">
         <f>$G$42*C20</f>
-        <v>25252.1284175</v>
+        <v>30302.554100999998</v>
       </c>
       <c r="E20" s="25">
         <f>$E$2*C20</f>
-        <v>11247.642606875001</v>
+        <v>13497.171128249998</v>
       </c>
       <c r="F20" s="19" cm="1">
         <f t="array" ref="F20">SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK")-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,GlobalETF!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,GrowthEngine!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,IncomeStrategy!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,Gold!A:A))</f>
@@ -6339,11 +6339,11 @@
       </c>
       <c r="G20" s="31">
         <f t="shared" ref="G20:G21" si="25">F20/E20</f>
-        <v>0.94444679398925213</v>
+        <v>0.78703899499104357</v>
       </c>
       <c r="H20" s="25">
         <f>$H$2*C20</f>
-        <v>14004.485810624998</v>
+        <v>16805.382972749998</v>
       </c>
       <c r="I20" s="19" cm="1">
         <f t="array" ref="I20">SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK")-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,GlobalETF!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,GrowthEngine!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,IncomeStrategy!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,Gold!A:A))</f>
@@ -6351,7 +6351,7 @@
       </c>
       <c r="J20" s="31">
         <f>I20/H20</f>
-        <v>0.25572806088195588</v>
+        <v>0.2131067174016299</v>
       </c>
       <c r="K20" s="39">
         <f t="shared" si="0"/>
@@ -6359,7 +6359,7 @@
       </c>
       <c r="L20" s="31">
         <f t="shared" si="1"/>
-        <v>0.56249278338678099</v>
+        <v>0.46874398615565088</v>
       </c>
       <c r="M20" s="49">
         <f t="shared" si="2"/>
@@ -6368,21 +6368,21 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="36" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B21" s="50" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="44">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D21" s="19">
         <f>$G$42*C21</f>
-        <v>25252.1284175</v>
+        <v>20201.702733999999</v>
       </c>
       <c r="E21" s="25">
         <f>$E$2*C21</f>
-        <v>11247.642606875001</v>
+        <v>8998.1140854999994</v>
       </c>
       <c r="F21" s="19">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"SPY*",[1]PositionsHK!D:D,"OPT")+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"SPY*",[1]PositionsHK!D:D,"FOP")+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"QQQ*",[1]PositionsHK!D:D,"OPT")+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"QQQ*",[1]PositionsHK!D:D,"FOP")</f>
@@ -6390,11 +6390,11 @@
       </c>
       <c r="G21" s="31">
         <f t="shared" si="25"/>
-        <v>0.56827196803827407</v>
+        <v>0.71033996004784272</v>
       </c>
       <c r="H21" s="25">
         <f>H2*C21</f>
-        <v>14004.485810624998</v>
+        <v>11203.588648499997</v>
       </c>
       <c r="I21" s="19">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"SPY*",[1]PositionsAL!D:D,"OPT")+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"SPY*",[1]PositionsAL!D:D,"FOP")+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"QQQ*",[1]PositionsAL!D:D,"OPT")+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"QQQ*",[1]PositionsAL!D:D,"FOP")</f>
@@ -6402,7 +6402,7 @@
       </c>
       <c r="J21" s="31">
         <f>I21/H21</f>
-        <v>0.45640518948226549</v>
+        <v>0.5705064868528319</v>
       </c>
       <c r="K21" s="39">
         <f t="shared" si="0"/>
@@ -6410,7 +6410,7 @@
       </c>
       <c r="L21" s="31">
         <f t="shared" si="1"/>
-        <v>0.50623217927012198</v>
+        <v>0.63279022408765251</v>
       </c>
       <c r="M21" s="49">
         <f t="shared" si="2"/>
@@ -6419,7 +6419,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="36" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B22" s="43" t="s">
         <v>15</v>
@@ -6470,7 +6470,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="35" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B23" s="43" t="s">
         <v>17</v>
@@ -6550,10 +6550,10 @@
       </c>
       <c r="H41" s="12"/>
       <c r="J41" s="48" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K41" s="48" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" spans="7:11" x14ac:dyDescent="0.2">
@@ -6619,7 +6619,7 @@
       </c>
       <c r="H46" s="12"/>
       <c r="J46" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="K46" s="47">
         <v>18152.184000000001</v>
@@ -6691,7 +6691,7 @@
       </c>
       <c r="B55" s="14">
         <f>D20</f>
-        <v>25252.1284175</v>
+        <v>30302.554100999998</v>
       </c>
       <c r="C55" s="15">
         <f>K20</f>
@@ -6707,7 +6707,7 @@
       </c>
       <c r="B56" s="14">
         <f>D21</f>
-        <v>25252.1284175</v>
+        <v>20201.702733999999</v>
       </c>
       <c r="C56" s="15">
         <f>K21</f>
@@ -6899,19 +6899,19 @@
         <v>130</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -6922,16 +6922,16 @@
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D2" s="1">
         <v>3.8E-3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G2" s="1">
         <v>-6.3500000000000001E-2</v>
@@ -6945,19 +6945,19 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -6968,19 +6968,19 @@
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -6991,65 +6991,65 @@
         <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>133</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>133</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -7086,7 +7086,7 @@
         <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
@@ -7109,42 +7109,42 @@
         <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>133</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -7157,10 +7157,10 @@
         <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -7173,26 +7173,26 @@
         <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -7205,10 +7205,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>

</xml_diff>

<commit_message>
Update IBKR positions dashboard spreadsheet
</commit_message>
<xml_diff>
--- a/projects/fetch-ibkr-positions-dashboard.xlsx
+++ b/projects/fetch-ibkr-positions-dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hongkiatkoh/Developer/timeless-workspace/projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F866631-A533-E549-80A7-C589A4BF845D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35C69D2-CA22-0843-BFF6-B6E4BE9485E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="1020" windowWidth="30780" windowHeight="22080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4120" yWindow="3000" windowWidth="38000" windowHeight="22840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -277,7 +277,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="208">
   <si>
     <t>HK</t>
   </si>
@@ -303,9 +303,6 @@
     <t>Actual %</t>
   </si>
   <si>
-    <t>Security (LOCK)</t>
-  </si>
-  <si>
     <t>Energy (INRA)</t>
   </si>
   <si>
@@ -639,12 +636,6 @@
     <t>Diversification: High liquidity and low correlation to traditional stocks.</t>
   </si>
   <si>
-    <t>Biotic (HEAL)</t>
-  </si>
-  <si>
-    <t>82846 (china etf)</t>
-  </si>
-  <si>
     <t>DHL (dividend)</t>
   </si>
   <si>
@@ -904,6 +895,12 @@
   </si>
   <si>
     <t>XMME (EM, unhedged) - india 18%</t>
+  </si>
+  <si>
+    <t>China Robotics (2807.HK)</t>
+  </si>
+  <si>
+    <t>China CSI300 (82846)</t>
   </si>
 </sst>
 </file>
@@ -917,7 +914,7 @@
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1030,6 +1027,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1169,7 +1173,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1252,6 +1256,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1573,25 +1580,25 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>400088.85820800002</c:v>
+                  <c:v>502604.56847499998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>250055.53638000001</c:v>
+                  <c:v>201041.82738999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200044.42910400001</c:v>
+                  <c:v>201041.82738999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30006.664365599998</c:v>
+                  <c:v>30156.274108499998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20004.442910400001</c:v>
+                  <c:v>20104.182739</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50011.107276000002</c:v>
+                  <c:v>50260.456847499998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50011.107276000002</c:v>
+                  <c:v>50260.456847499998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1720,25 +1727,25 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>307032.23610000004</c:v>
+                  <c:v>385495.53649999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>210651.57989999998</c:v>
+                  <c:v>212281.10440000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69449.5</c:v>
+                  <c:v>104807.22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14103.950000000012</c:v>
+                  <c:v>14637.170000000056</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14935.52</c:v>
+                  <c:v>13792.48</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18352.29952</c:v>
+                  <c:v>46333.246050000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>365697.06</c:v>
+                  <c:v>227862.38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2171,10 +2178,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.63438415992091457</c:v>
+                  <c:v>0.77331843531448707</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.36561584007908537</c:v>
+                  <c:v>0.2266815646855129</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3216,8 +3223,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.22452504317789299"/>
-                  <c:y val="0.18025751072961374"/>
+                  <c:x val="-0.21761658031088082"/>
+                  <c:y val="8.15450643776824E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -3271,8 +3278,8 @@
               <c:idx val="7"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.19861830742659758"/>
-                  <c:y val="-0.21030042918454944"/>
+                  <c:x val="-3.6269294058449947E-2"/>
+                  <c:y val="-0.1630901287553648"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -3326,8 +3333,8 @@
               <c:idx val="15"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.10880829015544041"/>
-                  <c:y val="1.7167381974248771E-2"/>
+                  <c:x val="1.2052137550602785E-2"/>
+                  <c:y val="-4.7210300429184469E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -3384,37 +3391,8 @@
               <c:idx val="16"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-8.635578583765121E-3"/>
-                  <c:y val="3.8568821601162519E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout>
-                    <c:manualLayout>
-                      <c:w val="0.27663198835896807"/>
-                      <c:h val="0.11763948497854078"/>
-                    </c:manualLayout>
-                  </c15:layout>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-5B79-724A-AB6E-048CA154099D}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="17"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-1.3035235880489042E-2"/>
-                  <c:y val="-2.575107296137339E-2"/>
+                  <c:x val="3.184416566573246E-3"/>
+                  <c:y val="1.7109594133351277E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -3457,8 +3435,66 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.26953367875647666"/>
-                      <c:h val="0.11575107296137339"/>
+                      <c:w val="0.27663196091452424"/>
+                      <c:h val="7.4721030042918454E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-5B79-724A-AB6E-048CA154099D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.0442991708264583E-7"/>
+                  <c:y val="-1.9313135750735101E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.26953372545299309"/>
+                      <c:h val="8.5708154506437761E-2"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -3471,10 +3507,36 @@
               <c:idx val="18"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-6.9084628670120912E-2"/>
-                  <c:y val="-7.2961373390557943E-2"/>
+                  <c:x val="0.18072289156626506"/>
+                  <c:y val="-4.2918454935622317E-3"/>
                 </c:manualLayout>
               </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="bg1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
               <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -3493,8 +3555,8 @@
               <c:idx val="19"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.22279819944786694"/>
-                  <c:y val="0.11587982832618025"/>
+                  <c:x val="0.17789319081228835"/>
+                  <c:y val="0.20600858369098712"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -3621,25 +3683,25 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.30696404541251054</c:v>
+                  <c:v>0.38349784371207413</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.21060479498830281</c:v>
+                  <c:v>0.21118103347538422</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.9434075531185399E-2</c:v>
+                  <c:v>0.10426409405509932</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.4100817566549266E-2</c:v>
+                  <c:v>1.4561318099845448E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.4932202878026915E-2</c:v>
+                  <c:v>1.3721005403760124E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.8348223544339667E-2</c:v>
+                  <c:v>4.6093140568324004E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.36561584007908537</c:v>
+                  <c:v>0.2266815646855129</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5955,8 +6017,8 @@
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>1041400</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
@@ -5985,14 +6047,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>1174750</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
@@ -6055,7 +6117,7 @@
             <v>EQCH</v>
           </cell>
           <cell r="V2">
-            <v>25592.961749999999</v>
+            <v>25722.762999999999</v>
           </cell>
         </row>
         <row r="3">
@@ -6066,7 +6128,7 @@
             <v>WORLD</v>
           </cell>
           <cell r="V3">
-            <v>29799.770325000001</v>
+            <v>34494.157499999987</v>
           </cell>
         </row>
         <row r="4">
@@ -6077,7 +6139,7 @@
             <v>XMME</v>
           </cell>
           <cell r="V4">
-            <v>12636.9918</v>
+            <v>25692.466799999998</v>
           </cell>
         </row>
         <row r="5">
@@ -6088,7 +6150,7 @@
             <v>82846</v>
           </cell>
           <cell r="V5">
-            <v>9169.4423999999999</v>
+            <v>13657.116</v>
           </cell>
         </row>
         <row r="6">
@@ -6099,7 +6161,7 @@
             <v>CBUK</v>
           </cell>
           <cell r="V6">
-            <v>20836.428199999998</v>
+            <v>20772.2592</v>
           </cell>
         </row>
         <row r="7">
@@ -6110,7 +6172,7 @@
             <v>ES3</v>
           </cell>
           <cell r="V7">
-            <v>19585.661499999998</v>
+            <v>31638.751199999999</v>
           </cell>
         </row>
         <row r="8">
@@ -6121,7 +6183,7 @@
             <v>GSD</v>
           </cell>
           <cell r="V8">
-            <v>13764.22464</v>
+            <v>23166.623025000001</v>
           </cell>
         </row>
         <row r="9">
@@ -6132,7 +6194,7 @@
             <v>BITO</v>
           </cell>
           <cell r="V9">
-            <v>950</v>
+            <v>936</v>
           </cell>
         </row>
         <row r="10">
@@ -6143,7 +6205,7 @@
             <v>CELH</v>
           </cell>
           <cell r="V10">
-            <v>2234</v>
+            <v>2416</v>
           </cell>
         </row>
         <row r="11">
@@ -6154,7 +6216,7 @@
             <v>CHA</v>
           </cell>
           <cell r="V11">
-            <v>1031</v>
+            <v>1034</v>
           </cell>
         </row>
         <row r="12">
@@ -6165,7 +6227,7 @@
             <v>CSNDX</v>
           </cell>
           <cell r="V12">
-            <v>21201</v>
+            <v>21465</v>
           </cell>
         </row>
         <row r="13">
@@ -6173,10 +6235,10 @@
             <v>STK</v>
           </cell>
           <cell r="F13" t="str">
-            <v>GRDU</v>
+            <v>GOOGL</v>
           </cell>
           <cell r="V13">
-            <v>4846.3999999999996</v>
+            <v>31498</v>
           </cell>
         </row>
         <row r="14">
@@ -6184,10 +6246,10 @@
             <v>STK</v>
           </cell>
           <cell r="F14" t="str">
-            <v>HEAL</v>
+            <v>GRDU</v>
           </cell>
           <cell r="V14">
-            <v>9047.5</v>
+            <v>4860</v>
           </cell>
         </row>
         <row r="15">
@@ -6195,10 +6257,10 @@
             <v>STK</v>
           </cell>
           <cell r="F15" t="str">
-            <v>INRA</v>
+            <v>HEAL</v>
           </cell>
           <cell r="V15">
-            <v>10470</v>
+            <v>9140</v>
           </cell>
         </row>
         <row r="16">
@@ -6206,10 +6268,10 @@
             <v>STK</v>
           </cell>
           <cell r="F16" t="str">
-            <v>LKNCY</v>
+            <v>INRA</v>
           </cell>
           <cell r="V16">
-            <v>3645</v>
+            <v>10733.03</v>
           </cell>
         </row>
         <row r="17">
@@ -6217,10 +6279,10 @@
             <v>STK</v>
           </cell>
           <cell r="F17" t="str">
-            <v>LOCK</v>
+            <v>LKNCY</v>
           </cell>
           <cell r="V17">
-            <v>9798</v>
+            <v>3890</v>
           </cell>
         </row>
         <row r="18">
@@ -6228,10 +6290,10 @@
             <v>STK</v>
           </cell>
           <cell r="F18" t="str">
-            <v>ORCL</v>
+            <v>LOCK</v>
           </cell>
           <cell r="V18">
-            <v>16014</v>
+            <v>9870</v>
           </cell>
         </row>
         <row r="19">
@@ -6239,10 +6301,10 @@
             <v>STK</v>
           </cell>
           <cell r="F19" t="str">
-            <v>SE</v>
+            <v>ORCL</v>
           </cell>
           <cell r="V19">
-            <v>2134.8000000000002</v>
+            <v>14808</v>
           </cell>
         </row>
         <row r="20">
@@ -6250,21 +6312,21 @@
             <v>STK</v>
           </cell>
           <cell r="F20" t="str">
-            <v>VWRA</v>
+            <v>SE</v>
           </cell>
           <cell r="V20">
-            <v>34984</v>
+            <v>2300</v>
           </cell>
         </row>
         <row r="21">
           <cell r="D21" t="str">
-            <v>OPT</v>
+            <v>STK</v>
           </cell>
           <cell r="F21" t="str">
-            <v>QQQ   261218P00560000</v>
+            <v>VWRA</v>
           </cell>
           <cell r="V21">
-            <v>6179.42</v>
+            <v>35320</v>
           </cell>
         </row>
         <row r="22">
@@ -6272,10 +6334,10 @@
             <v>OPT</v>
           </cell>
           <cell r="F22" t="str">
-            <v>SPY   261218P00620000</v>
+            <v>QQQ   261218P00560000</v>
           </cell>
           <cell r="V22">
-            <v>4721</v>
+            <v>5729.78</v>
           </cell>
         </row>
         <row r="23">
@@ -6283,10 +6345,10 @@
             <v>OPT</v>
           </cell>
           <cell r="F23" t="str">
-            <v>GOOGL 260227P00310000</v>
+            <v>SPY   261218P00620000</v>
           </cell>
           <cell r="V23">
-            <v>-925</v>
+            <v>4307.18</v>
           </cell>
         </row>
         <row r="24">
@@ -6294,10 +6356,10 @@
             <v>OPT</v>
           </cell>
           <cell r="F24" t="str">
-            <v>GOOGL 260227C00370000</v>
+            <v>GOOGL 260306C00325000</v>
           </cell>
           <cell r="V24">
-            <v>-6.69</v>
+            <v>-375</v>
           </cell>
         </row>
         <row r="25">
@@ -6305,10 +6367,10 @@
             <v>OPT</v>
           </cell>
           <cell r="F25" t="str">
-            <v>IWM   260227P00257000</v>
+            <v>GOOGL 260327P00300000</v>
           </cell>
           <cell r="V25">
-            <v>-562</v>
+            <v>-635</v>
           </cell>
         </row>
         <row r="26">
@@ -6316,10 +6378,10 @@
             <v>OPT</v>
           </cell>
           <cell r="F26" t="str">
-            <v>IWM   260227C00277000</v>
+            <v>IWM   260227P00257000</v>
           </cell>
           <cell r="V26">
-            <v>-101</v>
+            <v>-234</v>
           </cell>
         </row>
         <row r="27">
@@ -6327,10 +6389,10 @@
             <v>OPT</v>
           </cell>
           <cell r="F27" t="str">
-            <v>NVDA  260227P00175000</v>
+            <v>IWM   260227C00277000</v>
           </cell>
           <cell r="V27">
-            <v>-950</v>
+            <v>-15</v>
           </cell>
         </row>
         <row r="28">
@@ -6338,10 +6400,10 @@
             <v>OPT</v>
           </cell>
           <cell r="F28" t="str">
-            <v>ORCL  260227P00140000</v>
+            <v>NVDA  260227P00175000</v>
           </cell>
           <cell r="V28">
-            <v>-144.01</v>
+            <v>-301</v>
           </cell>
         </row>
         <row r="29">
@@ -6349,10 +6411,10 @@
             <v>OPT</v>
           </cell>
           <cell r="F29" t="str">
-            <v>ORCL  260227C00190000</v>
+            <v>ORCL  260227P00140000</v>
           </cell>
           <cell r="V29">
-            <v>-51.85</v>
+            <v>-246.5</v>
           </cell>
         </row>
         <row r="30">
@@ -6360,10 +6422,10 @@
             <v>OPT</v>
           </cell>
           <cell r="F30" t="str">
-            <v>QQQ   261218P00425000</v>
+            <v>ORCL  260306C00165000</v>
           </cell>
           <cell r="V30">
-            <v>-1696.66</v>
+            <v>-167</v>
           </cell>
         </row>
         <row r="31">
@@ -6371,10 +6433,10 @@
             <v>OPT</v>
           </cell>
           <cell r="F31" t="str">
-            <v>SMH   260227P00377500</v>
+            <v>QQQ   261218P00425000</v>
           </cell>
           <cell r="V31">
-            <v>-830</v>
+            <v>-1561.72</v>
           </cell>
         </row>
         <row r="32">
@@ -6382,10 +6444,10 @@
             <v>OPT</v>
           </cell>
           <cell r="F32" t="str">
-            <v>SMH   260227C00437500</v>
+            <v>SMH   260227P00377500</v>
           </cell>
           <cell r="V32">
-            <v>-612</v>
+            <v>-290.22000000000003</v>
           </cell>
         </row>
         <row r="33">
@@ -6393,10 +6455,21 @@
             <v>OPT</v>
           </cell>
           <cell r="F33" t="str">
+            <v>SMH   260227C00437500</v>
+          </cell>
+          <cell r="V33">
+            <v>-352</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="D34" t="str">
+            <v>OPT</v>
+          </cell>
+          <cell r="F34" t="str">
             <v>SPY   261218P00505000</v>
           </cell>
-          <cell r="V33">
-            <v>-1736</v>
+          <cell r="V34">
+            <v>-1579</v>
           </cell>
         </row>
       </sheetData>
@@ -6420,7 +6493,7 @@
             <v>EQCH</v>
           </cell>
           <cell r="V2">
-            <v>25592.961749999999</v>
+            <v>25722.762999999999</v>
           </cell>
         </row>
         <row r="3">
@@ -6431,7 +6504,7 @@
             <v>WORLD</v>
           </cell>
           <cell r="V3">
-            <v>25215.190275000001</v>
+            <v>41392.988999999987</v>
           </cell>
         </row>
         <row r="4">
@@ -6442,7 +6515,7 @@
             <v>XMME</v>
           </cell>
           <cell r="V4">
-            <v>16849.322400000001</v>
+            <v>42820.777999999998</v>
           </cell>
         </row>
         <row r="5">
@@ -6453,7 +6526,7 @@
             <v>82846</v>
           </cell>
           <cell r="V5">
-            <v>9169.4423999999999</v>
+            <v>9104.7440000000006</v>
           </cell>
         </row>
         <row r="6">
@@ -6464,7 +6537,7 @@
             <v>CBUK</v>
           </cell>
           <cell r="V6">
-            <v>20836.428199999998</v>
+            <v>20772.2592</v>
           </cell>
         </row>
         <row r="7">
@@ -6475,7 +6548,7 @@
             <v>DHL</v>
           </cell>
           <cell r="V7">
-            <v>57975.091999999997</v>
+            <v>58846.094999999987</v>
           </cell>
         </row>
         <row r="8">
@@ -6486,7 +6559,7 @@
             <v>ES3</v>
           </cell>
           <cell r="V8">
-            <v>39171.322999999997</v>
+            <v>39548.438999999998</v>
           </cell>
         </row>
         <row r="9">
@@ -6497,7 +6570,7 @@
             <v>GSD</v>
           </cell>
           <cell r="V9">
-            <v>4588.0748800000001</v>
+            <v>23166.623025000001</v>
           </cell>
         </row>
         <row r="10">
@@ -6508,7 +6581,7 @@
             <v>BITO</v>
           </cell>
           <cell r="V10">
-            <v>2850</v>
+            <v>2808</v>
           </cell>
         </row>
         <row r="11">
@@ -6519,7 +6592,7 @@
             <v>CSNDX</v>
           </cell>
           <cell r="V11">
-            <v>28268</v>
+            <v>28620</v>
           </cell>
         </row>
         <row r="12">
@@ -6530,7 +6603,7 @@
             <v>GOOGL</v>
           </cell>
           <cell r="V12">
-            <v>30572</v>
+            <v>31498</v>
           </cell>
         </row>
         <row r="13">
@@ -6541,7 +6614,7 @@
             <v>GRDU</v>
           </cell>
           <cell r="V13">
-            <v>4846.3999999999996</v>
+            <v>4860</v>
           </cell>
         </row>
         <row r="14">
@@ -6552,7 +6625,7 @@
             <v>HEAL</v>
           </cell>
           <cell r="V14">
-            <v>9047.5</v>
+            <v>9140</v>
           </cell>
         </row>
         <row r="15">
@@ -6563,7 +6636,7 @@
             <v>IBKR</v>
           </cell>
           <cell r="V15">
-            <v>1259.1500000000001</v>
+            <v>1253.17</v>
           </cell>
         </row>
         <row r="16">
@@ -6574,7 +6647,7 @@
             <v>INRA</v>
           </cell>
           <cell r="V16">
-            <v>10470</v>
+            <v>10733.03</v>
           </cell>
         </row>
         <row r="17">
@@ -6585,7 +6658,7 @@
             <v>JPM</v>
           </cell>
           <cell r="V17">
-            <v>30255</v>
+            <v>31079</v>
           </cell>
         </row>
         <row r="18">
@@ -6596,7 +6669,7 @@
             <v>LOCK</v>
           </cell>
           <cell r="V18">
-            <v>9798</v>
+            <v>9870</v>
           </cell>
         </row>
         <row r="19">
@@ -6607,7 +6680,7 @@
             <v>VWRA</v>
           </cell>
           <cell r="V19">
-            <v>52476</v>
+            <v>52980</v>
           </cell>
         </row>
         <row r="20">
@@ -6618,7 +6691,7 @@
             <v>QQQ   261218P00560000</v>
           </cell>
           <cell r="V20">
-            <v>6179.42</v>
+            <v>5729.78</v>
           </cell>
         </row>
         <row r="21">
@@ -6629,7 +6702,7 @@
             <v>SPY   261218P00620000</v>
           </cell>
           <cell r="V21">
-            <v>4721</v>
+            <v>4307.18</v>
           </cell>
         </row>
         <row r="22">
@@ -6637,10 +6710,10 @@
             <v>OPT</v>
           </cell>
           <cell r="F22" t="str">
-            <v>GOOGL 260220P00315000</v>
+            <v>GOOGL 260304P00295000</v>
           </cell>
           <cell r="V22">
-            <v>-1064.44</v>
+            <v>-140.91</v>
           </cell>
         </row>
         <row r="23">
@@ -6648,10 +6721,10 @@
             <v>OPT</v>
           </cell>
           <cell r="F23" t="str">
-            <v>GOOGL 260227C00345000</v>
+            <v>IWM   260227P00257000</v>
           </cell>
           <cell r="V23">
-            <v>-24</v>
+            <v>-234</v>
           </cell>
         </row>
         <row r="24">
@@ -6659,10 +6732,10 @@
             <v>OPT</v>
           </cell>
           <cell r="F24" t="str">
-            <v>IWM   260227P00257000</v>
+            <v>IWM   260227C00277000</v>
           </cell>
           <cell r="V24">
-            <v>-562</v>
+            <v>-15</v>
           </cell>
         </row>
         <row r="25">
@@ -6670,10 +6743,10 @@
             <v>OPT</v>
           </cell>
           <cell r="F25" t="str">
-            <v>IWM   260227C00277000</v>
+            <v>JPM   260327C00325000</v>
           </cell>
           <cell r="V25">
-            <v>-101</v>
+            <v>-427.93</v>
           </cell>
         </row>
         <row r="26">
@@ -6681,10 +6754,10 @@
             <v>OPT</v>
           </cell>
           <cell r="F26" t="str">
-            <v>JPM   260227C00340000</v>
+            <v>QQQ   261218P00425000</v>
           </cell>
           <cell r="V26">
-            <v>-15.51</v>
+            <v>-1561.72</v>
           </cell>
         </row>
         <row r="27">
@@ -6692,10 +6765,10 @@
             <v>OPT</v>
           </cell>
           <cell r="F27" t="str">
-            <v>QQQ   261218P00425000</v>
+            <v>SMH   260227P00377500</v>
           </cell>
           <cell r="V27">
-            <v>-1696.66</v>
+            <v>-290.22000000000003</v>
           </cell>
         </row>
         <row r="28">
@@ -6703,10 +6776,10 @@
             <v>OPT</v>
           </cell>
           <cell r="F28" t="str">
-            <v>SMH   260227P00377500</v>
+            <v>SMH   260227C00437500</v>
           </cell>
           <cell r="V28">
-            <v>-830</v>
+            <v>-352</v>
           </cell>
         </row>
         <row r="29">
@@ -6714,37 +6787,26 @@
             <v>OPT</v>
           </cell>
           <cell r="F29" t="str">
-            <v>SMH   260227C00437500</v>
+            <v>SPY   261218P00505000</v>
           </cell>
           <cell r="V29">
-            <v>-612</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="D30" t="str">
-            <v>OPT</v>
-          </cell>
-          <cell r="F30" t="str">
-            <v>SPY   261218P00505000</v>
-          </cell>
-          <cell r="V30">
-            <v>-1736</v>
+            <v>-1579</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="2">
         <row r="2">
           <cell r="C2" t="str">
-            <v>$191,006.19</v>
+            <v>$114,463.22</v>
           </cell>
         </row>
         <row r="3">
           <cell r="C3" t="str">
-            <v>$174,690.87</v>
+            <v>$113,399.16</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="3"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7060,7 +7122,7 @@
   <dimension ref="A1:N58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" activeCellId="5" sqref="E5 H5 E14 H14 E10 H10"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="38.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7102,13 +7164,13 @@
       </c>
       <c r="E2" s="21">
         <f>F4+F11+F19+F22+F23+F20+F21</f>
-        <v>442032.58061500004</v>
+        <v>442157.90672500001</v>
       </c>
       <c r="F2" s="22"/>
       <c r="G2" s="28"/>
       <c r="H2" s="21">
         <f>I4+I11+I19+I22+I23+I20+I21</f>
-        <v>558189.56490500004</v>
+        <v>563051.23022499995</v>
       </c>
       <c r="I2" s="22"/>
       <c r="J2" s="28"/>
@@ -7121,7 +7183,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>4</v>
@@ -7133,16 +7195,16 @@
         <v>5</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H3" s="23" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J3" s="29" t="s">
         <v>7</v>
@@ -7150,121 +7212,121 @@
       <c r="K3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="56" t="s">
-        <v>193</v>
-      </c>
-      <c r="M3" s="57"/>
+      <c r="L3" s="57" t="s">
+        <v>190</v>
+      </c>
+      <c r="M3" s="58"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="35" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B4" s="42"/>
       <c r="C4" s="43">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="D4" s="18">
         <f>$G$42*C4</f>
-        <v>400088.85820800002</v>
+        <v>502604.56847499998</v>
       </c>
       <c r="E4" s="24">
         <f>$E$2*C4</f>
-        <v>176813.03224600002</v>
+        <v>221078.9533625</v>
       </c>
       <c r="F4" s="18" cm="1">
         <f t="array" ref="F4">SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,GlobalETF!A:A))</f>
-        <v>106175.86602500001</v>
+        <v>140802.4915</v>
       </c>
       <c r="G4" s="30">
         <f>F4/E4</f>
-        <v>0.60049796486311879</v>
+        <v>0.63688781477596457</v>
       </c>
       <c r="H4" s="24">
         <f>$H$2*C4</f>
-        <v>223275.82596200003</v>
+        <v>281525.61511249997</v>
       </c>
       <c r="I4" s="18" cm="1">
         <f t="array" ref="I4">SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,GlobalETF!A:A))</f>
-        <v>200856.37007500001</v>
+        <v>244693.04499999998</v>
       </c>
       <c r="J4" s="30">
         <f>I4/H4</f>
-        <v>0.89958852110207554</v>
+        <v>0.86916796150935893</v>
       </c>
       <c r="K4" s="38">
         <f t="shared" ref="K4:K23" si="0">F4+I4</f>
-        <v>307032.23610000004</v>
+        <v>385495.53649999999</v>
       </c>
       <c r="L4" s="52" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="M4" s="49">
         <f t="shared" ref="M4:M21" si="1">K4/$G$42</f>
-        <v>0.30696404541251054</v>
+        <v>0.38349784371207413</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
-        <v>121</v>
+        <v>207</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="44">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D5" s="19">
         <f>$D$4*C5</f>
-        <v>40008.885820800002</v>
+        <v>25130.228423749999</v>
       </c>
       <c r="E5" s="25">
         <f>$E$4*C5</f>
-        <v>17681.303224600004</v>
+        <v>11053.947668125002</v>
       </c>
       <c r="F5" s="19">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"82846")</f>
-        <v>9169.4423999999999</v>
+        <v>13657.116</v>
       </c>
       <c r="G5" s="31">
         <f>F5/E5</f>
-        <v>0.51859539331029347</v>
+        <v>1.2354967121276914</v>
       </c>
       <c r="H5" s="25">
         <f>$H$4*C5</f>
-        <v>22327.582596200005</v>
+        <v>14076.280755624999</v>
       </c>
       <c r="I5" s="19">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"82846")</f>
-        <v>9169.4423999999999</v>
+        <v>9104.7440000000006</v>
       </c>
       <c r="J5" s="31">
         <f>I5/H5</f>
-        <v>0.41067779552456224</v>
+        <v>0.64681460664683521</v>
       </c>
       <c r="K5" s="39">
         <f t="shared" ref="K5:K7" si="2">F5+I5</f>
-        <v>18338.8848</v>
+        <v>22761.86</v>
       </c>
       <c r="L5" s="53"/>
       <c r="M5" s="50"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B6" s="42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="44">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D6" s="19">
         <f t="shared" ref="D6:D10" si="3">$D$4*C6</f>
-        <v>60013.328731200003</v>
+        <v>50260.456847499998</v>
       </c>
       <c r="E6" s="25">
         <f t="shared" ref="E6:E10" si="4">$E$4*C6</f>
-        <v>26521.9548369</v>
+        <v>22107.895336250003</v>
       </c>
       <c r="F6" s="19">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"DHL")</f>
@@ -7276,814 +7338,784 @@
       </c>
       <c r="H6" s="25">
         <f t="shared" ref="H6:H10" si="6">$H$4*C6</f>
-        <v>33491.373894300006</v>
+        <v>28152.561511249998</v>
       </c>
       <c r="I6" s="19">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"DHL")</f>
-        <v>57975.091999999997</v>
+        <v>58846.094999999987</v>
       </c>
       <c r="J6" s="31">
         <f t="shared" ref="J6:J7" si="7">I6/H6</f>
-        <v>1.7310454979533385</v>
+        <v>2.0902572214071746</v>
       </c>
       <c r="K6" s="39">
         <f t="shared" si="2"/>
-        <v>57975.091999999997</v>
+        <v>58846.094999999987</v>
       </c>
       <c r="L6" s="53"/>
       <c r="M6" s="50"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B7" s="42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="44">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D7" s="19">
         <f t="shared" si="3"/>
-        <v>60013.328731200003</v>
+        <v>50260.456847499998</v>
       </c>
       <c r="E7" s="25">
         <f t="shared" si="4"/>
-        <v>26521.9548369</v>
+        <v>22107.895336250003</v>
       </c>
       <c r="F7" s="19">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"ES3")</f>
-        <v>19585.661499999998</v>
+        <v>31638.751199999999</v>
       </c>
       <c r="G7" s="31">
         <f t="shared" si="5"/>
-        <v>0.7384697553571905</v>
+        <v>1.431106431380756</v>
       </c>
       <c r="H7" s="25">
         <f t="shared" si="6"/>
-        <v>33491.373894300006</v>
+        <v>28152.561511249998</v>
       </c>
       <c r="I7" s="19">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"ES3")</f>
-        <v>39171.322999999997</v>
+        <v>39548.438999999998</v>
       </c>
       <c r="J7" s="31">
         <f t="shared" si="7"/>
-        <v>1.1695943893978824</v>
+        <v>1.4047900751125653</v>
       </c>
       <c r="K7" s="39">
         <f t="shared" si="2"/>
-        <v>58756.984499999991</v>
+        <v>71187.190199999997</v>
       </c>
       <c r="L7" s="53"/>
       <c r="M7" s="50"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B8" s="42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="44">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="D8" s="19">
         <f t="shared" si="3"/>
-        <v>80017.771641600004</v>
+        <v>150781.37054249999</v>
       </c>
       <c r="E8" s="25">
         <f t="shared" si="4"/>
-        <v>35362.606449200008</v>
+        <v>66323.686008749995</v>
       </c>
       <c r="F8" s="19">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"VWRA")</f>
-        <v>34984</v>
+        <v>35320</v>
       </c>
       <c r="G8" s="31">
         <f>F8/E8</f>
-        <v>0.98929359322696153</v>
+        <v>0.53253976257200597</v>
       </c>
       <c r="H8" s="25">
         <f t="shared" si="6"/>
-        <v>44655.165192400011</v>
+        <v>84457.684533749984</v>
       </c>
       <c r="I8" s="19">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"VWRA")</f>
-        <v>52476</v>
+        <v>52980</v>
       </c>
       <c r="J8" s="31">
         <f>I8/H8</f>
-        <v>1.1751384139752559</v>
+        <v>0.62729638270900923</v>
       </c>
       <c r="K8" s="39">
         <f>F8+I8</f>
-        <v>87460</v>
+        <v>88300</v>
       </c>
       <c r="L8" s="53"/>
       <c r="M8" s="50"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B9" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C9" s="44">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="D9" s="19">
         <f t="shared" ref="D9" si="8">$D$4*C9</f>
-        <v>80017.771641600004</v>
+        <v>150781.37054249999</v>
       </c>
       <c r="E9" s="25">
         <f t="shared" ref="E9" si="9">$E$4*C9</f>
-        <v>35362.606449200008</v>
+        <v>66323.686008749995</v>
       </c>
       <c r="F9" s="19">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"WORLD")</f>
-        <v>29799.770325000001</v>
+        <v>34494.157499999987</v>
       </c>
       <c r="G9" s="31">
         <f>F9/E9</f>
-        <v>0.84269156935048684</v>
+        <v>0.52008806469907631</v>
       </c>
       <c r="H9" s="25">
         <f t="shared" ref="H9" si="10">$H$4*C9</f>
-        <v>44655.165192400011</v>
+        <v>84457.684533749984</v>
       </c>
       <c r="I9" s="19">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"WORLD")</f>
-        <v>25215.190275000001</v>
+        <v>41392.988999999987</v>
       </c>
       <c r="J9" s="31">
         <f>I9/H9</f>
-        <v>0.56466458395929175</v>
+        <v>0.49010328933963387</v>
       </c>
       <c r="K9" s="39">
         <f>F9+I9</f>
-        <v>55014.960600000006</v>
+        <v>75887.146499999973</v>
       </c>
       <c r="L9" s="53"/>
       <c r="M9" s="50"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C10" s="44">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="D10" s="19">
         <f t="shared" si="3"/>
-        <v>80017.771641600004</v>
+        <v>75390.685271249997</v>
       </c>
       <c r="E10" s="25">
         <f t="shared" si="4"/>
-        <v>35362.606449200008</v>
+        <v>33161.843004374998</v>
       </c>
       <c r="F10" s="19">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"XMME")</f>
-        <v>12636.9918</v>
+        <v>25692.466799999998</v>
       </c>
       <c r="G10" s="31">
         <f>F10/E10</f>
-        <v>0.35735464856510546</v>
+        <v>0.77475991900119745</v>
       </c>
       <c r="H10" s="25">
         <f t="shared" si="6"/>
-        <v>44655.165192400011</v>
+        <v>42228.842266874992</v>
       </c>
       <c r="I10" s="19">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"XMME")</f>
-        <v>16849.322400000001</v>
+        <v>42820.777999999998</v>
       </c>
       <c r="J10" s="31">
         <f>I10/H10</f>
-        <v>0.37732079430013249</v>
+        <v>1.0140173327363353</v>
       </c>
       <c r="K10" s="39">
         <f>F10+I10</f>
-        <v>29486.314200000001</v>
+        <v>68513.2448</v>
       </c>
       <c r="L10" s="53"/>
       <c r="M10" s="50"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="35" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B11" s="42"/>
       <c r="C11" s="43">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D11" s="18">
         <f>$G$42*C11</f>
-        <v>250055.53638000001</v>
+        <v>201041.82738999999</v>
       </c>
       <c r="E11" s="24">
         <f>$E$2*C11</f>
-        <v>110508.14515375001</v>
+        <v>88431.581345000013</v>
       </c>
       <c r="F11" s="18" cm="1">
         <f t="array" ref="F11">SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,GrowthEngine!A:A))</f>
-        <v>101792.28994999999</v>
+        <v>102563.05220000001</v>
       </c>
       <c r="G11" s="30">
         <f>F11/E11</f>
-        <v>0.9211292960204549</v>
+        <v>1.1598011778152941</v>
       </c>
       <c r="H11" s="24">
         <f>$H$2*C11</f>
-        <v>139547.39122625001</v>
+        <v>112610.24604499999</v>
       </c>
       <c r="I11" s="18" cm="1">
         <f t="array" ref="I11">SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,GrowthEngine!A:A))</f>
-        <v>108859.28994999999</v>
+        <v>109718.05220000001</v>
       </c>
       <c r="J11" s="30">
         <f>I11/H11</f>
-        <v>0.7800883197701991</v>
+        <v>0.9743167789204169</v>
       </c>
       <c r="K11" s="38">
         <f>F11+I11</f>
-        <v>210651.57989999998</v>
+        <v>212281.10440000001</v>
       </c>
       <c r="L11" s="52" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M11" s="50">
         <f t="shared" si="1"/>
-        <v>0.21060479498830281</v>
+        <v>0.21118103347538422</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B12" s="42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="44">
         <v>0.25</v>
       </c>
       <c r="D12" s="19">
-        <f t="shared" ref="D12:D18" si="11">$D$11*C12</f>
-        <v>62513.884095000001</v>
+        <f t="shared" ref="D12:D17" si="11">$D$11*C12</f>
+        <v>50260.456847499998</v>
       </c>
       <c r="E12" s="25">
-        <f t="shared" ref="E12:E18" si="12">$E$11*C12</f>
-        <v>27627.036288437503</v>
+        <f t="shared" ref="E12:E15" si="12">$E$11*C12</f>
+        <v>22107.895336250003</v>
       </c>
       <c r="F12" s="19">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"CSNDX")</f>
-        <v>21201</v>
+        <v>21465</v>
       </c>
       <c r="G12" s="31">
         <f>F12/E12</f>
-        <v>0.76740044710742517</v>
+        <v>0.9709201022317191</v>
       </c>
       <c r="H12" s="25">
-        <f t="shared" ref="H12:H18" si="13">$H$11*C12</f>
-        <v>34886.847806562502</v>
+        <f t="shared" ref="H12:H15" si="13">$H$11*C12</f>
+        <v>28152.561511249998</v>
       </c>
       <c r="I12" s="19">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"CSNDX")</f>
-        <v>28268</v>
+        <v>28620</v>
       </c>
       <c r="J12" s="31">
         <f>I12/H12</f>
-        <v>0.81027670246213979</v>
+        <v>1.0166037640505008</v>
       </c>
       <c r="K12" s="39">
         <f t="shared" si="0"/>
-        <v>49469</v>
+        <v>50085</v>
       </c>
       <c r="L12" s="53"/>
       <c r="M12" s="50"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B13" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C13" s="44">
         <v>0.25</v>
       </c>
       <c r="D13" s="19">
         <f t="shared" si="11"/>
-        <v>62513.884095000001</v>
+        <v>50260.456847499998</v>
       </c>
       <c r="E13" s="25">
         <f t="shared" si="12"/>
-        <v>27627.036288437503</v>
+        <v>22107.895336250003</v>
       </c>
       <c r="F13" s="19">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"EQCH")</f>
-        <v>25592.961749999999</v>
+        <v>25722.762999999999</v>
       </c>
       <c r="G13" s="31">
-        <f t="shared" ref="G13:G18" si="14">F13/E13</f>
-        <v>0.92637376962186835</v>
+        <f t="shared" ref="G13:G15" si="14">F13/E13</f>
+        <v>1.1635102577052077</v>
       </c>
       <c r="H13" s="25">
         <f t="shared" si="13"/>
-        <v>34886.847806562502</v>
+        <v>28152.561511249998</v>
       </c>
       <c r="I13" s="19">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"EQCH")</f>
-        <v>25592.961749999999</v>
+        <v>25722.762999999999</v>
       </c>
       <c r="J13" s="31">
-        <f t="shared" ref="J13:J18" si="15">I13/H13</f>
-        <v>0.73359914578426755</v>
+        <f t="shared" ref="J13:J15" si="15">I13/H13</f>
+        <v>0.91369174310198975</v>
       </c>
       <c r="K13" s="39">
         <f t="shared" si="0"/>
-        <v>51185.923499999997</v>
+        <v>51445.525999999998</v>
       </c>
       <c r="L13" s="53"/>
       <c r="M13" s="50"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B14" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C14" s="44">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="D14" s="19">
         <f t="shared" si="11"/>
-        <v>50011.107276000002</v>
+        <v>36187.528930199995</v>
       </c>
       <c r="E14" s="25">
         <f t="shared" ref="E14" si="16">$E$11*C14</f>
-        <v>22101.629030750002</v>
+        <v>15917.684642100001</v>
       </c>
       <c r="F14" s="19">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"CBUK")</f>
-        <v>20836.428199999998</v>
+        <v>20772.2592</v>
       </c>
       <c r="G14" s="31">
         <f t="shared" ref="G14" si="17">F14/E14</f>
-        <v>0.94275531324004536</v>
+        <v>1.304979943192262</v>
       </c>
       <c r="H14" s="25">
         <f t="shared" ref="H14" si="18">$H$11*C14</f>
-        <v>27909.478245250004</v>
+        <v>20269.844288099997</v>
       </c>
       <c r="I14" s="19">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"CBUK")</f>
-        <v>20836.428199999998</v>
+        <v>20772.2592</v>
       </c>
       <c r="J14" s="31">
         <f t="shared" ref="J14" si="19">I14/H14</f>
-        <v>0.74657175662344066</v>
+        <v>1.0247863232079666</v>
       </c>
       <c r="K14" s="39">
         <f t="shared" ref="K14" si="20">F14+I14</f>
-        <v>41672.856399999997</v>
+        <v>41544.518400000001</v>
       </c>
       <c r="L14" s="53"/>
       <c r="M14" s="50"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="36" t="s">
-        <v>120</v>
+      <c r="A15" s="56" t="s">
+        <v>206</v>
       </c>
       <c r="B15" s="42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="44">
-        <v>7.4999999999999997E-2</v>
+        <v>0.12</v>
       </c>
       <c r="D15" s="19">
         <f t="shared" si="11"/>
-        <v>18754.165228499998</v>
+        <v>24125.019286799998</v>
       </c>
       <c r="E15" s="25">
         <f t="shared" si="12"/>
-        <v>8288.1108865312508</v>
+        <v>10611.789761400001</v>
       </c>
       <c r="F15" s="19">
-        <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"HEAL")</f>
-        <v>9047.5</v>
+        <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"2807")</f>
+        <v>0</v>
       </c>
       <c r="G15" s="31">
         <f t="shared" si="14"/>
-        <v>1.0916239084955788</v>
+        <v>0</v>
       </c>
       <c r="H15" s="25">
         <f t="shared" si="13"/>
-        <v>10466.054341968751</v>
+        <v>13513.229525399998</v>
       </c>
       <c r="I15" s="19">
-        <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"HEAL")</f>
-        <v>9047.5</v>
+        <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"2807")</f>
+        <v>0</v>
       </c>
       <c r="J15" s="31">
         <f t="shared" si="15"/>
-        <v>0.86446140105728619</v>
+        <v>0</v>
       </c>
       <c r="K15" s="39">
         <f t="shared" si="0"/>
-        <v>18095</v>
+        <v>0</v>
       </c>
       <c r="L15" s="53"/>
       <c r="M15" s="50"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="44">
-        <v>7.4999999999999997E-2</v>
+        <v>0.1</v>
       </c>
       <c r="D16" s="19">
         <f t="shared" si="11"/>
-        <v>18754.165228499998</v>
+        <v>20104.182739</v>
       </c>
       <c r="E16" s="25">
         <f>$E$11*C16</f>
-        <v>8288.1108865312508</v>
+        <v>8843.1581345000013</v>
       </c>
       <c r="F16" s="19">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"INRA")</f>
-        <v>10470</v>
+        <v>10733.03</v>
       </c>
       <c r="G16" s="31">
         <f>F16/E16</f>
-        <v>1.263255299469324</v>
+        <v>1.213710061129293</v>
       </c>
       <c r="H16" s="25">
         <f>$H$11*C16</f>
-        <v>10466.054341968751</v>
+        <v>11261.0246045</v>
       </c>
       <c r="I16" s="19">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"INRA")</f>
-        <v>10470</v>
+        <v>10733.03</v>
       </c>
       <c r="J16" s="31">
         <f>I16/H16</f>
-        <v>1.0003769957523942</v>
+        <v>0.95311309378642073</v>
       </c>
       <c r="K16" s="39">
         <f>F16+I16</f>
-        <v>20940</v>
+        <v>21466.06</v>
       </c>
       <c r="L16" s="53"/>
       <c r="M16" s="50"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B17" s="42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="44">
-        <v>7.4999999999999997E-2</v>
+        <v>0.1</v>
       </c>
       <c r="D17" s="19">
         <f t="shared" si="11"/>
-        <v>18754.165228499998</v>
+        <v>20104.182739</v>
       </c>
       <c r="E17" s="25">
         <f>$E$11*C17</f>
-        <v>8288.1108865312508</v>
+        <v>8843.1581345000013</v>
       </c>
       <c r="F17" s="19">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"GRDU")</f>
-        <v>4846.3999999999996</v>
+        <v>4860</v>
       </c>
       <c r="G17" s="31">
         <f>F17/E17</f>
-        <v>0.58474121139905744</v>
+        <v>0.54957741635757684</v>
       </c>
       <c r="H17" s="25">
         <f>$H$11*C17</f>
-        <v>10466.054341968751</v>
+        <v>11261.0246045</v>
       </c>
       <c r="I17" s="19">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"GRDU")</f>
-        <v>4846.3999999999996</v>
+        <v>4860</v>
       </c>
       <c r="J17" s="31">
         <f>I17/H17</f>
-        <v>0.46305893717425051</v>
+        <v>0.43157706964408044</v>
       </c>
       <c r="K17" s="39">
         <f>F17+I17</f>
-        <v>9692.7999999999993</v>
+        <v>9720</v>
       </c>
       <c r="L17" s="53"/>
       <c r="M17" s="50"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="44">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="D18" s="19">
-        <f t="shared" si="11"/>
-        <v>18754.165228499998</v>
-      </c>
-      <c r="E18" s="25">
-        <f t="shared" si="12"/>
-        <v>8288.1108865312508</v>
-      </c>
-      <c r="F18" s="19">
-        <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"LOCK")</f>
-        <v>9798</v>
-      </c>
-      <c r="G18" s="31">
-        <f t="shared" si="14"/>
-        <v>1.1821753031710065</v>
-      </c>
-      <c r="H18" s="25">
-        <f t="shared" si="13"/>
-        <v>10466.054341968751</v>
-      </c>
-      <c r="I18" s="19">
-        <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"LOCK")</f>
-        <v>9798</v>
-      </c>
-      <c r="J18" s="31">
-        <f t="shared" si="15"/>
-        <v>0.93616941780152418</v>
-      </c>
-      <c r="K18" s="39">
-        <f t="shared" si="0"/>
-        <v>19596</v>
-      </c>
+      <c r="A18" s="56"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="39"/>
       <c r="L18" s="53"/>
       <c r="M18" s="50"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="35" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="43">
         <v>0.2</v>
       </c>
       <c r="D19" s="18">
         <f>$G$42*C19</f>
-        <v>200044.42910400001</v>
+        <v>201041.82738999999</v>
       </c>
       <c r="E19" s="24">
         <f>$E$2*C19</f>
-        <v>88406.516123000009</v>
+        <v>88431.581345000013</v>
       </c>
       <c r="F19" s="18" cm="1">
         <f t="array" ref="F19">SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,IncomeStrategy!A:A))+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"OPT")-SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"OPT",[1]PositionsHK!F:F,"SPY*")-SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"OPT",[1]PositionsHK!F:F,"QQQ*")+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"FOP")-SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"FOP",[1]PositionsHK!F:F,"SPY*")-SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"FOP",[1]PositionsHK!F:F,"QQQ*")</f>
-        <v>11831.449999999999</v>
+        <v>43690.28</v>
       </c>
       <c r="G19" s="30">
         <f>F19/E19</f>
-        <v>0.13383006727172575</v>
+        <v>0.49405743214689535</v>
       </c>
       <c r="H19" s="24">
         <f>$H$2*C19</f>
-        <v>111637.91298100002</v>
+        <v>112610.24604499999</v>
       </c>
       <c r="I19" s="18" cm="1">
         <f t="array" ref="I19">SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,IncomeStrategy!A:A))+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"OPT")-SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"OPT",[1]PositionsAL!F:F,"SPY*")-SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"OPT",[1]PositionsAL!F:F,"QQQ*")+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"FOP")-SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"FOP",[1]PositionsAL!F:F,"SPY*")-SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"FOP",[1]PositionsAL!F:F,"QQQ*")</f>
-        <v>57618.049999999996</v>
+        <v>61116.939999999995</v>
       </c>
       <c r="J19" s="30">
         <f t="shared" ref="J19:J23" si="21">I19/H19</f>
-        <v>0.51611543481474953</v>
+        <v>0.54272983273277953</v>
       </c>
       <c r="K19" s="38">
         <f t="shared" si="0"/>
-        <v>69449.5</v>
+        <v>104807.22</v>
       </c>
       <c r="L19" s="52" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="M19" s="50">
         <f t="shared" si="1"/>
-        <v>6.9434075531185399E-2</v>
+        <v>0.10426409405509932</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="35" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B20" s="48" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="43">
         <v>0.03</v>
       </c>
       <c r="D20" s="18">
         <f>$G$42*C20</f>
-        <v>30006.664365599998</v>
+        <v>30156.274108499998</v>
       </c>
       <c r="E20" s="24">
         <f>$E$2*C20</f>
-        <v>13260.97741845</v>
+        <v>13264.73720175</v>
       </c>
       <c r="F20" s="18" cm="1">
         <f t="array" ref="F20">SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK")-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,GlobalETF!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,GrowthEngine!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,IncomeStrategy!A:A))-SUMPRODUCT(SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!D:D,"STK",[1]PositionsHK!F:F,Gold!A:A))</f>
-        <v>9994.7999999999738</v>
+        <v>10576.000000000007</v>
       </c>
       <c r="G20" s="30">
         <f t="shared" ref="G20:G21" si="22">F20/E20</f>
-        <v>0.75370009951862271</v>
+        <v>0.79730188688583514</v>
       </c>
       <c r="H20" s="24">
         <f>$H$2*C20</f>
-        <v>16745.686947149999</v>
+        <v>16891.53690675</v>
       </c>
       <c r="I20" s="18" cm="1">
         <f t="array" ref="I20">SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK")-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,GlobalETF!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,GrowthEngine!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,IncomeStrategy!A:A))-SUMPRODUCT(SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!D:D,"STK",[1]PositionsAL!F:F,Gold!A:A))</f>
-        <v>4109.1500000000378</v>
+        <v>4061.1700000000492</v>
       </c>
       <c r="J20" s="30">
         <f>I20/H20</f>
-        <v>0.24538557378796497</v>
+        <v>0.24042631658799335</v>
       </c>
       <c r="K20" s="38">
         <f t="shared" si="0"/>
-        <v>14103.950000000012</v>
+        <v>14637.170000000056</v>
       </c>
       <c r="L20" s="52" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="M20" s="50">
         <f t="shared" si="1"/>
-        <v>1.4100817566549266E-2</v>
+        <v>1.4561318099845448E-2</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="35" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B21" s="48" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" s="43">
         <v>0.02</v>
       </c>
       <c r="D21" s="18">
         <f>$G$42*C21</f>
-        <v>20004.442910400001</v>
+        <v>20104.182739</v>
       </c>
       <c r="E21" s="24">
         <f>$E$2*C21</f>
-        <v>8840.6516123000019</v>
+        <v>8843.1581344999995</v>
       </c>
       <c r="F21" s="18">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"SPY*",[1]PositionsHK!D:D,"OPT")+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"SPY*",[1]PositionsHK!D:D,"FOP")+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"QQQ*",[1]PositionsHK!D:D,"OPT")+SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"QQQ*",[1]PositionsHK!D:D,"FOP")</f>
-        <v>7467.76</v>
+        <v>6896.24</v>
       </c>
       <c r="G21" s="30">
         <f t="shared" si="22"/>
-        <v>0.84470696589944827</v>
+        <v>0.77983904563411044</v>
       </c>
       <c r="H21" s="24">
         <f>H2*C21</f>
-        <v>11163.791298100001</v>
+        <v>11261.024604499999</v>
       </c>
       <c r="I21" s="18">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"SPY*",[1]PositionsAL!D:D,"OPT")+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"SPY*",[1]PositionsAL!D:D,"FOP")+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"QQQ*",[1]PositionsAL!D:D,"OPT")+SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"QQQ*",[1]PositionsAL!D:D,"FOP")</f>
-        <v>7467.76</v>
+        <v>6896.24</v>
       </c>
       <c r="J21" s="30">
         <f>I21/H21</f>
-        <v>0.66892687265400252</v>
+        <v>0.61239898163833206</v>
       </c>
       <c r="K21" s="38">
         <f t="shared" si="0"/>
-        <v>14935.52</v>
+        <v>13792.48</v>
       </c>
       <c r="L21" s="52" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="M21" s="50">
         <f t="shared" si="1"/>
-        <v>1.4932202878026915E-2</v>
+        <v>1.3721005403760124E-2</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="35" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B22" s="42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C22" s="43">
         <v>0.05</v>
       </c>
       <c r="D22" s="18">
         <f>$G$42*C22</f>
-        <v>50011.107276000002</v>
+        <v>50260.456847499998</v>
       </c>
       <c r="E22" s="24">
         <f>$E$2*C22</f>
-        <v>22101.629030750002</v>
+        <v>22107.895336250003</v>
       </c>
       <c r="F22" s="18">
         <f>SUMIFS([1]PositionsHK!V:V,[1]PositionsHK!F:F,"GSD")</f>
-        <v>13764.22464</v>
+        <v>23166.623025000001</v>
       </c>
       <c r="G22" s="30">
         <f t="shared" ref="G22:G23" si="23">F22/H22</f>
-        <v>0.49317384291634236</v>
+        <v>0.82289574310111802</v>
       </c>
       <c r="H22" s="24">
         <f>$H$2*C22</f>
-        <v>27909.478245250004</v>
+        <v>28152.561511249998</v>
       </c>
       <c r="I22" s="18">
         <f>SUMIFS([1]PositionsAL!V:V,[1]PositionsAL!F:F,"GSD")</f>
-        <v>4588.0748800000001</v>
+        <v>23166.623025000001</v>
       </c>
       <c r="J22" s="30">
         <f t="shared" si="21"/>
-        <v>0.16439128097211411</v>
+        <v>0.82289574310111802</v>
       </c>
       <c r="K22" s="38">
         <f t="shared" si="0"/>
-        <v>18352.29952</v>
+        <v>46333.246050000002</v>
       </c>
       <c r="L22" s="52" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="M22" s="50">
         <f>K22/$G$42</f>
-        <v>1.8348223544339667E-2</v>
+        <v>4.6093140568324004E-2</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="34" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B23" s="42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" s="43">
         <v>0.05</v>
       </c>
       <c r="D23" s="18">
         <f>$G$42*C23</f>
-        <v>50011.107276000002</v>
+        <v>50260.456847499998</v>
       </c>
       <c r="E23" s="26">
         <f>$E$2*C23</f>
-        <v>22101.629030750002</v>
+        <v>22107.895336250003</v>
       </c>
       <c r="F23" s="45" t="str">
         <f>[1]Summary!$C$2</f>
-        <v>$191,006.19</v>
+        <v>$114,463.22</v>
       </c>
       <c r="G23" s="32">
         <f t="shared" si="23"/>
-        <v>6.8437750187074133</v>
+        <v>4.0658190180761897</v>
       </c>
       <c r="H23" s="26">
         <f>$H$2*C23</f>
-        <v>27909.478245250004</v>
+        <v>28152.561511249998</v>
       </c>
       <c r="I23" s="45" t="str">
         <f>[1]Summary!$C$3</f>
-        <v>$174,690.87</v>
+        <v>$113,399.16</v>
       </c>
       <c r="J23" s="32">
         <f t="shared" si="21"/>
-        <v>6.2591951187669066</v>
+        <v>4.0280228125843811</v>
       </c>
       <c r="K23" s="40">
         <f t="shared" si="0"/>
-        <v>365697.06</v>
+        <v>227862.38</v>
       </c>
       <c r="L23" s="54" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="M23" s="51">
         <f>K23/$G$42</f>
-        <v>0.36561584007908537</v>
+        <v>0.2266815646855129</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
@@ -8091,7 +8123,7 @@
       <c r="B24" s="5"/>
       <c r="C24" s="6">
         <f>C4+C11+C19+C20+C21+C22+C23</f>
-        <v>1.0000000000000002</v>
+        <v>1.05</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -8112,36 +8144,36 @@
     </row>
     <row r="40" spans="7:14" x14ac:dyDescent="0.2">
       <c r="H40" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="41" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G41" s="12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H41" s="11"/>
       <c r="J41" s="47" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K41" s="47" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L41" s="47"/>
     </row>
     <row r="42" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G42" s="16">
         <f>E2+H2</f>
-        <v>1000222.14552</v>
+        <v>1005209.13695</v>
       </c>
       <c r="H42" s="11"/>
       <c r="J42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K42" s="46">
         <v>365115.64</v>
@@ -8150,14 +8182,14 @@
     </row>
     <row r="43" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G43" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H43" s="17">
         <f>G44/G42</f>
-        <v>0.63438415992091457</v>
+        <v>0.77331843531448707</v>
       </c>
       <c r="J43" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K43" s="46">
         <v>127769.98974999999</v>
@@ -8167,11 +8199,11 @@
     <row r="44" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G44" s="16">
         <f>G42-G46</f>
-        <v>634525.08551999996</v>
+        <v>777346.75694999995</v>
       </c>
       <c r="H44" s="11"/>
       <c r="J44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K44" s="46">
         <v>99402.54</v>
@@ -8180,14 +8212,14 @@
     </row>
     <row r="45" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G45" s="12" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H45" s="17">
         <f>G46/G42</f>
-        <v>0.36561584007908537</v>
+        <v>0.2266815646855129</v>
       </c>
       <c r="J45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K45" s="46">
         <v>70588.302949999998</v>
@@ -8197,11 +8229,11 @@
     <row r="46" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G46" s="16">
         <f>F23+I23</f>
-        <v>365697.06</v>
+        <v>227862.38</v>
       </c>
       <c r="H46" s="11"/>
       <c r="J46" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="K46" s="46">
         <v>18152.184000000001</v>
@@ -8214,7 +8246,7 @@
         <v>5</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E51" s="15"/>
       <c r="F51" s="15"/>
@@ -8226,11 +8258,11 @@
       </c>
       <c r="B52" s="13">
         <f>D4</f>
-        <v>400088.85820800002</v>
+        <v>502604.56847499998</v>
       </c>
       <c r="C52" s="14">
         <f>K4</f>
-        <v>307032.23610000004</v>
+        <v>385495.53649999999</v>
       </c>
       <c r="E52" s="15"/>
       <c r="F52" s="15"/>
@@ -8242,11 +8274,11 @@
       </c>
       <c r="B53" s="13">
         <f>D11</f>
-        <v>250055.53638000001</v>
+        <v>201041.82738999999</v>
       </c>
       <c r="C53" s="14">
         <f>K11</f>
-        <v>210651.57989999998</v>
+        <v>212281.10440000001</v>
       </c>
       <c r="E53" s="15"/>
       <c r="F53" s="15"/>
@@ -8258,11 +8290,11 @@
       </c>
       <c r="B54" s="13">
         <f>D19</f>
-        <v>200044.42910400001</v>
+        <v>201041.82738999999</v>
       </c>
       <c r="C54" s="14">
         <f>K19</f>
-        <v>69449.5</v>
+        <v>104807.22</v>
       </c>
       <c r="E54" s="15"/>
       <c r="F54" s="15"/>
@@ -8274,11 +8306,11 @@
       </c>
       <c r="B55" s="13">
         <f>D20</f>
-        <v>30006.664365599998</v>
+        <v>30156.274108499998</v>
       </c>
       <c r="C55" s="14">
         <f>K20</f>
-        <v>14103.950000000012</v>
+        <v>14637.170000000056</v>
       </c>
       <c r="E55" s="15"/>
       <c r="F55" s="15"/>
@@ -8290,11 +8322,11 @@
       </c>
       <c r="B56" s="13">
         <f>D21</f>
-        <v>20004.442910400001</v>
+        <v>20104.182739</v>
       </c>
       <c r="C56" s="14">
         <f>K21</f>
-        <v>14935.52</v>
+        <v>13792.48</v>
       </c>
       <c r="E56" s="15"/>
       <c r="F56" s="15"/>
@@ -8306,11 +8338,11 @@
       </c>
       <c r="B57" s="13">
         <f>D22</f>
-        <v>50011.107276000002</v>
+        <v>50260.456847499998</v>
       </c>
       <c r="C57" s="14">
         <f>K22</f>
-        <v>18352.29952</v>
+        <v>46333.246050000002</v>
       </c>
       <c r="E57" s="15"/>
       <c r="F57" s="15"/>
@@ -8322,11 +8354,11 @@
       </c>
       <c r="B58" s="13">
         <f>D23</f>
-        <v>50011.107276000002</v>
+        <v>50260.456847499998</v>
       </c>
       <c r="C58" s="14">
         <f>K23</f>
-        <v>365697.06</v>
+        <v>227862.38</v>
       </c>
       <c r="E58" s="15"/>
       <c r="F58" s="15"/>
@@ -8435,25 +8467,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -8461,19 +8493,19 @@
         <v>82846</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D2" s="1">
         <v>3.8E-3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G2" s="1">
         <v>-6.3500000000000001E-2</v>
@@ -8481,117 +8513,117 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>191</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -8622,135 +8654,135 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -8781,408 +8813,408 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="D8" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="55" t="s">
+      <c r="E8" s="55" t="s">
         <v>57</v>
-      </c>
-      <c r="E8" s="55" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="55" t="s">
+      <c r="D9" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="55" t="s">
+      <c r="E9" s="55" t="s">
         <v>61</v>
-      </c>
-      <c r="E9" s="55" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="55" t="s">
+      <c r="E10" s="55" t="s">
         <v>64</v>
-      </c>
-      <c r="E10" s="55" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -9215,36 +9247,36 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>